<commit_message>
Changed all refereces to structured (table) refrences, including column values in VLOOKUPs.
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.talbert\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7950" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3"/>
+    <workbookView xWindow="7950" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="Elaboration">Table6[]</definedName>
     <definedName name="ItemIDs">ItemMap[ItemID]</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -86,9 +86,6 @@
     <t>Output (A)</t>
   </si>
   <si>
-    <t>Output (mAh)</t>
-  </si>
-  <si>
     <t>Battery Pack</t>
   </si>
   <si>
@@ -186,12 +183,15 @@
   </si>
   <si>
     <t>Battery Life (hrs)</t>
+  </si>
+  <si>
+    <t>Battery (mAh)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -236,12 +236,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -257,6 +254,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -314,17 +317,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:I6" totalsRowShown="0">
   <autoFilter ref="A1:I6"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID" dataDxfId="19">
+    <tableColumn id="1" name="ID" dataDxfId="20">
       <calculatedColumnFormula>ComponentData[[#This Row],[Manufacturer]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Name" dataDxfId="16"/>
+    <tableColumn id="6" name="Name" dataDxfId="19"/>
     <tableColumn id="2" name="Manufacturer" dataDxfId="18"/>
     <tableColumn id="3" name="Source" dataDxfId="17"/>
-    <tableColumn id="4" name="Price" dataDxfId="15"/>
-    <tableColumn id="5" name="Consumption (W)" dataDxfId="14"/>
-    <tableColumn id="7" name="Output (V)" dataDxfId="13"/>
+    <tableColumn id="4" name="Price" dataDxfId="16"/>
+    <tableColumn id="5" name="Consumption (W)" dataDxfId="15"/>
+    <tableColumn id="7" name="Output (V)" dataDxfId="14"/>
     <tableColumn id="8" name="Output (A)"/>
-    <tableColumn id="9" name="Output (mAh)"/>
+    <tableColumn id="9" name="Battery (mAh)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -345,32 +348,32 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:K16" totalsRowShown="0">
   <autoFilter ref="A1:K16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ItemID" dataDxfId="12">
+    <tableColumn id="1" name="ItemID" dataDxfId="13">
       <calculatedColumnFormula>ItemMap[[#This Row],[ItemID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</calculatedColumnFormula>
+    <tableColumn id="2" name="Component" dataDxfId="5">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Supply ID" dataDxfId="9"/>
-    <tableColumn id="13" name="Supply Component" dataDxfId="2">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</calculatedColumnFormula>
+    <tableColumn id="5" name="Supply ID" dataDxfId="12"/>
+    <tableColumn id="13" name="Supply Component" dataDxfId="4">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="3">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</calculatedColumnFormula>
+    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="2">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Input Current (A)" dataDxfId="4">
+    <tableColumn id="9" name="Input Current (A)" dataDxfId="11">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Input Voltage (V)]]&lt;=0, 0, Table6[[#This Row],[Total Consumption (W)]]/Table6[[#This Row],[Input Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="6">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</calculatedColumnFormula>
+    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="1">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Output Current (A)" dataDxfId="5">
+    <tableColumn id="7" name="Output Current (A)" dataDxfId="10">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Table6[[#This Row],[Children Consumption (W)]]/Table6[[#This Row],[Output Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="10">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</calculatedColumnFormula>
+    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="7">
+    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="9">
       <calculatedColumnFormula>SUMIFS(Table6[Total Consumption (W)], Table6[Supply ID], Table6[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Total Consumption (W)" dataDxfId="8">
@@ -388,13 +391,13 @@
     <tableColumn id="1" name="ItemID">
       <calculatedColumnFormula>ItemMap[[#This Row],[ItemID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component">
-      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</calculatedColumnFormula>
+    <tableColumn id="2" name="Component" dataDxfId="3">
+      <calculatedColumnFormula>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="1">
+    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="7">
       <calculatedColumnFormula>IF(VLOOKUP(Table7[[#This Row],[Component]], ComponentData[], 8, FALSE)&gt;0, VLOOKUP(Table7[[#This Row],[ItemID]], Elaboration, 8, FALSE)/VLOOKUP(Table7[[#This Row],[Component]], ComponentData[], 8, FALSE), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="0">
+    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="6">
       <calculatedColumnFormula>IF(VLOOKUP(Table7[[#This Row],[Component]], ComponentData[], 9, FALSE)&gt;0, VLOOKUP(Table7[[#This Row],[Component]], ComponentData[], 9, FALSE)/(VLOOKUP(Table7[[#This Row],[ItemID]], Elaboration, 8, FALSE)-VLOOKUP(Table7[[#This Row],[ItemID]], Elaboration, 6, FALSE)), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -703,7 +706,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -778,16 +781,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="3">
         <v>7.25</v>
@@ -809,7 +812,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4">
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5">
         <v>12</v>
@@ -823,10 +826,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -846,10 +849,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -902,7 +905,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -910,7 +913,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -918,7 +921,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -926,7 +929,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -934,7 +937,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -942,7 +945,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -950,7 +953,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -958,66 +961,66 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1037,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,28 +1070,28 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
         <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1097,18 +1100,18 @@
         <v>FrontRight ESC</v>
       </c>
       <c r="B2" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E2" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F2" s="1">
@@ -1116,7 +1119,7 @@
         <v>85</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H2" s="1">
@@ -1124,7 +1127,7 @@
         <v>85</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J2" s="1">
@@ -1142,18 +1145,18 @@
         <v>MidRight ESC</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E3" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F3" s="1">
@@ -1161,7 +1164,7 @@
         <v>85</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H3" s="1">
@@ -1169,7 +1172,7 @@
         <v>85</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J3" s="1">
@@ -1187,18 +1190,18 @@
         <v>BackRight ESC</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E4" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F4" s="1">
@@ -1206,7 +1209,7 @@
         <v>85</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H4" s="1">
@@ -1214,7 +1217,7 @@
         <v>85</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J4" s="1">
@@ -1232,18 +1235,18 @@
         <v>FrontLeft ESC</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E5" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F5" s="1">
@@ -1251,7 +1254,7 @@
         <v>85</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H5" s="1">
@@ -1259,7 +1262,7 @@
         <v>85</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J5" s="1">
@@ -1277,18 +1280,18 @@
         <v>MidLeft ESC</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E6" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F6" s="1">
@@ -1296,7 +1299,7 @@
         <v>85</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H6" s="1">
@@ -1304,7 +1307,7 @@
         <v>85</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J6" s="1">
@@ -1322,18 +1325,18 @@
         <v>BackLeft ESC</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E7" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F7" s="1">
@@ -1341,7 +1344,7 @@
         <v>85</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H7" s="1">
@@ -1349,7 +1352,7 @@
         <v>85</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J7" s="1">
@@ -1367,15 +1370,15 @@
         <v>Battery Pack</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="D8" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="E8" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
@@ -1383,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H8" s="1">
@@ -1391,8 +1394,8 @@
         <v>510.58333333333331</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
-        <v>-8000</v>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <f>SUMIFS(Table6[Total Consumption (W)], Table6[Supply ID], Table6[[#This Row],[ItemID]])</f>
@@ -1400,7 +1403,7 @@
       </c>
       <c r="K8" s="1">
         <f>Table6[[#This Row],[Self Consumption (W)]]+Table6[[#This Row],[Children Consumption (W)]]</f>
-        <v>-1873</v>
+        <v>6127</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1409,18 +1412,18 @@
         <v>FrontRight Motor</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E9" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F9" s="1">
@@ -1428,7 +1431,7 @@
         <v>85</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H9" s="1">
@@ -1436,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J9" s="1">
@@ -1454,18 +1457,18 @@
         <v>MidRight Motor</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E10" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F10" s="1">
@@ -1473,7 +1476,7 @@
         <v>85</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H10" s="1">
@@ -1481,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J10" s="1">
@@ -1499,18 +1502,18 @@
         <v>BackRight Motor</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E11" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F11" s="1">
@@ -1518,7 +1521,7 @@
         <v>85</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H11" s="1">
@@ -1526,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J11" s="1">
@@ -1544,18 +1547,18 @@
         <v>FrontLeft Motor</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E12" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F12" s="1">
@@ -1563,7 +1566,7 @@
         <v>85</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H12" s="1">
@@ -1571,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J12" s="1">
@@ -1589,18 +1592,18 @@
         <v>MidLeft Motor</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E13" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F13" s="1">
@@ -1608,7 +1611,7 @@
         <v>85</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H13" s="1">
@@ -1616,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J13" s="1">
@@ -1634,18 +1637,18 @@
         <v>BackLeft Motor</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="E14" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F14" s="1">
@@ -1653,7 +1656,7 @@
         <v>85</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H14" s="1">
@@ -1661,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>1020</v>
       </c>
       <c r="J14" s="1">
@@ -1679,18 +1682,18 @@
         <v>Logic Supply</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>5V Regulator</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E15" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="F15" s="1">
@@ -1698,7 +1701,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="G15" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>5</v>
       </c>
       <c r="H15" s="1">
@@ -1706,7 +1709,7 @@
         <v>1.4</v>
       </c>
       <c r="I15" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J15" s="1">
@@ -1724,18 +1727,18 @@
         <v>Master Control</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Raspberry Pi</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), "", VLOOKUP(Table6[[#This Row],[Supply ID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>5V Regulator</v>
       </c>
       <c r="E16" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[Supply ID]]), 0,VLOOKUP(Table6[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>5</v>
       </c>
       <c r="F16" s="1">
@@ -1743,7 +1746,7 @@
         <v>1.4</v>
       </c>
       <c r="G16" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 7, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>3.3</v>
       </c>
       <c r="H16" s="1">
@@ -1751,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], 6, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>7</v>
       </c>
       <c r="J16" s="1">
@@ -1780,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,10 +1803,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +1815,7 @@
         <v>FrontRight ESC</v>
       </c>
       <c r="B2" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C2" s="6">
@@ -1830,7 +1833,7 @@
         <v>MidRight ESC</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C3" s="6">
@@ -1848,7 +1851,7 @@
         <v>BackRight ESC</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C4" s="6">
@@ -1866,7 +1869,7 @@
         <v>FrontLeft ESC</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C5" s="6">
@@ -1884,7 +1887,7 @@
         <v>MidLeft ESC</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C6" s="6">
@@ -1902,7 +1905,7 @@
         <v>BackLeft ESC</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>VEX ESC</v>
       </c>
       <c r="C7" s="6">
@@ -1920,7 +1923,7 @@
         <v>Battery Pack</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="C8" s="6">
@@ -1938,7 +1941,7 @@
         <v>FrontRight Motor</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C9" s="6">
@@ -1956,7 +1959,7 @@
         <v>MidRight Motor</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C10" s="6">
@@ -1974,7 +1977,7 @@
         <v>BackRight Motor</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C11" s="6">
@@ -1992,7 +1995,7 @@
         <v>FrontLeft Motor</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C12" s="6">
@@ -2010,7 +2013,7 @@
         <v>MidLeft Motor</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C13" s="6">
@@ -2028,7 +2031,7 @@
         <v>BackLeft Motor</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Motor</v>
       </c>
       <c r="C14" s="6">
@@ -2046,7 +2049,7 @@
         <v>Logic Supply</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>5V Regulator</v>
       </c>
       <c r="C15" s="6">
@@ -2064,7 +2067,7 @@
         <v>Master Control</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], 2, FALSE))</f>
+        <f>IF(ISBLANK(Table6[[#This Row],[ItemID]]), "", VLOOKUP(Table6[[#This Row],[ItemID]], ItemMap[], COLUMN(ItemMap[ComponentID])-COLUMN(ItemMap[])+1, FALSE))</f>
         <v>Raspberry Pi</v>
       </c>
       <c r="C16" s="6">

</xml_diff>

<commit_message>
Added a sample of using a higher-voltage battery with a regulator
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Status:</t>
+  </si>
+  <si>
+    <t>12V Regulator</t>
+  </si>
+  <si>
+    <t>Dirty Power</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -253,83 +259,55 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -360,18 +338,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:I6" totalsRowShown="0">
-  <autoFilter ref="A1:I6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:I7" totalsRowShown="0">
+  <autoFilter ref="A1:I7"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID" dataDxfId="27">
+    <tableColumn id="1" name="ID" dataDxfId="23">
       <calculatedColumnFormula>ComponentData[[#This Row],[Manufacturer]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Name" dataDxfId="26"/>
-    <tableColumn id="2" name="Manufacturer" dataDxfId="25"/>
-    <tableColumn id="3" name="Source" dataDxfId="24"/>
-    <tableColumn id="4" name="Price" dataDxfId="23"/>
-    <tableColumn id="5" name="Consumption (W)" dataDxfId="2"/>
-    <tableColumn id="7" name="Output (V)" dataDxfId="22"/>
+    <tableColumn id="6" name="Name" dataDxfId="22"/>
+    <tableColumn id="2" name="Manufacturer" dataDxfId="21"/>
+    <tableColumn id="3" name="Source" dataDxfId="20"/>
+    <tableColumn id="4" name="Price" dataDxfId="19"/>
+    <tableColumn id="5" name="Consumption (W)" dataDxfId="18"/>
+    <tableColumn id="7" name="Output (V)" dataDxfId="17"/>
     <tableColumn id="8" name="Output (A)"/>
     <tableColumn id="9" name="Battery (mAh)"/>
   </tableColumns>
@@ -383,31 +361,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Analysis" displayName="Analysis" ref="A1:K19" totalsRowShown="0">
   <autoFilter ref="A1:K19"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ItemID" dataDxfId="21"/>
-    <tableColumn id="2" name="ComponentID" dataDxfId="20"/>
-    <tableColumn id="5" name="Supply Item" dataDxfId="19"/>
+    <tableColumn id="1" name="ItemID" dataDxfId="16"/>
+    <tableColumn id="2" name="ComponentID" dataDxfId="15"/>
+    <tableColumn id="5" name="Supply Item" dataDxfId="14"/>
     <tableColumn id="13" name="Supply Component" dataDxfId="13">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="18">
+    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="12">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Input Current (A)" dataDxfId="17">
+    <tableColumn id="9" name="Input Current (A)" dataDxfId="11">
       <calculatedColumnFormula>IF(Analysis[[#This Row],[Input Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Output Voltage (V)" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Output Current (A)" dataDxfId="16">
+    <tableColumn id="7" name="Output Current (A)" dataDxfId="9">
       <calculatedColumnFormula>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="9">
+    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="15">
+    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="7">
       <calculatedColumnFormula>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="14">
+    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="6">
       <calculatedColumnFormula>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -416,19 +394,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Results" displayName="Results" ref="A1:D16" totalsRowShown="0">
-  <autoFilter ref="A1:D16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Results" displayName="Results" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ItemID" dataDxfId="12">
+    <tableColumn id="1" name="ItemID" dataDxfId="5">
       <calculatedColumnFormula>Analysis[[#This Row],[ItemID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component" dataDxfId="11">
+    <tableColumn id="2" name="Component" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="4">
+    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="3">
       <calculatedColumnFormula>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="3">
+    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="2">
       <calculatedColumnFormula>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -734,13 +712,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +810,12 @@
       <c r="F3" s="4">
         <v>1020</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="I3">
         <v>0</v>
       </c>
@@ -849,10 +832,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H4">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="I4">
         <v>5000</v>
@@ -903,6 +886,29 @@
         <v>0.5</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>550</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
@@ -923,7 +929,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,11 +1003,11 @@
       </c>
       <c r="G2">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>510.58333333333331</v>
+        <v>382.9375</v>
       </c>
       <c r="I2">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1024,11 +1030,11 @@
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E3" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1060,104 +1066,104 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
+      <c r="A4" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>5V Regulator</v>
+        <v>LiPo</v>
       </c>
       <c r="E4" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1">
         <f>IF(Analysis[[#This Row],[Input Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>1.4</v>
+        <v>382.9375</v>
       </c>
       <c r="G4" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>3.3</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>510.58333333333331</v>
       </c>
       <c r="I4" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>6127</v>
       </c>
       <c r="K4" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
-        <v>7</v>
+        <v>6127</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="str">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>5V Regulator</v>
       </c>
       <c r="E5" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
         <f>IF(Analysis[[#This Row],[Input Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
-      </c>
-      <c r="G5">
+        <v>1.4</v>
+      </c>
+      <c r="G5" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>3.3</v>
       </c>
       <c r="H5" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
-      </c>
-      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J5" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
-        <v>1020</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D6" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E6" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1169,19 +1175,19 @@
       </c>
       <c r="G6">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I6">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K6" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1190,17 +1196,17 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>VEX ESC</v>
       </c>
       <c r="E7" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1212,19 +1218,19 @@
       </c>
       <c r="G7">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J7" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1233,17 +1239,17 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E8" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1255,19 +1261,19 @@
       </c>
       <c r="G8">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I8">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K8" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1276,17 +1282,17 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>VEX ESC</v>
       </c>
       <c r="E9" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1298,19 +1304,19 @@
       </c>
       <c r="G9">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J9" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K9" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1319,17 +1325,17 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E10" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1341,19 +1347,19 @@
       </c>
       <c r="G10">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I10">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K10" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1362,17 +1368,17 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>VEX ESC</v>
       </c>
       <c r="E11" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1384,19 +1390,19 @@
       </c>
       <c r="G11">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J11" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1405,17 +1411,17 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E12" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1427,19 +1433,19 @@
       </c>
       <c r="G12">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I12">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K12" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1448,17 +1454,17 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>VEX ESC</v>
       </c>
       <c r="E13" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1470,19 +1476,19 @@
       </c>
       <c r="G13">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J13" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1491,17 +1497,17 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E14" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1513,19 +1519,19 @@
       </c>
       <c r="G14">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I14">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K14" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1534,17 +1540,17 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>LiPo</v>
+        <v>VEX ESC</v>
       </c>
       <c r="E15" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1556,19 +1562,19 @@
       </c>
       <c r="G15">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J15" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="K15" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1577,17 +1583,17 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D16" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>12V Regulator</v>
       </c>
       <c r="E16" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1599,19 +1605,19 @@
       </c>
       <c r="G16">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H16" s="1">
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I16">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="K16" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
@@ -1619,22 +1625,28 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="str">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
+        <v>VEX ESC</v>
       </c>
       <c r="E17" s="1">
         <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1">
         <f>IF(Analysis[[#This Row],[Input Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
+        <v>85</v>
+      </c>
+      <c r="G17">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
@@ -1642,9 +1654,9 @@
         <f>IF(Analysis[[#This Row],[Output Voltage (V)]]&lt;=0, 0, Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), 0, VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J17" s="1">
         <f>SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]])</f>
@@ -1652,7 +1664,7 @@
       </c>
       <c r="K17" s="1">
         <f>Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]]</f>
-        <v>0</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1731,10 +1743,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 C5:C17">
       <formula1>ItemIDs</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17">
       <formula1>ComponentIDs</formula1>
     </dataValidation>
   </dataValidations>
@@ -1750,7 +1762,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,11 +1798,11 @@
       </c>
       <c r="C2" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0.51058333333333328</v>
+        <v>0.95734375000000005</v>
       </c>
       <c r="D2" s="5">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
-        <v>9.7927207442467772</v>
+        <v>13.056960992329035</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1821,15 +1833,15 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>Master Control</v>
+        <v>Dirty Power</v>
       </c>
       <c r="B4" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Raspberry Pi</v>
+        <v>12V Regulator</v>
       </c>
       <c r="C4" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>0.92833333333333334</v>
       </c>
       <c r="D4" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1839,15 +1851,15 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>FrontRight ESC</v>
+        <v>Master Control</v>
       </c>
       <c r="B5" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Raspberry Pi</v>
       </c>
       <c r="C5" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1857,15 +1869,15 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>FrontRight Motor</v>
+        <v>FrontRight ESC</v>
       </c>
       <c r="B6" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C6" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D6" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1875,15 +1887,15 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>MidRight ESC</v>
+        <v>FrontRight Motor</v>
       </c>
       <c r="B7" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Motor</v>
       </c>
       <c r="C7" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1893,15 +1905,15 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>MidRight Motor</v>
+        <v>MidRight ESC</v>
       </c>
       <c r="B8" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C8" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D8" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1911,15 +1923,15 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>BackRight ESC</v>
+        <v>MidRight Motor</v>
       </c>
       <c r="B9" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Motor</v>
       </c>
       <c r="C9" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1929,15 +1941,15 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>BackRight Motor</v>
+        <v>BackRight ESC</v>
       </c>
       <c r="B10" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C10" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D10" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1947,15 +1959,15 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>FrontLeft ESC</v>
+        <v>BackRight Motor</v>
       </c>
       <c r="B11" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Motor</v>
       </c>
       <c r="C11" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1965,15 +1977,15 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>FrontLeft Motor</v>
+        <v>FrontLeft ESC</v>
       </c>
       <c r="B12" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C12" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D12" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -1983,15 +1995,15 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>MidLeft ESC</v>
+        <v>FrontLeft Motor</v>
       </c>
       <c r="B13" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Motor</v>
       </c>
       <c r="C13" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -2001,15 +2013,15 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>MidLeft Motor</v>
+        <v>MidLeft ESC</v>
       </c>
       <c r="B14" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C14" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D14" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -2019,15 +2031,15 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>BackLeft ESC</v>
+        <v>MidLeft Motor</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>VEX ESC</v>
+        <v>Motor</v>
       </c>
       <c r="C15" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>1.4166666666666667</v>
+        <v>0</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
@@ -2037,51 +2049,65 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Analysis[[#This Row],[ItemID]]</f>
-        <v>BackLeft Motor</v>
+        <v>BackLeft ESC</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>Motor</v>
+        <v>VEX ESC</v>
       </c>
       <c r="C16" s="6">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="D16" s="5" t="str">
         <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>Analysis[[#This Row],[ItemID]]</f>
+        <v>BackLeft Motor</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>IF(ISBLANK(Analysis[[#This Row],[ItemID]]), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>Motor</v>
+      </c>
+      <c r="C17" s="6">
+        <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f>IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" s="6"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C16">
+  <conditionalFormatting sqref="C2:C17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percent" val="75"/>
@@ -2100,7 +2126,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17">
       <formula1>ItemIDs</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adjusted motor currents to something closer to reality (not always at stall) and changed results color coding
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -288,40 +288,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -335,6 +302,81 @@
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -393,50 +435,50 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:I10" totalsRowShown="0">
   <autoFilter ref="A1:I10"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID" dataDxfId="20"/>
-    <tableColumn id="6" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Manufacturer" dataDxfId="19"/>
-    <tableColumn id="3" name="Source" dataDxfId="17"/>
-    <tableColumn id="4" name="Price" dataDxfId="18"/>
-    <tableColumn id="5" name="Consumption (W)" dataDxfId="24"/>
-    <tableColumn id="7" name="Output (V)" dataDxfId="23"/>
-    <tableColumn id="8" name="Output (A)" dataDxfId="22"/>
-    <tableColumn id="9" name="Battery (mAh)" dataDxfId="21"/>
+    <tableColumn id="1" name="ID" dataDxfId="26"/>
+    <tableColumn id="6" name="Name" dataDxfId="31"/>
+    <tableColumn id="2" name="Manufacturer" dataDxfId="25"/>
+    <tableColumn id="3" name="Source" dataDxfId="23"/>
+    <tableColumn id="4" name="Price" dataDxfId="24"/>
+    <tableColumn id="5" name="Consumption (W)" dataDxfId="30"/>
+    <tableColumn id="7" name="Output (V)" dataDxfId="29"/>
+    <tableColumn id="8" name="Output (A)" dataDxfId="28"/>
+    <tableColumn id="9" name="Battery (mAh)" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Analysis" displayName="Analysis" ref="A1:K36" totalsRowShown="0">
-  <autoFilter ref="A1:K36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Analysis" displayName="Analysis" ref="A1:K30" totalsRowShown="0">
+  <autoFilter ref="A1:K30"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ItemID" dataDxfId="16"/>
-    <tableColumn id="2" name="ComponentID" dataDxfId="15"/>
-    <tableColumn id="5" name="Supply Item" dataDxfId="14"/>
-    <tableColumn id="13" name="Supply Component" dataDxfId="13">
+    <tableColumn id="1" name="ItemID" dataDxfId="22"/>
+    <tableColumn id="2" name="ComponentID" dataDxfId="21"/>
+    <tableColumn id="5" name="Supply Item" dataDxfId="20"/>
+    <tableColumn id="13" name="Supply Component" dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="6">
+    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Input Current (A)" dataDxfId="5">
+    <tableColumn id="9" name="Input Current (A)" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="3">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
+    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="10">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Output Current (A)" dataDxfId="4">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</calculatedColumnFormula>
+    <tableColumn id="7" name="Output Current (A)" dataDxfId="9">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="2">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
+    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="8">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="1">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
+    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="7">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="0">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</calculatedColumnFormula>
+    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="6">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -447,16 +489,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Results" displayName="Results" ref="A1:D30" totalsRowShown="0">
   <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ItemID" dataDxfId="10">
+    <tableColumn id="1" name="ItemID" dataDxfId="18">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component" dataDxfId="9">
+    <tableColumn id="2" name="Component" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="8">
+    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="11">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="7">
+    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -768,7 +810,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,11 +900,9 @@
         <v>7.25</v>
       </c>
       <c r="F3" s="4">
-        <v>1020</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="5">
         <v>0</v>
       </c>
@@ -981,9 +1021,7 @@
       <c r="F8" s="4">
         <v>8</v>
       </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="5">
         <v>0</v>
       </c>
@@ -1039,9 +1077,7 @@
       <c r="F10" s="4">
         <v>0</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5">
         <v>0</v>
       </c>
@@ -1060,13 +1096,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,25 +1175,25 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
         <v/>
       </c>
-      <c r="G2" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
+      <c r="G2">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>24</v>
+      </c>
+      <c r="H2" s="5">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>150.72916666666666</v>
+      </c>
+      <c r="I2" s="5">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>3617.5</v>
+      </c>
+      <c r="K2" s="5">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>3617.5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1183,23 +1219,23 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="G3" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>5</v>
       </c>
       <c r="H3" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v>1.4</v>
       </c>
       <c r="I3" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J3" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>7</v>
       </c>
       <c r="K3" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v>7</v>
       </c>
     </row>
@@ -1226,23 +1262,23 @@
         <v>0.4375</v>
       </c>
       <c r="G4" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>24</v>
       </c>
       <c r="H4" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="I4" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>2.5</v>
       </c>
       <c r="J4" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>8</v>
       </c>
       <c r="K4" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v>10.5</v>
       </c>
     </row>
@@ -1269,23 +1305,23 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G5" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H5" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I5" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>8</v>
       </c>
       <c r="J5" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K5" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v>8</v>
       </c>
     </row>
@@ -1312,23 +1348,23 @@
         <v/>
       </c>
       <c r="G6" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I6" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J6" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K6" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1352,27 +1388,27 @@
       </c>
       <c r="F7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>255.29166666666666</v>
+        <v>150.29166666666666</v>
       </c>
       <c r="G7" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H7" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>510.58333333333331</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>300.58333333333331</v>
       </c>
       <c r="I7" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J7" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>6127</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>3607</v>
       </c>
       <c r="K7" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>6127</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>3607</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1398,23 +1434,23 @@
         <v>1.4</v>
       </c>
       <c r="G8" s="1">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>3.3</v>
       </c>
       <c r="H8" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v>0</v>
       </c>
       <c r="I8" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>7</v>
       </c>
       <c r="J8" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K8" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v>7</v>
       </c>
     </row>
@@ -1438,27 +1474,27 @@
       </c>
       <c r="F9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G9">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H9" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I9" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K9" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1481,27 +1517,27 @@
       </c>
       <c r="F10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G10">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H10" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I10" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J10" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K10" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1524,27 +1560,27 @@
       </c>
       <c r="F11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G11">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H11" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I11" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K11" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1567,27 +1603,27 @@
       </c>
       <c r="F12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H12" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I12" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J12" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K12" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1610,27 +1646,27 @@
       </c>
       <c r="F13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G13">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H13" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I13" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J13" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K13" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1653,27 +1689,27 @@
       </c>
       <c r="F14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G14">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H14" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I14" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J14" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K14" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1696,27 +1732,27 @@
       </c>
       <c r="F15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G15">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H15" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I15" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J15" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K15" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1739,27 +1775,27 @@
       </c>
       <c r="F16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G16">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H16" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I16" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J16" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K16" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,27 +1818,27 @@
       </c>
       <c r="F17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G17">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H17" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I17" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J17" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K17" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1825,27 +1861,27 @@
       </c>
       <c r="F18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G18">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H18" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I18" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J18" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K18" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1868,27 +1904,27 @@
       </c>
       <c r="F19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G19">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="H19" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>85</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <v>50</v>
       </c>
       <c r="I19" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="J19" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <v>600</v>
       </c>
       <c r="K19" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1911,27 +1947,27 @@
       </c>
       <c r="F20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G20">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v>0</v>
       </c>
       <c r="H20" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I20" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <v>600</v>
       </c>
       <c r="J20" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>0</v>
       </c>
       <c r="K20" s="5">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>1020</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1951,23 +1987,23 @@
         <v/>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -1988,23 +2024,23 @@
         <v/>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2025,23 +2061,23 @@
         <v/>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2062,23 +2098,23 @@
         <v/>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2099,23 +2135,23 @@
         <v/>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2136,23 +2172,23 @@
         <v/>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2173,23 +2209,23 @@
         <v/>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2210,23 +2246,23 @@
         <v/>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2247,23 +2283,23 @@
         <v/>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2284,245 +2320,23 @@
         <v/>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="H30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
         <v/>
       </c>
       <c r="I30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
         <v/>
       </c>
       <c r="J30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v/>
       </c>
       <c r="K30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E31" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F31" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G31" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H31" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I31" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J31" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K31" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E32" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F32" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G32" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H32" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I32" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J32" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K32" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E33" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F33" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G33" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H33" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I33" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J33" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K33" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E34" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F34" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G34" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H34" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I34" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J34" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K34" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E35" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F35" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G35" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H35" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I35" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J35" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K35" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="str">
-        <f>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E36" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F36" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="G36" s="1" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H36" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
-      </c>
-      <c r="I36" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J36" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="K36" s="5" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
         <v/>
       </c>
     </row>
@@ -2547,7 +2361,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,13 +2395,13 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
-      <c r="C2" s="6" t="e">
+      <c r="C2" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D2" s="5" t="e">
+        <v>0.37682291666666662</v>
+      </c>
+      <c r="D2" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
-        <v>#VALUE!</v>
+        <v>33.1720801658604</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2612,7 +2426,7 @@
       </c>
       <c r="H3" t="str">
         <f>IF(COUNTIF(Results[Current Output % Capacity], "&gt;1")=0, "GO", "HOLD")</f>
-        <v>HOLD</v>
+        <v>GO</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2680,7 +2494,7 @@
       </c>
       <c r="C7" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.92833333333333334</v>
+        <v>0.54651515151515151</v>
       </c>
       <c r="D7" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2716,7 +2530,7 @@
       </c>
       <c r="C9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2752,7 +2566,7 @@
       </c>
       <c r="C11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D11" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2788,7 +2602,7 @@
       </c>
       <c r="C13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2824,7 +2638,7 @@
       </c>
       <c r="C15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2860,7 +2674,7 @@
       </c>
       <c r="C17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D17" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2896,7 +2710,7 @@
       </c>
       <c r="C19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>1.4166666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D19" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -3105,18 +2919,20 @@
   <conditionalFormatting sqref="C2:C30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="percent" val="75"/>
-        <cfvo type="percent" val="100"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.8"/>
+        <cfvo type="num" val="1"/>
         <color theme="9"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Power Rail Summary
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>http://www.balticnetworks.com/ubiquiti-airmax-omni-3-4-3-7-ghz-12dbi-omni-directional-antenna.html</t>
+  </si>
+  <si>
+    <t>Power Rail</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Current (W)</t>
+  </si>
+  <si>
+    <t>Power (W)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +300,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="40">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -304,6 +319,15 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -332,24 +356,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -364,6 +370,52 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -420,6 +472,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB985"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -435,15 +492,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:I10" totalsRowShown="0">
   <autoFilter ref="A1:I10"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ID" dataDxfId="26"/>
-    <tableColumn id="6" name="Name" dataDxfId="31"/>
-    <tableColumn id="2" name="Manufacturer" dataDxfId="25"/>
-    <tableColumn id="3" name="Source" dataDxfId="23"/>
-    <tableColumn id="4" name="Price" dataDxfId="24"/>
-    <tableColumn id="5" name="Consumption (W)" dataDxfId="30"/>
-    <tableColumn id="7" name="Output (V)" dataDxfId="29"/>
-    <tableColumn id="8" name="Output (A)" dataDxfId="28"/>
-    <tableColumn id="9" name="Battery (mAh)" dataDxfId="27"/>
+    <tableColumn id="1" name="ID" dataDxfId="34"/>
+    <tableColumn id="6" name="Name" dataDxfId="39"/>
+    <tableColumn id="2" name="Manufacturer" dataDxfId="33"/>
+    <tableColumn id="3" name="Source" dataDxfId="31"/>
+    <tableColumn id="4" name="Price" dataDxfId="32"/>
+    <tableColumn id="5" name="Consumption (W)" dataDxfId="38"/>
+    <tableColumn id="7" name="Output (V)" dataDxfId="37"/>
+    <tableColumn id="8" name="Output (A)" dataDxfId="36"/>
+    <tableColumn id="9" name="Battery (mAh)" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -453,31 +510,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Analysis" displayName="Analysis" ref="A1:K30" totalsRowShown="0">
   <autoFilter ref="A1:K30"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ItemID" dataDxfId="22"/>
-    <tableColumn id="2" name="ComponentID" dataDxfId="21"/>
-    <tableColumn id="5" name="Supply Item" dataDxfId="20"/>
-    <tableColumn id="13" name="Supply Component" dataDxfId="19">
+    <tableColumn id="1" name="ItemID" dataDxfId="30"/>
+    <tableColumn id="2" name="ComponentID" dataDxfId="29"/>
+    <tableColumn id="5" name="Supply Item" dataDxfId="28"/>
+    <tableColumn id="13" name="Supply Component" dataDxfId="27">
       <calculatedColumnFormula>IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="15">
+    <tableColumn id="11" name="Input Voltage (V)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Input Current (A)" dataDxfId="14">
+    <tableColumn id="9" name="Input Current (A)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="10">
+    <tableColumn id="8" name="Output Voltage (V)" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Output Current (A)" dataDxfId="9">
+    <tableColumn id="7" name="Output Current (A)" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="8">
+    <tableColumn id="3" name="Self Consumption (W)" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="7">
+    <tableColumn id="4" name="Children Consumption (W)" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="6">
+    <tableColumn id="6" name="Total Consumption (W)" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -489,17 +546,36 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Results" displayName="Results" ref="A1:D30" totalsRowShown="0">
   <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ItemID" dataDxfId="18">
+    <tableColumn id="1" name="ItemID" dataDxfId="26">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component" dataDxfId="17">
+    <tableColumn id="2" name="Component" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[ComponentID])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="11">
+    <tableColumn id="3" name="Current Output % Capacity" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="16">
+    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="RailSummary" displayName="RailSummary" ref="K1:N8" totalsRowShown="0">
+  <autoFilter ref="K1:N8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Power Rail" dataDxfId="5"/>
+    <tableColumn id="2" name="Voltage (V)" dataDxfId="4">
+      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Current (W)" dataDxfId="3">
+      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Power (W)" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -810,7 +886,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +976,7 @@
         <v>7.25</v>
       </c>
       <c r="F3" s="4">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5">
@@ -928,7 +1004,7 @@
         <v>400</v>
       </c>
       <c r="I4" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1019,11 +1095,13 @@
         <v>180</v>
       </c>
       <c r="F8" s="4">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>24</v>
+      </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>
@@ -1075,12 +1153,10 @@
         <v>150</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="5">
         <v>0</v>
       </c>
@@ -1102,7 +1178,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1257,7 @@
       </c>
       <c r="H2" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>150.72916666666666</v>
+        <v>175.72916666666666</v>
       </c>
       <c r="I2" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1189,11 +1265,11 @@
       </c>
       <c r="J2" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>3617.5</v>
+        <v>4217.5</v>
       </c>
       <c r="K2" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>3617.5</v>
+        <v>4217.5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1306,19 +1382,19 @@
       </c>
       <c r="G5" s="1">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="str">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v/>
+        <v>0.3125</v>
       </c>
       <c r="I5" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="K5" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
@@ -1341,11 +1417,11 @@
       </c>
       <c r="E6" s="1">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", IF(ISBLANK(Analysis[[#This Row],[Supply Item]]), 0,VLOOKUP(Analysis[[#This Row],[Supply Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="str">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v/>
+        <v>0.3125</v>
       </c>
       <c r="G6" s="1">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1357,7 +1433,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="J6" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1365,7 +1441,7 @@
       </c>
       <c r="K6" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1388,7 +1464,7 @@
       </c>
       <c r="F7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>150.29166666666666</v>
+        <v>175.29166666666666</v>
       </c>
       <c r="G7" s="1">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1396,7 +1472,7 @@
       </c>
       <c r="H7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>300.58333333333331</v>
+        <v>350.58333333333331</v>
       </c>
       <c r="I7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1404,11 +1480,11 @@
       </c>
       <c r="J7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>3607</v>
+        <v>4207</v>
       </c>
       <c r="K7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>3607</v>
+        <v>4207</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1474,7 +1550,7 @@
       </c>
       <c r="F9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G9">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1482,7 +1558,7 @@
       </c>
       <c r="H9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1490,11 +1566,11 @@
       </c>
       <c r="J9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1517,7 +1593,7 @@
       </c>
       <c r="F10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G10">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1529,7 +1605,7 @@
       </c>
       <c r="I10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1537,7 +1613,7 @@
       </c>
       <c r="K10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1560,7 +1636,7 @@
       </c>
       <c r="F11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G11">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1568,7 +1644,7 @@
       </c>
       <c r="H11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1576,11 +1652,11 @@
       </c>
       <c r="J11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1603,7 +1679,7 @@
       </c>
       <c r="F12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1615,7 +1691,7 @@
       </c>
       <c r="I12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1623,7 +1699,7 @@
       </c>
       <c r="K12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1646,7 +1722,7 @@
       </c>
       <c r="F13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G13">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1654,7 +1730,7 @@
       </c>
       <c r="H13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1662,11 +1738,11 @@
       </c>
       <c r="J13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1689,7 +1765,7 @@
       </c>
       <c r="F14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G14">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1701,7 +1777,7 @@
       </c>
       <c r="I14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1709,7 +1785,7 @@
       </c>
       <c r="K14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1732,7 +1808,7 @@
       </c>
       <c r="F15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G15">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1740,7 +1816,7 @@
       </c>
       <c r="H15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1748,11 +1824,11 @@
       </c>
       <c r="J15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1775,7 +1851,7 @@
       </c>
       <c r="F16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G16">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1787,7 +1863,7 @@
       </c>
       <c r="I16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1795,7 +1871,7 @@
       </c>
       <c r="K16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1818,7 +1894,7 @@
       </c>
       <c r="F17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G17">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1826,7 +1902,7 @@
       </c>
       <c r="H17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1834,11 +1910,11 @@
       </c>
       <c r="J17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1861,7 +1937,7 @@
       </c>
       <c r="F18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G18">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1873,7 +1949,7 @@
       </c>
       <c r="I18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1881,7 +1957,7 @@
       </c>
       <c r="K18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,7 +1980,7 @@
       </c>
       <c r="F19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G19">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1912,7 +1988,7 @@
       </c>
       <c r="H19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", Analysis[[#This Row],[Output Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Children Consumption (W)]]/Analysis[[#This Row],[Output Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1920,11 +1996,11 @@
       </c>
       <c r="J19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="K19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1947,7 +2023,7 @@
       </c>
       <c r="F20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input Voltage (V)]]&lt;=0), "", Analysis[[#This Row],[Total Consumption (W)]]/Analysis[[#This Row],[Input Voltage (V)]])</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="G20">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE))</f>
@@ -1959,7 +2035,7 @@
       </c>
       <c r="I20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", VLOOKUP(Analysis[[#This Row],[ComponentID]], ComponentData[], COLUMN(ComponentData[Consumption (W)])-COLUMN(ComponentData[])+1, FALSE))</f>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="J20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", SUMIFS(Analysis[Total Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -1967,7 +2043,7 @@
       </c>
       <c r="K20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[ComponentID]]), Analysis[[#This Row],[ComponentID]]=""), "", Analysis[[#This Row],[Self Consumption (W)]]+Analysis[[#This Row],[Children Consumption (W)]])</f>
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2358,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,9 +2446,13 @@
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2385,8 +2465,20 @@
       <c r="D1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Battery Pack</v>
@@ -2397,14 +2489,29 @@
       </c>
       <c r="C2" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.37682291666666662</v>
+        <v>0.43932291666666662</v>
       </c>
       <c r="D2" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
-        <v>33.1720801658604</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.6905749851807945</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>24</v>
+      </c>
+      <c r="M2" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>175.72916666666666</v>
+      </c>
+      <c r="N2" s="4">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v>4217.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Logic Supply</v>
@@ -2428,8 +2535,23 @@
         <f>IF(COUNTIF(Results[Current Output % Capacity], "&gt;1")=0, "GO", "HOLD")</f>
         <v>GO</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>24</v>
+      </c>
+      <c r="M3" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N3" s="4">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Comms Power</v>
@@ -2446,8 +2568,23 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>5</v>
+      </c>
+      <c r="M4" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>1.4</v>
+      </c>
+      <c r="N4" s="4">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Transceiver</v>
@@ -2458,14 +2595,29 @@
       </c>
       <c r="C5" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>12</v>
+      </c>
+      <c r="M5" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>350.58333333333331</v>
+      </c>
+      <c r="N5" s="4">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Antenna</v>
@@ -2482,8 +2634,20 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L6" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="M6" s="5" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N6" s="4" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Dirty Power</v>
@@ -2494,14 +2658,26 @@
       </c>
       <c r="C7" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.54651515151515151</v>
+        <v>0.63742424242424234</v>
       </c>
       <c r="D7" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L7" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="M7" s="5" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N7" s="4" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Master Control</v>
@@ -2518,8 +2694,20 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L8" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Voltage (V)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="M8" s="5" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N8" s="4" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight ESC</v>
@@ -2530,14 +2718,14 @@
       </c>
       <c r="C9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight Motor</v>
@@ -2555,7 +2743,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight ESC</v>
@@ -2566,14 +2754,14 @@
       </c>
       <c r="C11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D11" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight Motor</v>
@@ -2591,7 +2779,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight ESC</v>
@@ -2602,14 +2790,14 @@
       </c>
       <c r="C13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight Motor</v>
@@ -2627,7 +2815,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft ESC</v>
@@ -2638,14 +2826,14 @@
       </c>
       <c r="C15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft Motor</v>
@@ -2674,7 +2862,7 @@
       </c>
       <c r="C17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D17" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2710,7 +2898,7 @@
       </c>
       <c r="C19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)/VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE), 0))</f>
-        <v>0.83333333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="D19" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=""), "", IF(VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)&gt;0, VLOOKUP(Results[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)/(VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Output Current (A)])-COLUMN(Analysis[])+1, FALSE)), ""))</f>
@@ -2920,31 +3108,32 @@
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.8"/>
+        <cfvo type="num" val="0.99"/>
         <cfvo type="num" val="1"/>
         <color theme="9"/>
-        <color rgb="FFFFEB84"/>
+        <color rgb="FFFFB985"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 K2:K8">
       <formula1>ItemIDs</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed efficiency to Transmission Loss
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.talbert\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
     <definedName name="ComponentIDs">ComponentData[ID]</definedName>
     <definedName name="ItemIDs">Analysis[ItemID]</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -333,12 +333,15 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Transmission Loss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -459,41 +462,38 @@
       <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -544,10 +544,40 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -572,6 +602,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -627,37 +661,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,7 +950,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="13">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -973,61 +976,61 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ComponentData" displayName="ComponentData" ref="A1:K11" totalsRowShown="0">
   <autoFilter ref="A1:K11"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="60"/>
-    <tableColumn id="6" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" name="Manufacturer" dataDxfId="58"/>
-    <tableColumn id="3" name="Source" dataDxfId="57"/>
-    <tableColumn id="4" name="Price" dataDxfId="56"/>
-    <tableColumn id="5" name="Peak Consumption (W)" dataDxfId="55"/>
-    <tableColumn id="10" name="Constant Consumption (W)" dataDxfId="54"/>
-    <tableColumn id="7" name="Output (V)" dataDxfId="53"/>
-    <tableColumn id="8" name="Output (A)" dataDxfId="52"/>
-    <tableColumn id="9" name="Battery (mAh)" dataDxfId="51"/>
-    <tableColumn id="11" name="Efficiency" dataDxfId="9"/>
+    <tableColumn id="1" name="ID" dataDxfId="12"/>
+    <tableColumn id="6" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Manufacturer" dataDxfId="10"/>
+    <tableColumn id="3" name="Source" dataDxfId="9"/>
+    <tableColumn id="4" name="Price" dataDxfId="8"/>
+    <tableColumn id="5" name="Peak Consumption (W)" dataDxfId="7"/>
+    <tableColumn id="10" name="Constant Consumption (W)" dataDxfId="6"/>
+    <tableColumn id="7" name="Output (V)" dataDxfId="5"/>
+    <tableColumn id="8" name="Output (A)" dataDxfId="4"/>
+    <tableColumn id="9" name="Battery (mAh)" dataDxfId="3"/>
+    <tableColumn id="11" name="Transmission Loss" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Items" displayName="Items" ref="A1:N31" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Items" displayName="Items" ref="A1:N31" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:N31"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="ItemID" dataDxfId="48"/>
-    <tableColumn id="2" name="Component" dataDxfId="47"/>
-    <tableColumn id="3" name="Supply Item" dataDxfId="46"/>
-    <tableColumn id="4" name="Supply Component" dataDxfId="45">
+    <tableColumn id="1" name="ItemID" dataDxfId="58"/>
+    <tableColumn id="2" name="Component" dataDxfId="57"/>
+    <tableColumn id="3" name="Supply Item" dataDxfId="56"/>
+    <tableColumn id="4" name="Supply Component" dataDxfId="55">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Analysis[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="44">
+    <tableColumn id="5" name="Name" dataDxfId="54">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Manufacturer" dataDxfId="43">
+    <tableColumn id="6" name="Manufacturer" dataDxfId="53">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Source" dataDxfId="42">
+    <tableColumn id="7" name="Source" dataDxfId="52">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Price" dataDxfId="41">
+    <tableColumn id="8" name="Price" dataDxfId="51">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Peak Consumption (W)" dataDxfId="40">
+    <tableColumn id="9" name="Peak Consumption (W)" dataDxfId="50">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Constant Consumption (W)" dataDxfId="39">
+    <tableColumn id="10" name="Constant Consumption (W)" dataDxfId="49">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Output (V)" dataDxfId="38">
+    <tableColumn id="11" name="Output (V)" dataDxfId="48">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Output (A)" dataDxfId="37">
+    <tableColumn id="12" name="Output (A)" dataDxfId="47">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Battery (mAh)" dataDxfId="36">
+    <tableColumn id="13" name="Battery (mAh)" dataDxfId="46">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Efficiency" dataDxfId="8">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
+    <tableColumn id="14" name="Efficiency" dataDxfId="45">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1038,47 +1041,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="ItemID" dataDxfId="35">
+    <tableColumn id="1" name="ItemID" dataDxfId="44">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Supply Item" dataDxfId="34"/>
-    <tableColumn id="11" name="Input (V)" dataDxfId="33">
+    <tableColumn id="5" name="Supply Item" dataDxfId="43"/>
+    <tableColumn id="11" name="Input (V)" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Output (V)" dataDxfId="32">
+    <tableColumn id="8" name="Output (V)" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Peak Output (A)" dataDxfId="31">
+    <tableColumn id="7" name="Peak Output (A)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Constant Output (A)" dataDxfId="30">
+    <tableColumn id="17" name="Constant Output (A)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Peak Input (A)" dataDxfId="6">
+    <tableColumn id="9" name="Peak Input (A)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Constant Input (A)" dataDxfId="7">
+    <tableColumn id="16" name="Constant Input (A)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Efficiency" dataDxfId="2">
+    <tableColumn id="2" name="Efficiency" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Self Peak Consumption (W)" dataDxfId="1">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Children Peak Consumption (W)" dataDxfId="29">
+    <tableColumn id="4" name="Children Peak Consumption (W)" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total Peak Consumption (W)" dataDxfId="28">
+    <tableColumn id="6" name="Total Peak Consumption (W)" dataDxfId="34">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" name="Self Constant Consumption (W)" dataDxfId="0">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Children Constant Consumption (W)" dataDxfId="27">
+    <tableColumn id="14" name="Children Constant Consumption (W)" dataDxfId="33">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Total Constant Consumption (W)" dataDxfId="26">
+    <tableColumn id="15" name="Total Constant Consumption (W)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1090,28 +1093,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="ItemID" dataDxfId="25">
+    <tableColumn id="1" name="ItemID" dataDxfId="28">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Current Capacity" dataDxfId="24">
+    <tableColumn id="4" name="Current Capacity" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Peak Current Used" dataDxfId="23">
+    <tableColumn id="5" name="Peak Current Used" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Constant Current Used" dataDxfId="22">
+    <tableColumn id="8" name="Constant Current Used" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Peak % Capacity" dataDxfId="21">
+    <tableColumn id="3" name="Peak % Capacity" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Constant % Capacity" dataDxfId="20">
+    <tableColumn id="7" name="Constant % Capacity" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Battery (mAh)" dataDxfId="19">
+    <tableColumn id="9" name="Battery (mAh)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="18">
+    <tableColumn id="6" name="Battery Life (hrs)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1123,14 +1126,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="RailSummary" displayName="RailSummary" ref="O1:R8" totalsRowShown="0">
   <autoFilter ref="O1:R8"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Power Rail" dataDxfId="17"/>
-    <tableColumn id="2" name="Voltage (V)" dataDxfId="16">
+    <tableColumn id="1" name="Power Rail" dataDxfId="20"/>
+    <tableColumn id="2" name="Voltage (V)" dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current (W)" dataDxfId="15">
+    <tableColumn id="3" name="Current (W)" dataDxfId="18">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Power (W)" dataDxfId="14">
+    <tableColumn id="4" name="Power (W)" dataDxfId="17">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1142,13 +1145,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Item" totalsRowLabel="Total" dataDxfId="12">
+    <tableColumn id="1" name="Item" totalsRowLabel="Total" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Component Name" dataDxfId="11">
+    <tableColumn id="2" name="Component Name" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Cost" totalsRowFunction="count" dataDxfId="10">
+    <tableColumn id="3" name="Cost" totalsRowFunction="count" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1460,7 +1463,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1512,7 @@
         <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,7 +1541,7 @@
         <v>1000</v>
       </c>
       <c r="K2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1569,7 +1572,7 @@
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4">
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1602,7 +1605,7 @@
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1631,7 +1634,7 @@
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1664,7 +1667,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1693,7 +1696,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1726,7 +1729,7 @@
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1755,7 +1758,7 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1782,7 +1785,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1809,7 +1812,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +1943,7 @@
         <v/>
       </c>
       <c r="N2" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -1992,8 +1995,8 @@
         <v>1000</v>
       </c>
       <c r="N3" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2046,8 +2049,8 @@
         <v/>
       </c>
       <c r="N4" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0.95</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2101,8 +2104,8 @@
         <v/>
       </c>
       <c r="N5" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2156,8 +2159,8 @@
         <v/>
       </c>
       <c r="N6" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2211,8 +2214,8 @@
         <v/>
       </c>
       <c r="N7" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2266,8 +2269,8 @@
         <v/>
       </c>
       <c r="N8" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2320,8 +2323,8 @@
         <v/>
       </c>
       <c r="N9" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0.95</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2375,8 +2378,8 @@
         <v/>
       </c>
       <c r="N10" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2430,8 +2433,8 @@
         <v/>
       </c>
       <c r="N11" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2485,8 +2488,8 @@
         <v/>
       </c>
       <c r="N12" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2540,8 +2543,8 @@
         <v/>
       </c>
       <c r="N13" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2595,8 +2598,8 @@
         <v/>
       </c>
       <c r="N14" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2650,8 +2653,8 @@
         <v/>
       </c>
       <c r="N15" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2705,8 +2708,8 @@
         <v/>
       </c>
       <c r="N16" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2760,8 +2763,8 @@
         <v/>
       </c>
       <c r="N17" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2815,8 +2818,8 @@
         <v/>
       </c>
       <c r="N18" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -2870,8 +2873,8 @@
         <v/>
       </c>
       <c r="N19" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2925,8 +2928,8 @@
         <v/>
       </c>
       <c r="N20" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2980,8 +2983,8 @@
         <v/>
       </c>
       <c r="N21" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3035,8 +3038,8 @@
         <v/>
       </c>
       <c r="N22" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3090,8 +3093,8 @@
         <v/>
       </c>
       <c r="N23" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -3145,8 +3148,8 @@
         <v/>
       </c>
       <c r="N24" s="26">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -3191,7 +3194,7 @@
         <v/>
       </c>
       <c r="N25" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3237,7 +3240,7 @@
         <v/>
       </c>
       <c r="N26" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3283,7 +3286,7 @@
         <v/>
       </c>
       <c r="N27" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3329,7 +3332,7 @@
         <v/>
       </c>
       <c r="N28" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3375,7 +3378,7 @@
         <v/>
       </c>
       <c r="N29" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3421,7 +3424,7 @@
         <v/>
       </c>
       <c r="N30" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3467,7 +3470,7 @@
         <v/>
       </c>
       <c r="N31" s="26" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Efficiency])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Transmission Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
     </row>
@@ -3490,10 +3493,10 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3598,7 +3601,7 @@
         <v/>
       </c>
       <c r="J2" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K2" s="12" t="str">
@@ -3610,7 +3613,7 @@
         <v/>
       </c>
       <c r="M2" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N2" s="12" t="str">
@@ -3645,7 +3648,7 @@
       </c>
       <c r="F3" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>36.634062500000006</v>
+        <v>36.634062499999999</v>
       </c>
       <c r="G3" s="12" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -3657,10 +3660,10 @@
       </c>
       <c r="I3" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K3" s="12">
@@ -3672,16 +3675,16 @@
         <v>6819.6975000000011</v>
       </c>
       <c r="M3" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N3" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>879.21750000000009</v>
+        <v>879.21749999999997</v>
       </c>
       <c r="O3" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>879.21750000000009</v>
+        <v>879.21749999999997</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3711,19 +3714,19 @@
       </c>
       <c r="G4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.61250000000000004</v>
+        <v>0.61249999999999993</v>
       </c>
       <c r="H4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.61250000000000004</v>
+        <v>0.61249999999999993</v>
       </c>
       <c r="I4" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="J4" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0.35000000000000031</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
+        <v>0.35000000000000003</v>
       </c>
       <c r="K4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -3731,11 +3734,11 @@
       </c>
       <c r="L4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>7.3500000000000005</v>
+        <v>7.35</v>
       </c>
       <c r="M4" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0.35000000000000031</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
+        <v>0.35000000000000003</v>
       </c>
       <c r="N4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -3743,7 +3746,7 @@
       </c>
       <c r="O4" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>7.3500000000000005</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3781,10 +3784,10 @@
       </c>
       <c r="I5" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>7</v>
       </c>
       <c r="K5" s="12">
@@ -3796,7 +3799,7 @@
         <v>7</v>
       </c>
       <c r="M5" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>7</v>
       </c>
       <c r="N5" s="12">
@@ -3843,10 +3846,10 @@
       </c>
       <c r="I6" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>2.5</v>
       </c>
       <c r="K6" s="12">
@@ -3858,7 +3861,7 @@
         <v>10.5</v>
       </c>
       <c r="M6" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>2.5</v>
       </c>
       <c r="N6" s="12">
@@ -3905,10 +3908,10 @@
       </c>
       <c r="I7" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0.5</v>
       </c>
       <c r="K7" s="12">
@@ -3920,7 +3923,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0.5</v>
       </c>
       <c r="N7" s="12">
@@ -3967,10 +3970,10 @@
       </c>
       <c r="I8" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>7.5</v>
       </c>
       <c r="K8" s="12">
@@ -3982,7 +3985,7 @@
         <v>7.5</v>
       </c>
       <c r="M8" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>7.5</v>
       </c>
       <c r="N8" s="12">
@@ -4025,15 +4028,15 @@
       </c>
       <c r="H9" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>36.196562500000006</v>
+        <v>36.196562499999999</v>
       </c>
       <c r="I9" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="J9" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>324.24750000000034</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
+        <v>324.24750000000006</v>
       </c>
       <c r="K9" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4044,8 +4047,8 @@
         <v>6809.1975000000011</v>
       </c>
       <c r="M9" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>41.367500000000035</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
+        <v>41.367500000000007</v>
       </c>
       <c r="N9" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4053,7 +4056,7 @@
       </c>
       <c r="O9" s="12">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>868.71750000000009</v>
+        <v>868.71749999999997</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4091,10 +4094,10 @@
       </c>
       <c r="I10" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K10" s="12">
@@ -4106,7 +4109,7 @@
         <v>1020</v>
       </c>
       <c r="M10" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N10" s="12">
@@ -4153,10 +4156,10 @@
       </c>
       <c r="I11" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K11" s="12">
@@ -4168,7 +4171,7 @@
         <v>1020</v>
       </c>
       <c r="M11" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N11" s="12">
@@ -4215,10 +4218,10 @@
       </c>
       <c r="I12" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K12" s="12">
@@ -4230,7 +4233,7 @@
         <v>1020</v>
       </c>
       <c r="M12" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N12" s="12">
@@ -4277,10 +4280,10 @@
       </c>
       <c r="I13" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K13" s="12">
@@ -4292,7 +4295,7 @@
         <v>1020</v>
       </c>
       <c r="M13" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N13" s="12">
@@ -4339,10 +4342,10 @@
       </c>
       <c r="I14" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K14" s="12">
@@ -4354,7 +4357,7 @@
         <v>1020</v>
       </c>
       <c r="M14" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N14" s="12">
@@ -4401,10 +4404,10 @@
       </c>
       <c r="I15" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K15" s="12">
@@ -4416,7 +4419,7 @@
         <v>1020</v>
       </c>
       <c r="M15" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N15" s="12">
@@ -4463,10 +4466,10 @@
       </c>
       <c r="I16" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K16" s="12">
@@ -4478,7 +4481,7 @@
         <v>1020</v>
       </c>
       <c r="M16" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N16" s="12">
@@ -4525,10 +4528,10 @@
       </c>
       <c r="I17" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K17" s="12">
@@ -4540,7 +4543,7 @@
         <v>1020</v>
       </c>
       <c r="M17" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N17" s="12">
@@ -4587,10 +4590,10 @@
       </c>
       <c r="I18" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K18" s="12">
@@ -4602,7 +4605,7 @@
         <v>1020</v>
       </c>
       <c r="M18" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N18" s="12">
@@ -4649,10 +4652,10 @@
       </c>
       <c r="I19" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K19" s="12">
@@ -4664,7 +4667,7 @@
         <v>1020</v>
       </c>
       <c r="M19" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N19" s="12">
@@ -4711,10 +4714,10 @@
       </c>
       <c r="I20" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="K20" s="12">
@@ -4726,7 +4729,7 @@
         <v>1020</v>
       </c>
       <c r="M20" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>0</v>
       </c>
       <c r="N20" s="12">
@@ -4773,10 +4776,10 @@
       </c>
       <c r="I21" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>1020</v>
       </c>
       <c r="K21" s="12">
@@ -4788,7 +4791,7 @@
         <v>1020</v>
       </c>
       <c r="M21" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>120</v>
       </c>
       <c r="N21" s="12">
@@ -4835,10 +4838,10 @@
       </c>
       <c r="I22" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>240</v>
       </c>
       <c r="K22" s="12">
@@ -4850,7 +4853,7 @@
         <v>240</v>
       </c>
       <c r="M22" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>60</v>
       </c>
       <c r="N22" s="12">
@@ -4897,10 +4900,10 @@
       </c>
       <c r="I23" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>58.8</v>
       </c>
       <c r="K23" s="12">
@@ -4912,7 +4915,7 @@
         <v>58.8</v>
       </c>
       <c r="M23" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>20</v>
       </c>
       <c r="N23" s="12">
@@ -4959,10 +4962,10 @@
       </c>
       <c r="I24" s="5">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Efficiency])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v>58.8</v>
       </c>
       <c r="K24" s="12">
@@ -4974,7 +4977,7 @@
         <v>58.8</v>
       </c>
       <c r="M24" s="12">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v>20</v>
       </c>
       <c r="N24" s="12">
@@ -5024,7 +5027,7 @@
         <v/>
       </c>
       <c r="J25" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K25" s="12" t="str">
@@ -5036,7 +5039,7 @@
         <v/>
       </c>
       <c r="M25" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N25" s="12" t="str">
@@ -5086,7 +5089,7 @@
         <v/>
       </c>
       <c r="J26" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K26" s="12" t="str">
@@ -5098,7 +5101,7 @@
         <v/>
       </c>
       <c r="M26" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N26" s="12" t="str">
@@ -5148,7 +5151,7 @@
         <v/>
       </c>
       <c r="J27" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K27" s="12" t="str">
@@ -5160,7 +5163,7 @@
         <v/>
       </c>
       <c r="M27" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N27" s="12" t="str">
@@ -5210,7 +5213,7 @@
         <v/>
       </c>
       <c r="J28" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K28" s="12" t="str">
@@ -5222,7 +5225,7 @@
         <v/>
       </c>
       <c r="M28" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N28" s="12" t="str">
@@ -5272,7 +5275,7 @@
         <v/>
       </c>
       <c r="J29" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K29" s="12" t="str">
@@ -5284,7 +5287,7 @@
         <v/>
       </c>
       <c r="M29" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N29" s="12" t="str">
@@ -5334,7 +5337,7 @@
         <v/>
       </c>
       <c r="J30" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Peak Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="K30" s="12" t="str">
@@ -5346,7 +5349,7 @@
         <v/>
       </c>
       <c r="M30" s="12" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(1-Analysis[[#This Row],[Efficiency]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Efficiency]]*Analysis[[#This Row],[Children Constant Consumption (W)]]))</f>
         <v/>
       </c>
       <c r="N30" s="12" t="str">
@@ -5501,7 +5504,7 @@
       </c>
       <c r="D3" s="13">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>36.634062500000006</v>
+        <v>36.634062499999999</v>
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -5509,7 +5512,7 @@
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>9.1585156250000022E-2</v>
+        <v>9.1585156249999994E-2</v>
       </c>
       <c r="G3" s="12">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -5517,7 +5520,7 @@
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
-        <v>27.296999889105933</v>
+        <v>27.29699988910594</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
@@ -6537,13 +6540,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="29" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Corrected battery life units.
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12720" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13650" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -503,32 +503,7 @@
   </cellStyles>
   <dxfs count="61">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -555,9 +530,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -577,6 +549,30 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -646,6 +642,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -997,7 +997,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1046,37 +1046,37 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="47"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="46"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="43">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="42">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="41">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="40">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="39">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="38">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="37">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="36">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="35">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="34">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1088,47 +1088,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="33">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="31">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="29">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="27">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="22">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="20">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="21">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1140,29 +1140,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="15">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="11">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="10">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="14">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="9">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="13">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="0">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1173,14 +1173,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="O1:R8" totalsRowShown="0">
   <autoFilter ref="O1:R8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1192,13 +1192,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="3">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="2">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="1">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1510,7 +1510,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1582,8 @@
         <v>24</v>
       </c>
       <c r="I2" s="11">
-        <v>400</v>
+        <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
+        <v>160</v>
       </c>
       <c r="J2" s="11">
         <v>16000</v>
@@ -2133,7 +2134,7 @@
       </c>
       <c r="L3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="M3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -5746,7 +5747,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5837,7 +5838,7 @@
         <v/>
       </c>
       <c r="H2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="O2" t="s">
@@ -5863,7 +5864,7 @@
       </c>
       <c r="B3">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -5875,26 +5876,26 @@
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.67098437500000008</v>
+        <v>1.6774609375</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.100234375</v>
+        <v>0.25058593750000002</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
         <v>16000</v>
       </c>
       <c r="H3" s="5">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
-        <v>399.06469212782542</v>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
+        <v>0.39906469212782542</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
       </c>
       <c r="L3" s="12" t="str">
         <f>IF(COUNTIF(Results[Constant % Capacity], "&gt;1")=0, IF(COUNTIF(Results[Peak % Capacity], "&gt;1")=0, "GO", "MAYBE"), "HOLD")</f>
-        <v>GO</v>
+        <v>MAYBE</v>
       </c>
       <c r="O3" t="s">
         <v>46</v>
@@ -5942,15 +5943,15 @@
         <v/>
       </c>
       <c r="H4" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="K4" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="13" t="str">
-        <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "0#"))</f>
-        <v>399:04</v>
+        <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00"))</f>
+        <v>0:24</v>
       </c>
       <c r="O4" t="s">
         <v>29</v>
@@ -5998,7 +5999,7 @@
         <v/>
       </c>
       <c r="H5" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="O5" t="s">
@@ -6047,7 +6048,7 @@
         <v/>
       </c>
       <c r="H6" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="O6" t="s">
@@ -6096,7 +6097,7 @@
         <v/>
       </c>
       <c r="H7" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="J7" s="14"/>
@@ -6144,7 +6145,7 @@
         <v/>
       </c>
       <c r="H8" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
       <c r="P8" t="str">
@@ -6190,7 +6191,7 @@
         <v/>
       </c>
       <c r="H9" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6224,7 +6225,7 @@
         <v/>
       </c>
       <c r="H10" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6258,7 +6259,7 @@
         <v/>
       </c>
       <c r="H11" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6292,7 +6293,7 @@
         <v/>
       </c>
       <c r="H12" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6326,7 +6327,7 @@
         <v/>
       </c>
       <c r="H13" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6360,7 +6361,7 @@
         <v/>
       </c>
       <c r="H14" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6394,7 +6395,7 @@
         <v/>
       </c>
       <c r="H15" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6428,7 +6429,7 @@
         <v/>
       </c>
       <c r="H16" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6462,7 +6463,7 @@
         <v/>
       </c>
       <c r="H17" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6496,7 +6497,7 @@
         <v/>
       </c>
       <c r="H18" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6530,7 +6531,7 @@
         <v/>
       </c>
       <c r="H19" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6564,7 +6565,7 @@
         <v/>
       </c>
       <c r="H20" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6598,7 +6599,7 @@
         <v/>
       </c>
       <c r="H21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6632,7 +6633,7 @@
         <v/>
       </c>
       <c r="H22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6666,7 +6667,7 @@
         <v/>
       </c>
       <c r="H23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6700,7 +6701,7 @@
         <v/>
       </c>
       <c r="H24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6734,7 +6735,7 @@
         <v/>
       </c>
       <c r="H25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6768,7 +6769,7 @@
         <v/>
       </c>
       <c r="H26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6802,7 +6803,7 @@
         <v/>
       </c>
       <c r="H27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6836,7 +6837,7 @@
         <v/>
       </c>
       <c r="H28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6870,7 +6871,7 @@
         <v/>
       </c>
       <c r="H29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
@@ -6904,19 +6905,19 @@
         <v/>
       </c>
       <c r="H30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", Results[[#This Row],[Battery (mAh)]]/Results[[#This Row],[Constant Current Used]])</f>
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates to the electrical design documents
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A4557-65E1-49D3-9C5F-7106F8CCDC31}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15510" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -375,6 +376,9 @@
   </si>
   <si>
     <t>LiFePo</t>
+  </si>
+  <si>
+    <t>Battery Life (mins)</t>
   </si>
 </sst>
 </file>
@@ -504,27 +508,9 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="62">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -573,6 +559,27 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -944,7 +951,7 @@
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -1000,7 +1007,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1026,60 +1033,60 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:K15" totalsRowShown="0">
   <autoFilter ref="A1:K15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="44">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="45">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="43">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="42">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="41">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="40">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="39">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="38">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="37">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="36">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="35">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="34">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1091,47 +1098,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="34">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="31">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="30">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="29">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="28">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="27">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="26">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="21">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="20">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="19">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="20">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1140,32 +1147,35 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
-  <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:I30" totalsRowShown="0">
+  <autoFilter ref="A1:I30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="16">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="17">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="16">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="15">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="11">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="10">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="9">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{777FC24A-35A7-482F-9E3B-2D80A6FE3BD6}" name="Battery Life (mins)" dataDxfId="0">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1176,14 +1186,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="O1:R8" totalsRowShown="0">
   <autoFilter ref="O1:R8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1195,13 +1205,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="3">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="2">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="1">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1510,10 +1520,10 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,10 +1594,10 @@
       </c>
       <c r="I2" s="11">
         <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="J2" s="11">
-        <v>16000</v>
+        <v>10000</v>
       </c>
       <c r="K2" s="4"/>
     </row>
@@ -1608,14 +1618,14 @@
         <v>0</v>
       </c>
       <c r="H3" s="11">
-        <v>14.4</v>
+        <v>28.8</v>
       </c>
       <c r="I3" s="11">
         <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="J3" s="11">
-        <v>16000</v>
+        <v>13500</v>
       </c>
       <c r="K3" s="4">
         <v>0</v>
@@ -1861,8 +1871,7 @@
         <v>1224</v>
       </c>
       <c r="G11" s="15">
-        <f>60*14.4</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -2012,7 +2021,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2138,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="D3" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2137,7 +2146,7 @@
       </c>
       <c r="E3" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>24 V Lithuim Ion Battery back</v>
       </c>
       <c r="F3" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2165,15 +2174,15 @@
       </c>
       <c r="L3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="M3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>16000</v>
-      </c>
-      <c r="N3" s="23" t="str">
+        <v>13500</v>
+      </c>
+      <c r="N3" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2188,7 +2197,7 @@
       </c>
       <c r="D4" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E4" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2297,7 +2306,7 @@
       </c>
       <c r="D6" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2462,7 +2471,7 @@
       </c>
       <c r="D9" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2517,7 +2526,7 @@
       </c>
       <c r="D10" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E10" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2572,7 +2581,7 @@
       </c>
       <c r="D11" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2651,7 +2660,7 @@
       </c>
       <c r="J12" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K12" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2682,7 +2691,7 @@
       </c>
       <c r="D13" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E13" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2761,7 +2770,7 @@
       </c>
       <c r="J14" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K14" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2792,7 +2801,7 @@
       </c>
       <c r="D15" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E15" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2871,7 +2880,7 @@
       </c>
       <c r="J16" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K16" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2902,7 +2911,7 @@
       </c>
       <c r="D17" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E17" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2981,7 +2990,7 @@
       </c>
       <c r="J18" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K18" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3012,7 +3021,7 @@
       </c>
       <c r="D19" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E19" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3091,7 +3100,7 @@
       </c>
       <c r="J20" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K20" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3122,7 +3131,7 @@
       </c>
       <c r="D21" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiFePo</v>
+        <v>LiPo</v>
       </c>
       <c r="E21" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3201,7 +3210,7 @@
       </c>
       <c r="J22" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="K22" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4047,7 +4056,7 @@
       </c>
       <c r="F3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>188.41145833333334</v>
+        <v>29.244791666666664</v>
       </c>
       <c r="G3" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4057,33 +4066,33 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
         <v/>
       </c>
-      <c r="I3" s="30" t="str">
+      <c r="I3" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J3" s="29" t="e">
+        <v>0</v>
+      </c>
+      <c r="J3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="K3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
         <v>7665.45</v>
       </c>
-      <c r="L3" s="29" t="e">
+      <c r="L3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M3" s="29" t="e">
+        <v>7665.45</v>
+      </c>
+      <c r="M3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="N3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>5426.25</v>
-      </c>
-      <c r="O3" s="29" t="e">
+        <v>842.25</v>
+      </c>
+      <c r="O3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>#VALUE!</v>
+        <v>842.25</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4543,7 +4552,7 @@
       </c>
       <c r="F11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4551,7 +4560,7 @@
       </c>
       <c r="H11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I11" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4575,11 +4584,11 @@
       </c>
       <c r="N11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4613,7 +4622,7 @@
       </c>
       <c r="H12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I12" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4633,7 +4642,7 @@
       </c>
       <c r="M12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4641,7 +4650,7 @@
       </c>
       <c r="O12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -4667,7 +4676,7 @@
       </c>
       <c r="F13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4675,7 +4684,7 @@
       </c>
       <c r="H13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I13" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4699,11 +4708,11 @@
       </c>
       <c r="N13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4737,7 +4746,7 @@
       </c>
       <c r="H14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I14" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4757,7 +4766,7 @@
       </c>
       <c r="M14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4765,7 +4774,7 @@
       </c>
       <c r="O14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4791,7 +4800,7 @@
       </c>
       <c r="F15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4799,7 +4808,7 @@
       </c>
       <c r="H15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I15" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4823,11 +4832,11 @@
       </c>
       <c r="N15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -4861,7 +4870,7 @@
       </c>
       <c r="H16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I16" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4881,7 +4890,7 @@
       </c>
       <c r="M16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4889,7 +4898,7 @@
       </c>
       <c r="O16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -4915,7 +4924,7 @@
       </c>
       <c r="F17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4923,7 +4932,7 @@
       </c>
       <c r="H17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I17" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4947,11 +4956,11 @@
       </c>
       <c r="N17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -4985,7 +4994,7 @@
       </c>
       <c r="H18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I18" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5005,7 +5014,7 @@
       </c>
       <c r="M18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -5013,7 +5022,7 @@
       </c>
       <c r="O18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -5039,7 +5048,7 @@
       </c>
       <c r="F19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5047,7 +5056,7 @@
       </c>
       <c r="H19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I19" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5071,11 +5080,11 @@
       </c>
       <c r="N19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -5109,7 +5118,7 @@
       </c>
       <c r="H20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I20" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5129,7 +5138,7 @@
       </c>
       <c r="M20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -5137,7 +5146,7 @@
       </c>
       <c r="O20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -5163,7 +5172,7 @@
       </c>
       <c r="F21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="G21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5171,7 +5180,7 @@
       </c>
       <c r="H21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I21" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5195,11 +5204,11 @@
       </c>
       <c r="N21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="O21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -5233,7 +5242,7 @@
       </c>
       <c r="H22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="I22" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5253,7 +5262,7 @@
       </c>
       <c r="M22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
       <c r="N22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -5261,7 +5270,7 @@
       </c>
       <c r="O22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>864</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -5778,7 +5787,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,6 +5800,7 @@
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.140625" customWidth="1"/>
@@ -5826,6 +5836,9 @@
       <c r="H1" t="s">
         <v>33</v>
       </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
       <c r="O1" t="s">
         <v>50</v>
       </c>
@@ -5870,6 +5883,10 @@
       </c>
       <c r="H2" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
+        <v/>
+      </c>
+      <c r="I2" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
         <v/>
       </c>
       <c r="O2" t="s">
@@ -5895,7 +5912,7 @@
       </c>
       <c r="B3">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -5903,30 +5920,34 @@
       </c>
       <c r="D3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>188.41145833333334</v>
+        <v>29.244791666666664</v>
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.6635091145833332</v>
+        <v>1.9715663580246912</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.1775716145833335</v>
+        <v>0.21662808641975306</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>16000</v>
+        <v>13500</v>
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>8.4920525224602625E-2</v>
+        <v>0.46162065894924315</v>
+      </c>
+      <c r="I3" s="5">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v>27.697239536954587</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
       </c>
       <c r="L3" s="12" t="str">
         <f>IF(COUNTIF(Results[Constant % Capacity], "&gt;1")=0, IF(COUNTIF(Results[Peak % Capacity], "&gt;1")=0, "GO", "MAYBE"), "HOLD")</f>
-        <v>HOLD</v>
+        <v>MAYBE</v>
       </c>
       <c r="O3" t="s">
         <v>46</v>
@@ -5977,12 +5998,16 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I4" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
       <c r="K4" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="13" t="str">
         <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00"))</f>
-        <v>0:05</v>
+        <v>0:28</v>
       </c>
       <c r="O4" t="s">
         <v>29</v>
@@ -6033,6 +6058,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I5" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
       <c r="O5" t="s">
         <v>102</v>
       </c>
@@ -6082,6 +6111,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I6" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
       <c r="O6" t="s">
         <v>103</v>
       </c>
@@ -6131,6 +6164,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I7" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="P7" t="str">
@@ -6179,6 +6216,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I8" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
       <c r="P8" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
@@ -6225,6 +6266,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I9" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -6259,6 +6304,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I10" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
@@ -6275,7 +6324,7 @@
       </c>
       <c r="D11" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6283,7 +6332,7 @@
       </c>
       <c r="F11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G11" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6291,6 +6340,10 @@
       </c>
       <c r="H11" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
+        <v/>
+      </c>
+      <c r="I11" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
         <v/>
       </c>
     </row>
@@ -6327,6 +6380,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I12" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
@@ -6343,7 +6400,7 @@
       </c>
       <c r="D13" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6351,7 +6408,7 @@
       </c>
       <c r="F13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G13" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6359,6 +6416,10 @@
       </c>
       <c r="H13" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
+        <v/>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
         <v/>
       </c>
     </row>
@@ -6395,6 +6456,10 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I14" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
@@ -6411,7 +6476,7 @@
       </c>
       <c r="D15" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6419,7 +6484,7 @@
       </c>
       <c r="F15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G15" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6427,6 +6492,10 @@
       </c>
       <c r="H15" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
+        <v/>
+      </c>
+      <c r="I15" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
         <v/>
       </c>
     </row>
@@ -6463,8 +6532,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft ESC</v>
@@ -6479,7 +6552,7 @@
       </c>
       <c r="D17" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6487,7 +6560,7 @@
       </c>
       <c r="F17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G17" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6497,8 +6570,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft Motor</v>
@@ -6531,8 +6608,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft ESC</v>
@@ -6547,7 +6628,7 @@
       </c>
       <c r="D19" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6555,7 +6636,7 @@
       </c>
       <c r="F19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G19" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6565,8 +6646,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft Motor</v>
@@ -6599,8 +6684,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft ESC</v>
@@ -6615,7 +6704,7 @@
       </c>
       <c r="D21" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>30</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="E21" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6623,7 +6712,7 @@
       </c>
       <c r="F21" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.5</v>
+        <v>5.7870370370370371E-2</v>
       </c>
       <c r="G21" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6633,8 +6722,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft Motor</v>
@@ -6667,8 +6760,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Shoulder ESC</v>
@@ -6701,8 +6798,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Shoulder Motor</v>
@@ -6735,8 +6836,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Base ESC</v>
@@ -6769,8 +6874,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Base Motor</v>
@@ -6803,8 +6912,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Elbow ESC</v>
@@ -6837,8 +6950,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Elbow Motor</v>
@@ -6871,8 +6988,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -6905,8 +7026,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -6939,16 +7064,20 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="I30" s="5" t="str">
+        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6964,14 +7093,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 O2:O8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>ItemIDs</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -6984,7 +7113,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7048,7 +7177,7 @@
       </c>
       <c r="B3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>24 V Lithuim Ion Battery back</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>

</xml_diff>

<commit_message>
Added the option to set output voltage equal to input voltage.
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A4557-65E1-49D3-9C5F-7106F8CCDC31}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75AF8C2-AFA4-463C-BDEC-EBC516922DA7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15510" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16440" yWindow="0" windowWidth="18825" windowHeight="4845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Status:</t>
   </si>
   <si>
-    <t>Antenna</t>
-  </si>
-  <si>
     <t>Ubiquity</t>
   </si>
   <si>
@@ -174,21 +171,9 @@
     <t>?</t>
   </si>
   <si>
-    <t>RM3</t>
-  </si>
-  <si>
-    <t>Comms Power</t>
-  </si>
-  <si>
     <t>AMO-3G12 - Ubiquiti Antenna 3.4-3.7 GHz 12dBi Omni-directional</t>
   </si>
   <si>
-    <t>3GHz Antenna</t>
-  </si>
-  <si>
-    <t>http://www.balticnetworks.com/ubiquiti-airmax-omni-3-4-3-7-ghz-12dbi-omni-directional-antenna.html</t>
-  </si>
-  <si>
     <t>Power Rail</t>
   </si>
   <si>
@@ -354,9 +339,6 @@
     <t>12V VEX ESC</t>
   </si>
   <si>
-    <t>24V VEX ESC</t>
-  </si>
-  <si>
     <t>Talon SRX DC Motor  Driver</t>
   </si>
   <si>
@@ -378,7 +360,22 @@
     <t>LiFePo</t>
   </si>
   <si>
-    <t>Battery Life (mins)</t>
+    <t>28V VEX ESC</t>
+  </si>
+  <si>
+    <t>[INPUT]</t>
+  </si>
+  <si>
+    <t>RM5</t>
+  </si>
+  <si>
+    <t>Ubiquity Rocket M5</t>
+  </si>
+  <si>
+    <t>Network Power</t>
+  </si>
+  <si>
+    <t>Network Switch</t>
   </si>
 </sst>
 </file>
@@ -508,9 +505,33 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="61">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -561,27 +582,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -613,12 +613,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1007,7 +1001,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="4">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1033,60 +1027,60 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:K15" totalsRowShown="0">
   <autoFilter ref="A1:K15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="43">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="42">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="41">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="40">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="39">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="38">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="37">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="36">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="35">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="34">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1098,47 +1092,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="33">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="32">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="3">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="31">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="4">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="29">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="27">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="22">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="21">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="20">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1147,35 +1141,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:I30" totalsRowShown="0">
-  <autoFilter ref="A1:I30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
+  <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="20">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="13">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{777FC24A-35A7-482F-9E3B-2D80A6FE3BD6}" name="Battery Life (mins)" dataDxfId="0">
-      <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1183,17 +1174,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="O1:R8" totalsRowShown="0">
-  <autoFilter ref="O1:R8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:P8" totalsRowShown="0">
+  <autoFilter ref="M1:P8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="11">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="9">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1205,13 +1196,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="7">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="5">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1519,11 +1510,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,10 +1548,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -1572,12 +1563,12 @@
         <v>34</v>
       </c>
       <c r="K1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1593,20 +1584,22 @@
         <v>28.8</v>
       </c>
       <c r="I2" s="11">
-        <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
-        <v>100</v>
+        <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*15</f>
+        <v>180</v>
       </c>
       <c r="J2" s="11">
-        <v>10000</v>
-      </c>
-      <c r="K2" s="4"/>
+        <v>12000</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7"/>
@@ -1618,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="11">
-        <v>28.8</v>
+        <v>22.2</v>
       </c>
       <c r="I3" s="11">
         <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
@@ -1633,16 +1626,16 @@
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E4" s="3">
         <v>8.48</v>
@@ -1664,19 +1657,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="F5" s="11">
         <v>2.5</v>
@@ -1726,61 +1719,61 @@
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="E7" s="3">
         <v>180</v>
       </c>
       <c r="F7" s="11">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="G7" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="11">
-        <v>24</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="F8" s="11">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="11">
-        <v>7.5</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>12</v>
+      </c>
+      <c r="I8" s="11">
+        <v>60</v>
+      </c>
       <c r="J8" s="11"/>
       <c r="K8" s="4">
         <v>0</v>
@@ -1788,19 +1781,17 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="3">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -1808,8 +1799,8 @@
       <c r="G9" s="11">
         <v>0</v>
       </c>
-      <c r="H9" s="11">
-        <v>12</v>
+      <c r="H9" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="I9" s="11">
         <v>60</v>
@@ -1821,57 +1812,54 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>15</v>
+      </c>
       <c r="E10" s="3">
-        <v>90</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <v>28.8</v>
-      </c>
-      <c r="I10" s="11">
-        <v>60</v>
-      </c>
+        <v>7.25</v>
+      </c>
+      <c r="F10" s="15">
+        <f>85*14.4</f>
+        <v>1224</v>
+      </c>
+      <c r="G10" s="15">
+        <v>100</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E11" s="3">
-        <v>7.25</v>
-      </c>
-      <c r="F11" s="15">
-        <f>85*14.4</f>
-        <v>1224</v>
-      </c>
-      <c r="G11" s="15">
-        <v>100</v>
+        <v>60</v>
+      </c>
+      <c r="F11" s="11">
+        <v>240</v>
+      </c>
+      <c r="G11" s="11">
+        <f>15*12</f>
+        <v>180</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -1882,7 +1870,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>56</v>
@@ -1892,14 +1880,15 @@
         <v>55</v>
       </c>
       <c r="E12" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F12" s="11">
-        <v>240</v>
+        <f>1.5*12</f>
+        <v>18</v>
       </c>
       <c r="G12" s="11">
-        <f>15*12</f>
-        <v>180</v>
+        <f>1*12</f>
+        <v>12</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -1908,50 +1897,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F13" s="11">
-        <f>1.5*12</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G13" s="11">
-        <f>1*12</f>
-        <v>12</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>22</v>
+      </c>
+      <c r="I13" s="11">
+        <v>40</v>
+      </c>
       <c r="J13" s="11"/>
       <c r="K13" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="E14" s="3">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
@@ -1960,50 +1951,40 @@
         <v>0</v>
       </c>
       <c r="H14" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I14" s="11">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="3">
-        <v>16</v>
-      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="11">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G15" s="11">
-        <v>0</v>
-      </c>
-      <c r="H15" s="11">
-        <v>12</v>
-      </c>
-      <c r="I15" s="11">
-        <v>20</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2018,10 +1999,10 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,10 +2049,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>10</v>
@@ -2083,7 +2064,7 @@
         <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2170,7 +2151,7 @@
       </c>
       <c r="K3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>22.2</v>
       </c>
       <c r="L3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2190,7 +2171,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>12</v>
@@ -2296,10 +2277,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>12</v>
@@ -2310,35 +2291,33 @@
       </c>
       <c r="E6" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Homemade POE injection</v>
+        <v>Adjustable Linear Voltage Regulator</v>
       </c>
       <c r="F6" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Gabe</v>
+        <v>Aihsd</v>
       </c>
       <c r="G6" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Gabe</v>
-      </c>
-      <c r="H6" s="17" t="str">
+        <v>https://www.aliexpress.com/item/DC-Adjustable-Voltage-Regulator-Module-DC-4-5-30V-to-0-8-30V-12A-Buck-Converters/1724570414.html</v>
+      </c>
+      <c r="H6" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>?</v>
+        <v>8.48</v>
       </c>
       <c r="I6" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K6" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L6" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M6" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2346,26 +2325,26 @@
       </c>
       <c r="N6" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>POE Injector</v>
+        <v>Regulator</v>
       </c>
       <c r="E7" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Ubiquity Rocket M3</v>
+        <v>Ubiquity Rocket M5</v>
       </c>
       <c r="F7" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2381,19 +2360,19 @@
       </c>
       <c r="I7" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="J7" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0.5</v>
-      </c>
-      <c r="K7" s="18">
+        <v>6</v>
+      </c>
+      <c r="K7" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>24</v>
-      </c>
-      <c r="L7" s="18">
+        <v/>
+      </c>
+      <c r="L7" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="M7" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2406,41 +2385,41 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="14" t="str">
+        <v>111</v>
+      </c>
+      <c r="D8" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>RM3</v>
+        <v>Regulator</v>
       </c>
       <c r="E8" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>AMO-3G12 - Ubiquiti Antenna 3.4-3.7 GHz 12dBi Omni-directional</v>
+        <v/>
       </c>
       <c r="F8" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Ubiquity</v>
+        <v/>
       </c>
       <c r="G8" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>http://www.balticnetworks.com/ubiquiti-airmax-omni-3-4-3-7-ghz-12dbi-omni-directional-antenna.html</v>
-      </c>
-      <c r="H8" s="17">
+        <v/>
+      </c>
+      <c r="H8" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>150</v>
+        <v/>
       </c>
       <c r="I8" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="J8" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="K8" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2461,10 +2440,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>12</v>
@@ -2516,10 +2495,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>12</v>
@@ -2574,7 +2553,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>12</v>
@@ -2607,9 +2586,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L11" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2629,14 +2608,14 @@
         <v>22</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E12" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2684,7 +2663,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>12</v>
@@ -2717,9 +2696,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L13" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2739,14 +2718,14 @@
         <v>27</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E14" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2794,7 +2773,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>12</v>
@@ -2827,9 +2806,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L15" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2849,14 +2828,14 @@
         <v>23</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E16" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2904,7 +2883,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>12</v>
@@ -2937,9 +2916,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L17" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2959,14 +2938,14 @@
         <v>24</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E18" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3014,7 +2993,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>12</v>
@@ -3047,9 +3026,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L19" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3069,14 +3048,14 @@
         <v>25</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E20" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3124,7 +3103,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>12</v>
@@ -3157,9 +3136,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>28.8</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L21" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3179,14 +3158,14 @@
         <v>26</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E22" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3231,13 +3210,13 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D23" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3245,7 +3224,7 @@
       </c>
       <c r="E23" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="F23" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3253,11 +3232,11 @@
       </c>
       <c r="G23" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.vexrobotics.com/217-9090.html</v>
+        <v/>
       </c>
       <c r="H23" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="I23" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3267,9 +3246,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K23" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12</v>
+        <v>[INPUT]</v>
       </c>
       <c r="L23" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3286,17 +3265,17 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12V VEX ESC</v>
+        <v>28V VEX ESC</v>
       </c>
       <c r="E24" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3341,13 +3320,13 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D25" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3396,13 +3375,13 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D26" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3451,13 +3430,13 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D27" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3506,13 +3485,13 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D28" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3903,7 +3882,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3935,43 +3914,43 @@
         <v>35</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3981,11 +3960,11 @@
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v/>
       </c>
       <c r="D2" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E2" s="29" t="str">
@@ -4043,20 +4022,20 @@
         <v/>
       </c>
       <c r="C3" s="28" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v/>
       </c>
       <c r="D3" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>266.16145833333331</v>
+        <v>346.33108108108109</v>
       </c>
       <c r="F3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>29.244791666666664</v>
+        <v>38.128378378378379</v>
       </c>
       <c r="G3" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4076,11 +4055,11 @@
       </c>
       <c r="K3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>7665.45</v>
+        <v>7688.55</v>
       </c>
       <c r="L3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>7665.45</v>
+        <v>7688.55</v>
       </c>
       <c r="M3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4088,11 +4067,11 @@
       </c>
       <c r="N3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>842.25</v>
+        <v>846.45</v>
       </c>
       <c r="O3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>842.25</v>
+        <v>846.45</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4105,11 +4084,11 @@
         <v>Battery Pack</v>
       </c>
       <c r="C4" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D4" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>5</v>
       </c>
       <c r="E4" s="29">
@@ -4122,11 +4101,11 @@
       </c>
       <c r="G4" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.25520833333333331</v>
+        <v>0.33108108108108109</v>
       </c>
       <c r="H4" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.25520833333333331</v>
+        <v>0.33108108108108109</v>
       </c>
       <c r="I4" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4167,11 +4146,11 @@
         <v>Logic Supply</v>
       </c>
       <c r="C5" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>5</v>
       </c>
       <c r="D5" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>3.3</v>
       </c>
       <c r="E5" s="29">
@@ -4222,63 +4201,63 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Comms Power</v>
+        <v>Network Power</v>
       </c>
       <c r="B6" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
         <v>Battery Pack</v>
       </c>
       <c r="C6" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D6" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>12</v>
       </c>
       <c r="E6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>0.33333333333333331</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="F6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>0.33333333333333331</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.36458333333333331</v>
+        <v>1.5135135135135136</v>
       </c>
       <c r="H6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.36458333333333331</v>
+        <v>0.66216216216216217</v>
       </c>
       <c r="I6" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="K6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>10.5</v>
+        <v>33.6</v>
       </c>
       <c r="M6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>2.5</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="N6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="O6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>10.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -4288,31 +4267,31 @@
       </c>
       <c r="B7" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Comms Power</v>
+        <v>Network Power</v>
       </c>
       <c r="C7" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24</v>
-      </c>
-      <c r="D7" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24</v>
-      </c>
-      <c r="E7" s="29">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>12</v>
+      </c>
+      <c r="D7" s="26" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="E7" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>0.3125</v>
-      </c>
-      <c r="F7" s="29">
+        <v/>
+      </c>
+      <c r="F7" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>0.3125</v>
+        <v/>
       </c>
       <c r="G7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4320,11 +4299,11 @@
       </c>
       <c r="J7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="K7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="L7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -4332,32 +4311,32 @@
       </c>
       <c r="M7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="N7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="O7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Antenna</v>
+        <v>Network Switch</v>
       </c>
       <c r="B8" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Transceiver</v>
+        <v>Network Power</v>
       </c>
       <c r="C8" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>12</v>
       </c>
       <c r="D8" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E8" s="29" t="str">
@@ -4370,11 +4349,11 @@
       </c>
       <c r="G8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.3125</v>
+        <v>2</v>
       </c>
       <c r="H8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.3125</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I8" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4382,7 +4361,7 @@
       </c>
       <c r="J8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="K8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4390,11 +4369,11 @@
       </c>
       <c r="L8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>7.5</v>
+        <v>24</v>
       </c>
       <c r="M8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="N8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4402,7 +4381,7 @@
       </c>
       <c r="O8" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4415,11 +4394,11 @@
         <v>Battery Pack</v>
       </c>
       <c r="C9" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D9" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>12</v>
       </c>
       <c r="E9" s="29">
@@ -4432,11 +4411,11 @@
       </c>
       <c r="G9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>9.1666666666666661</v>
+        <v>11.891891891891893</v>
       </c>
       <c r="H9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>6.875</v>
+        <v>8.9189189189189193</v>
       </c>
       <c r="I9" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4477,11 +4456,11 @@
         <v>Battery Pack</v>
       </c>
       <c r="C10" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D10" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>12</v>
       </c>
       <c r="E10" s="29">
@@ -4494,11 +4473,11 @@
       </c>
       <c r="G10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.375</v>
+        <v>1.783783783783784</v>
       </c>
       <c r="H10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.91666666666666663</v>
+        <v>1.1891891891891893</v>
       </c>
       <c r="I10" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4539,28 +4518,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C11" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D11" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I11" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4601,11 +4580,11 @@
         <v>FrontRight ESC</v>
       </c>
       <c r="C12" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D12" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E12" s="29" t="str">
@@ -4618,11 +4597,11 @@
       </c>
       <c r="G12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I12" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4663,28 +4642,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C13" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D13" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I13" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4725,11 +4704,11 @@
         <v>MidRight ESC</v>
       </c>
       <c r="C14" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D14" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E14" s="29" t="str">
@@ -4742,11 +4721,11 @@
       </c>
       <c r="G14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I14" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4787,28 +4766,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C15" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D15" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I15" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4849,11 +4828,11 @@
         <v>BackRight ESC</v>
       </c>
       <c r="C16" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D16" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E16" s="29" t="str">
@@ -4866,11 +4845,11 @@
       </c>
       <c r="G16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I16" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4911,28 +4890,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C17" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D17" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I17" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4973,11 +4952,11 @@
         <v>FrontLeft ESC</v>
       </c>
       <c r="C18" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D18" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E18" s="29" t="str">
@@ -4990,11 +4969,11 @@
       </c>
       <c r="G18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I18" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5035,28 +5014,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C19" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D19" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I19" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5097,11 +5076,11 @@
         <v>MidLeft ESC</v>
       </c>
       <c r="C20" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D20" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E20" s="29" t="str">
@@ -5114,11 +5093,11 @@
       </c>
       <c r="G20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I20" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5159,28 +5138,28 @@
         <v>Battery Pack</v>
       </c>
       <c r="C21" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D21" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
+        <v>22.2</v>
       </c>
       <c r="E21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="F21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I21" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5221,11 +5200,11 @@
         <v>BackLeft ESC</v>
       </c>
       <c r="C22" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28.8</v>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
+        <v>22.2</v>
       </c>
       <c r="D22" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E22" s="29" t="str">
@@ -5238,11 +5217,11 @@
       </c>
       <c r="G22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="H22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I22" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5283,11 +5262,11 @@
         <v>Dirty Power 1</v>
       </c>
       <c r="C23" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D23" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>12</v>
       </c>
       <c r="E23" s="29">
@@ -5345,11 +5324,11 @@
         <v>Shoulder ESC</v>
       </c>
       <c r="C24" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D24" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E24" s="29" t="str">
@@ -5407,11 +5386,11 @@
         <v>Dirty Power 2</v>
       </c>
       <c r="C25" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D25" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>12</v>
       </c>
       <c r="E25" s="29">
@@ -5469,11 +5448,11 @@
         <v>Base ESC</v>
       </c>
       <c r="C26" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D26" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E26" s="29" t="str">
@@ -5531,11 +5510,11 @@
         <v>Dirty Power 2</v>
       </c>
       <c r="C27" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D27" s="26">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v>12</v>
       </c>
       <c r="E27" s="29">
@@ -5593,11 +5572,11 @@
         <v>Elbow ESC</v>
       </c>
       <c r="C28" s="28">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
       <c r="D28" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E28" s="29" t="str">
@@ -5655,11 +5634,11 @@
         <v/>
       </c>
       <c r="C29" s="28" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v/>
       </c>
       <c r="D29" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E29" s="29" t="str">
@@ -5717,11 +5696,11 @@
         <v/>
       </c>
       <c r="C30" s="28" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v/>
       </c>
       <c r="D30" s="26" t="str">
-        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
         <v/>
       </c>
       <c r="E30" s="29" t="str">
@@ -5784,10 +5763,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5800,35 +5779,34 @@
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
         <v>34</v>
@@ -5836,23 +5814,20 @@
       <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>113</v>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>111</v>
-      </c>
-      <c r="R1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -5885,27 +5860,23 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I2" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-      <c r="O2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="P2">
+      <c r="N2">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>28.8</v>
-      </c>
-      <c r="Q2" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="O2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>266.16145833333331</v>
-      </c>
-      <c r="R2" s="4">
+        <v>346.33108108108109</v>
+      </c>
+      <c r="P2" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
-        <v>7665.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>7688.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Battery Pack</v>
@@ -5916,19 +5887,19 @@
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>266.16145833333331</v>
+        <v>346.33108108108109</v>
       </c>
       <c r="D3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>29.244791666666664</v>
+        <v>38.128378378378379</v>
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.9715663580246912</v>
+        <v>2.5654154154154156</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.21662808641975306</v>
+        <v>0.28243243243243243</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -5936,36 +5907,32 @@
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>0.46162065894924315</v>
-      </c>
-      <c r="I3" s="5">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v>27.697239536954587</v>
-      </c>
-      <c r="K3" t="s">
+        <v>0.35406698564593303</v>
+      </c>
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="12" t="str">
+      <c r="K3" s="12" t="str">
         <f>IF(COUNTIF(Results[Constant % Capacity], "&gt;1")=0, IF(COUNTIF(Results[Peak % Capacity], "&gt;1")=0, "GO", "MAYBE"), "HOLD")</f>
         <v>MAYBE</v>
       </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3">
+      <c r="M3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>24</v>
-      </c>
-      <c r="Q3" s="5">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="R3" s="4">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="P3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Logic Supply</v>
@@ -5998,34 +5965,30 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I4" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-      <c r="K4" t="s">
-        <v>82</v>
-      </c>
-      <c r="L4" s="13" t="str">
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="13" t="str">
         <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00"))</f>
-        <v>0:28</v>
-      </c>
-      <c r="O4" t="s">
+        <v>0:21</v>
+      </c>
+      <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="P4">
+      <c r="N4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>5</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="O4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>1.4</v>
       </c>
-      <c r="R4" s="4">
+      <c r="P4" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Master Control</v>
@@ -6058,50 +6021,46 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I5" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-      <c r="O5" t="s">
-        <v>102</v>
-      </c>
-      <c r="P5">
+      <c r="M5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>12</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="O5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>20</v>
       </c>
-      <c r="R5" s="4">
+      <c r="P5" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Comms Power</v>
+        <v>Network Power</v>
       </c>
       <c r="B6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.33333333333333331</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="D6" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.33333333333333331</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="E6" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.33333333333333331</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="F6" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.33333333333333331</v>
+        <v>0.23333333333333334</v>
       </c>
       <c r="G6" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6111,50 +6070,46 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I6" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-      <c r="O6" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6">
+      <c r="M6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>12</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="O6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>3</v>
       </c>
-      <c r="R6" s="4">
+      <c r="P6" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Transceiver</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="11">
+        <v/>
+      </c>
+      <c r="C7" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.3125</v>
-      </c>
-      <c r="D7" s="11">
+        <v/>
+      </c>
+      <c r="D7" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.3125</v>
-      </c>
-      <c r="E7" s="6">
+        <v/>
+      </c>
+      <c r="E7" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.3125</v>
-      </c>
-      <c r="F7" s="6">
+        <v/>
+      </c>
+      <c r="F7" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.3125</v>
+        <v/>
       </c>
       <c r="G7" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6164,29 +6119,25 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I7" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
+      <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="P7" t="str">
+      <c r="N7" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="Q7" s="5" t="str">
+      <c r="O7" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="R7" s="4" t="str">
+      <c r="P7" s="4" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Antenna</v>
+        <v>Network Switch</v>
       </c>
       <c r="B8" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6216,24 +6167,20 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I8" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-      <c r="P8" t="str">
+      <c r="N8" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="Q8" s="5" t="str">
+      <c r="O8" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="R8" s="4" t="str">
+      <c r="P8" s="4" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Dirty Power 1</v>
@@ -6266,12 +6213,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I9" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Dirty Power 2</v>
@@ -6304,12 +6247,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I10" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight ESC</v>
@@ -6320,19 +6259,19 @@
       </c>
       <c r="C11" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D11" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G11" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6342,12 +6281,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I11" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight Motor</v>
@@ -6380,12 +6315,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I12" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight ESC</v>
@@ -6396,19 +6327,19 @@
       </c>
       <c r="C13" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D13" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F13" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G13" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6418,12 +6349,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I13" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight Motor</v>
@@ -6456,12 +6383,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I14" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight ESC</v>
@@ -6472,19 +6395,19 @@
       </c>
       <c r="C15" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D15" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F15" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G15" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6494,12 +6417,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I15" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight Motor</v>
@@ -6532,12 +6451,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I16" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft ESC</v>
@@ -6548,19 +6463,19 @@
       </c>
       <c r="C17" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D17" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F17" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G17" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6570,12 +6485,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I17" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft Motor</v>
@@ -6608,12 +6519,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I18" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft ESC</v>
@@ -6624,19 +6531,19 @@
       </c>
       <c r="C19" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D19" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F19" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G19" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6646,12 +6553,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I19" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft Motor</v>
@@ -6684,12 +6587,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I20" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft ESC</v>
@@ -6700,19 +6599,19 @@
       </c>
       <c r="C21" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>42.5</v>
+        <v>55.135135135135137</v>
       </c>
       <c r="D21" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.4722222222222223</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="E21" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.70833333333333337</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="F21" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>5.7870370370370371E-2</v>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G21" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6722,12 +6621,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I21" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft Motor</v>
@@ -6760,12 +6655,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I22" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Shoulder ESC</v>
@@ -6798,12 +6689,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I23" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Shoulder Motor</v>
@@ -6836,12 +6723,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I24" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Base ESC</v>
@@ -6874,12 +6757,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I25" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Base Motor</v>
@@ -6912,12 +6791,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I26" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Elbow ESC</v>
@@ -6950,12 +6825,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I27" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Elbow Motor</v>
@@ -6988,12 +6859,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I28" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -7026,12 +6893,8 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I29" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -7064,20 +6927,16 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="I30" s="5" t="str">
-        <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery Life (hrs)]]*60))</f>
-        <v/>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="19" priority="2">
+  <conditionalFormatting sqref="K3">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7093,8 +6952,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 O2:O8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 M2:M8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>ItemIDs</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
@@ -7113,7 +6972,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7129,22 +6988,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -7161,7 +7020,7 @@
         <v/>
       </c>
       <c r="E2" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -7184,7 +7043,7 @@
         <v/>
       </c>
       <c r="E3" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -7207,7 +7066,7 @@
         <v>8.48</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -7242,18 +7101,18 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Comms Power</v>
+        <v>Network Power</v>
       </c>
       <c r="B6" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Homemade POE injection</v>
-      </c>
-      <c r="C6" s="3" t="str">
+        <v>Adjustable Linear Voltage Regulator</v>
+      </c>
+      <c r="C6" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>8.48</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -7269,7 +7128,7 @@
       </c>
       <c r="B7" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Ubiquity Rocket M3</v>
+        <v>Ubiquity Rocket M5</v>
       </c>
       <c r="C7" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
@@ -7288,18 +7147,18 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Antenna</v>
+        <v>Network Switch</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>AMO-3G12 - Ubiquiti Antenna 3.4-3.7 GHz 12dBi Omni-directional</v>
-      </c>
-      <c r="C8" s="3">
+        <v/>
+      </c>
+      <c r="C8" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>150</v>
+        <v/>
       </c>
       <c r="E8" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -7345,7 +7204,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -7368,7 +7227,7 @@
         <v>90</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -7391,7 +7250,7 @@
         <v>7.25</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F12" s="1">
         <v>22</v>
@@ -7547,11 +7406,11 @@
       </c>
       <c r="B23" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C23" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added battery discharge rate
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75AF8C2-AFA4-463C-BDEC-EBC516922DA7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2972F6ED-F05F-4897-81CE-348FBF79C15A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="0" windowWidth="18825" windowHeight="4845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17370" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Costs" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Component Data'!$C$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Component Data'!$C$1:$J$1</definedName>
     <definedName name="ComponentIDs">ComponentData[ID]</definedName>
     <definedName name="ItemIDs">Analysis[ItemID]</definedName>
   </definedNames>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -376,16 +376,35 @@
   </si>
   <si>
     <t>Network Switch</t>
+  </si>
+  <si>
+    <t>BatterySpace</t>
+  </si>
+  <si>
+    <t>http://www.batteryspace.com/lipo-battery-pack-tattu-22-2v-12ah-266wh-15c-6s1p.aspx</t>
+  </si>
+  <si>
+    <t>Output Current Limit (A)</t>
+  </si>
+  <si>
+    <t>Discharge (for batteries)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>12-40V input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#\C"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -458,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -500,12 +519,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="64">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -528,10 +552,13 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="167" formatCode="#\C"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -621,6 +648,12 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -681,9 +714,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -1001,7 +1031,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1024,63 +1054,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:K15" totalsRowShown="0">
-  <autoFilter ref="A1:K15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N15" totalsRowShown="0">
+  <autoFilter ref="A1:N15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="60"/>
+    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="5">
+      <calculatedColumnFormula>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="44">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="48">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="43">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="47">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="42">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="46">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="41">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="45">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="40">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="39">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="38">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="37">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="36">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="35">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="34">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1092,47 +1127,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="37">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="34">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="33">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="30">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="29">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="28">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="23">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="22">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="21">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1144,28 +1179,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="22">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="20">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="14">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1177,14 +1212,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:P8" totalsRowShown="0">
   <autoFilter ref="M1:P8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="13">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="12">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="11">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1196,13 +1231,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="9">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="8">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="7">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1508,13 +1543,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,15 +1558,18 @@
     <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1545,86 +1583,111 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="11">
         <v>0</v>
       </c>
       <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
         <v>28.8</v>
       </c>
-      <c r="I2" s="11">
-        <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*15</f>
-        <v>180</v>
-      </c>
       <c r="J2" s="11">
-        <v>12000</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>100</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="31">
+        <v>10</v>
+      </c>
+      <c r="M2" s="11">
+        <v>10000</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="11">
-        <v>0</v>
+      <c r="C3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3">
+        <v>254</v>
       </c>
       <c r="G3" s="11">
         <v>0</v>
       </c>
       <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
         <v>22.2</v>
       </c>
-      <c r="I3" s="11">
-        <f>ComponentData[[#This Row],[Battery (mAh)]]/1000*10</f>
-        <v>135</v>
-      </c>
       <c r="J3" s="11">
-        <v>13500</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>180</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="31">
+        <v>15</v>
+      </c>
+      <c r="M3" s="11">
+        <v>12000</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -1637,25 +1700,31 @@
       <c r="D4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="7"/>
+      <c r="F4" s="3">
         <v>8.48</v>
       </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
       <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11">
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>12</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="4">
+      <c r="K4" s="11">
+        <v>12</v>
+      </c>
+      <c r="L4" s="31"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="4">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -1668,27 +1737,33 @@
       <c r="D5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.5</v>
       </c>
       <c r="G5" s="11">
         <v>2.5</v>
       </c>
       <c r="H5" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="I5" s="11">
         <v>24</v>
       </c>
-      <c r="I5" s="11">
+      <c r="J5" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>1</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="11">
+        <v>1</v>
+      </c>
+      <c r="L5" s="31"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1697,27 +1772,33 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="3">
+      <c r="E6" s="7"/>
+      <c r="F6" s="3">
         <v>30</v>
-      </c>
-      <c r="F6" s="11">
-        <v>7</v>
       </c>
       <c r="G6" s="11">
         <v>7</v>
       </c>
       <c r="H6" s="11">
+        <v>7</v>
+      </c>
+      <c r="I6" s="11">
         <v>3.3</v>
       </c>
-      <c r="I6" s="11">
+      <c r="J6" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>0.5</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="31"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
@@ -1730,23 +1811,29 @@
       <c r="D7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="7"/>
+      <c r="F7" s="3">
         <v>180</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="11">
         <v>8</v>
       </c>
-      <c r="G7" s="11">
+      <c r="H7" s="11">
         <v>6</v>
       </c>
-      <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>99</v>
       </c>
@@ -1759,27 +1846,33 @@
       <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7"/>
+      <c r="F8" s="3">
         <v>60</v>
       </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
       <c r="G8" s="11">
         <v>0</v>
       </c>
       <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
         <v>12</v>
       </c>
-      <c r="I8" s="11">
+      <c r="J8" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>60</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="11">
+        <v>60</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>107</v>
       </c>
@@ -1790,27 +1883,33 @@
         <v>101</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="3">
+      <c r="E9" s="7"/>
+      <c r="F9" s="3">
         <v>90</v>
       </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
       <c r="G9" s="11">
         <v>0</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="11">
+      <c r="J9" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>60</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="11">
+        <v>60</v>
+      </c>
+      <c r="L9" s="31"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
@@ -1823,24 +1922,30 @@
       <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="7"/>
+      <c r="F10" s="3">
         <v>7.25</v>
       </c>
-      <c r="F10" s="15">
+      <c r="G10" s="15">
         <f>85*14.4</f>
         <v>1224</v>
       </c>
-      <c r="G10" s="15">
+      <c r="H10" s="15">
         <v>100</v>
       </c>
-      <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="J10" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1851,24 +1956,30 @@
       <c r="D11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="7"/>
+      <c r="F11" s="3">
         <v>60</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G11" s="11">
         <v>240</v>
       </c>
-      <c r="G11" s="11">
+      <c r="H11" s="11">
         <f>15*12</f>
         <v>180</v>
       </c>
-      <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="J11" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
@@ -1879,25 +1990,31 @@
       <c r="D12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="7"/>
+      <c r="F12" s="3">
         <v>50</v>
       </c>
-      <c r="F12" s="11">
+      <c r="G12" s="11">
         <f>1.5*12</f>
         <v>18</v>
       </c>
-      <c r="G12" s="11">
+      <c r="H12" s="11">
         <f>1*12</f>
         <v>12</v>
       </c>
-      <c r="H12" s="11"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
@@ -1910,27 +2027,33 @@
       <c r="D13" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="7"/>
+      <c r="F13" s="3">
         <v>40</v>
       </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
       <c r="G13" s="11">
         <v>0</v>
       </c>
       <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
         <v>22</v>
       </c>
-      <c r="I13" s="11">
+      <c r="J13" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>40</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K13" s="11">
+        <v>40</v>
+      </c>
+      <c r="L13" s="31"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>93</v>
       </c>
@@ -1938,58 +2061,74 @@
         <v>95</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="3">
         <v>16</v>
       </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
       <c r="G14" s="11">
         <v>0</v>
       </c>
       <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
         <v>12</v>
       </c>
-      <c r="I14" s="11">
+      <c r="J14" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
         <v>20</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="4">
+      <c r="K14" s="11">
+        <v>20</v>
+      </c>
+      <c r="L14" s="31"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="11">
+      <c r="E15" s="7"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="11">
         <v>24</v>
       </c>
-      <c r="G15" s="11">
+      <c r="H15" s="11">
         <v>8</v>
       </c>
-      <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="4">
+      <c r="J15" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{86EF303B-6B5E-4E0B-8983-28A252B0769B}"/>
+    <hyperlink ref="D14" r:id="rId3" xr:uid="{7D768727-DEDA-40C8-9759-80357E423FFD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1998,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
@@ -2131,15 +2270,15 @@
       </c>
       <c r="F3" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>BatterySpace</v>
       </c>
       <c r="G3" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H3" s="17" t="str">
+        <v>http://www.batteryspace.com/lipo-battery-pack-tattu-22-2v-12ah-266wh-15c-6s1p.aspx</v>
+      </c>
+      <c r="H3" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>254</v>
       </c>
       <c r="I3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2155,11 +2294,11 @@
       </c>
       <c r="L3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="M3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>13500</v>
+        <v>12000</v>
       </c>
       <c r="N3" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2370,9 +2509,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L7" s="18" t="str">
+      <c r="L7" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M7" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2425,9 +2564,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L8" s="18" t="str">
+      <c r="L8" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M8" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2645,9 +2784,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L12" s="18" t="str">
+      <c r="L12" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M12" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2755,9 +2894,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L14" s="18" t="str">
+      <c r="L14" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M14" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2865,9 +3004,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L16" s="18" t="str">
+      <c r="L16" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M16" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2975,9 +3114,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L18" s="18" t="str">
+      <c r="L18" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M18" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3085,9 +3224,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L20" s="18" t="str">
+      <c r="L20" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M20" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3195,9 +3334,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L22" s="18" t="str">
+      <c r="L22" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M22" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3305,9 +3444,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L24" s="18" t="str">
+      <c r="L24" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3415,9 +3554,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L26" s="18" t="str">
+      <c r="L26" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3525,9 +3664,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L28" s="18" t="str">
+      <c r="L28" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -5883,7 +6022,7 @@
       </c>
       <c r="B3">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -5895,19 +6034,19 @@
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>2.5654154154154156</v>
+        <v>1.9240615615615617</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.28243243243243243</v>
+        <v>0.21182432432432433</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>13500</v>
+        <v>12000</v>
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>0.35406698564593303</v>
+        <v>0.31472620946305158</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
@@ -5970,7 +6109,7 @@
       </c>
       <c r="K4" s="13" t="str">
         <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00"))</f>
-        <v>0:21</v>
+        <v>0:19</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
@@ -6091,9 +6230,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Transceiver</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6139,9 +6278,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Network Switch</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C8" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6287,9 +6426,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight Motor</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C12" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6355,9 +6494,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight Motor</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C14" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6423,9 +6562,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight Motor</v>
       </c>
-      <c r="B16" s="1" t="str">
+      <c r="B16" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C16" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6491,9 +6630,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft Motor</v>
       </c>
-      <c r="B18" s="1" t="str">
+      <c r="B18" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C18" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6559,9 +6698,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft Motor</v>
       </c>
-      <c r="B20" s="1" t="str">
+      <c r="B20" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C20" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6627,9 +6766,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft Motor</v>
       </c>
-      <c r="B22" s="1" t="str">
+      <c r="B22" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C22" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6695,9 +6834,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Shoulder Motor</v>
       </c>
-      <c r="B24" s="1" t="str">
+      <c r="B24" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C24" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6763,9 +6902,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Base Motor</v>
       </c>
-      <c r="B26" s="1" t="str">
+      <c r="B26" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C26" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6831,9 +6970,9 @@
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Elbow Motor</v>
       </c>
-      <c r="B28" s="1" t="str">
+      <c r="B28" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C28" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6930,13 +7069,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7038,9 +7177,9 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>24 V Lithuim Ion Battery back</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>254</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Updates to power budget and diagrams
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2972F6ED-F05F-4897-81CE-348FBF79C15A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E3C510-F874-4C7F-BE83-75FAC0E21B47}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17370" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19230" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>12-40V input</t>
+  </si>
+  <si>
+    <t>Peak Current (A)</t>
   </si>
 </sst>
 </file>
@@ -525,41 +528,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#\C"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
+  <dxfs count="65">
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -577,6 +546,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -607,6 +579,27 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -719,6 +712,15 @@
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="#\C"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
@@ -729,6 +731,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1031,7 +1037,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="10">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1057,65 +1063,65 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N15" totalsRowShown="0">
   <autoFilter ref="A1:N15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="60"/>
-    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="60" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="59"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="58"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="57"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="5">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="55">
       <calculatedColumnFormula>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="45">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="47">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="46">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="45">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="44">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="43">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="42">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="41">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="40">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="39">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="38">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1127,47 +1133,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="34">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="33">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="32">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="31">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="30">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="29">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="28">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="27">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="26">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="25">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="24">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="23">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="20">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1179,28 +1185,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="16">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="20">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="11">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="10">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="9">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1209,18 +1215,21 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:P8" totalsRowShown="0">
-  <autoFilter ref="M1:P8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0">
+  <autoFilter ref="M1:Q8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current (A)" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="6">
+      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="4">
+      <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1231,13 +1240,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="2">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="1">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="0">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1549,7 +1558,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,14 +1683,14 @@
       </c>
       <c r="J3" s="11">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="31">
         <v>15</v>
       </c>
       <c r="M3" s="11">
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="N3" s="4">
         <v>0</v>
@@ -2081,10 +2090,10 @@
       </c>
       <c r="J14" s="11">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L14" s="31"/>
       <c r="M14" s="11"/>
@@ -2137,11 +2146,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,11 +2303,11 @@
       </c>
       <c r="L3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="M3" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="N3" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2621,7 +2630,7 @@
       </c>
       <c r="L9" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2676,7 +2685,7 @@
       </c>
       <c r="L10" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -5902,10 +5911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5924,11 +5933,12 @@
     <col min="12" max="12" width="2.42578125" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -5963,10 +5973,13 @@
         <v>105</v>
       </c>
       <c r="P1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -6002,27 +6015,31 @@
       <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>22.2</v>
       </c>
       <c r="O2" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>38.128378378378379</v>
+      </c>
+      <c r="P2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>346.33108108108109</v>
       </c>
-      <c r="P2" s="4">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
+      <c r="Q2" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v>7688.55</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Battery Pack</v>
       </c>
       <c r="B3">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6034,44 +6051,48 @@
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.9240615615615617</v>
+        <v>0.96203078078078086</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.21182432432432433</v>
+        <v>0.10591216216216216</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>0.31472620946305158</v>
+        <v>0.62945241892610315</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
       </c>
       <c r="K3" s="12" t="str">
         <f>IF(COUNTIF(Results[Constant % Capacity], "&gt;1")=0, IF(COUNTIF(Results[Peak % Capacity], "&gt;1")=0, "GO", "MAYBE"), "HOLD")</f>
-        <v>MAYBE</v>
+        <v>GO</v>
       </c>
       <c r="M3" t="s">
         <v>111</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="O3" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="P3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="P3" s="4">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
+      <c r="Q3" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Logic Supply</v>
@@ -6108,26 +6129,30 @@
         <v>77</v>
       </c>
       <c r="K4" s="13" t="str">
-        <f>CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00"))</f>
-        <v>0:19</v>
+        <f>IF(MIN(Results[Battery Life (hrs)]) &lt; 1, CONCATENATE(TEXT(MIN(Results[Battery Life (hrs)])*60, "#.#"), " min"), CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00")))</f>
+        <v>37.8 min</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>5</v>
       </c>
       <c r="O4" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>1.4</v>
+      </c>
+      <c r="P4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>1.4</v>
       </c>
-      <c r="P4" s="4">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
+      <c r="Q4" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Master Control</v>
@@ -6163,20 +6188,24 @@
       <c r="M5" t="s">
         <v>97</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="O5" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="P5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>20</v>
       </c>
-      <c r="P5" s="4">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
+      <c r="Q5" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Network Power</v>
@@ -6212,20 +6241,24 @@
       <c r="M6" t="s">
         <v>98</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>12</v>
       </c>
       <c r="O6" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v>3</v>
       </c>
-      <c r="P6" s="4">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
+      <c r="Q6" s="5">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Transceiver</v>
@@ -6264,16 +6297,20 @@
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="O7" s="5" t="str">
+      <c r="O7" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="P7" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="P7" s="4" t="str">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="4" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Network Switch</v>
@@ -6310,23 +6347,27 @@
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="O8" s="5" t="str">
+      <c r="O8" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="P8" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="P8" s="4" t="str">
-        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Current (A)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="4" t="str">
+        <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Dirty Power 1</v>
       </c>
       <c r="B9">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6338,11 +6379,11 @@
       </c>
       <c r="E9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="F9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.75</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G9" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6353,14 +6394,14 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>Dirty Power 2</v>
       </c>
       <c r="B10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6372,11 +6413,11 @@
       </c>
       <c r="E10" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.15</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="F10" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.1</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="G10" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6387,7 +6428,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight ESC</v>
@@ -6421,7 +6462,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontRight Motor</v>
@@ -6455,7 +6496,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight ESC</v>
@@ -6489,7 +6530,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidRight Motor</v>
@@ -6523,7 +6564,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight ESC</v>
@@ -6557,7 +6598,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight Motor</v>
@@ -7069,13 +7110,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates to the power budget.
1. Removed the arm.
2. Moved [INPUT] substitution to the items page
3. Updated the costs page.
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E3C510-F874-4C7F-BE83-75FAC0E21B47}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F9760-9407-4130-98EF-5D511958517D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19230" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20160" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="ComponentIDs">ComponentData[ID]</definedName>
     <definedName name="ItemIDs">Analysis[ItemID]</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Peak Current (A)</t>
+  </si>
+  <si>
+    <t>Virtual Node for system isolation</t>
+  </si>
+  <si>
+    <t>Drivetrain Power</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,67 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="69">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -540,21 +606,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -579,27 +630,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -753,6 +783,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDCDE80"/>
       <color rgb="FFFFF8CB"/>
       <color rgb="FFFFB985"/>
     </mruColors>
@@ -1037,7 +1068,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1060,68 +1091,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N15" totalsRowShown="0">
-  <autoFilter ref="A1:N15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N16" totalsRowShown="0">
+  <autoFilter ref="A1:N16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="61"/>
-    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="60" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="64" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="59">
       <calculatedColumnFormula>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N35" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N36" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="49">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="48">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="43">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="47">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="42">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="46">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="41">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="45">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="40">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="39">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="38">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="37">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="36">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="35">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1133,47 +1164,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="38">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="31">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="34">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="29">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="33">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="27">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="22">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="21">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="20">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1185,28 +1216,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="23">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="13">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="20">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1215,20 +1246,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0" dataDxfId="0">
   <autoFilter ref="M1:Q8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1240,13 +1271,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1552,13 +1583,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,8 +1967,7 @@
         <v>7.25</v>
       </c>
       <c r="G10" s="15">
-        <f>85*14.4</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="H10" s="15">
         <v>100</v>
@@ -2125,6 +2155,41 @@
       <c r="L15" s="31"/>
       <c r="M15" s="11"/>
       <c r="N15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="11">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="31"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2144,13 +2209,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,25 +2763,25 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>LiPo</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Virtual Node for system isolation</v>
       </c>
       <c r="F11" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Cross The Road Electronics</v>
+        <v/>
       </c>
       <c r="G11" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2724,7 +2789,7 @@
       </c>
       <c r="H11" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I11" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2739,758 +2804,757 @@
         <v>[INPUT]</v>
       </c>
       <c r="L11" s="18">
+        <v>400</v>
+      </c>
+      <c r="M11" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="N11" s="23">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="14" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
+        <v>Power Rail</v>
+      </c>
+      <c r="E12" s="21" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>Talon SRX DC Motor  Driver</v>
+      </c>
+      <c r="F12" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>Cross The Road Electronics</v>
+      </c>
+      <c r="G12" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="H12" s="17">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>90</v>
+      </c>
+      <c r="I12" s="18">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>[INPUT]</v>
+      </c>
+      <c r="L12" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M11" s="18" t="str">
+      <c r="M12" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N11" s="23">
+      <c r="N12" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B13" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="14" t="str">
+      <c r="D13" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E12" s="21" t="str">
+      <c r="E13" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F12" s="16" t="str">
+      <c r="F13" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G12" s="16" t="str">
+      <c r="G13" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H13" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I13" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J12" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J13" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K12" s="18" t="str">
+      <c r="K13" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L12" s="18">
+      <c r="L13" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M12" s="18" t="str">
+      <c r="M13" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N12" s="23">
+      <c r="N13" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="14" t="str">
+      <c r="C14" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiPo</v>
-      </c>
-      <c r="E13" s="21" t="str">
+        <v>Power Rail</v>
+      </c>
+      <c r="E14" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F13" s="16" t="str">
+      <c r="F14" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G13" s="16" t="str">
+      <c r="G14" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H13" s="17">
+      <c r="H14" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I14" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J14" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K13" s="18" t="str">
+      <c r="K14" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L14" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M13" s="18" t="str">
+      <c r="M14" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N13" s="23">
+      <c r="N14" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="14" t="str">
+      <c r="D15" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E14" s="21" t="str">
+      <c r="E15" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F14" s="16" t="str">
+      <c r="F15" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G14" s="16" t="str">
+      <c r="G15" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H15" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I15" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J14" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J15" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K14" s="18" t="str">
+      <c r="K15" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L14" s="18">
+      <c r="L15" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M14" s="18" t="str">
+      <c r="M15" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N14" s="23">
+      <c r="N15" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="14" t="str">
+      <c r="C16" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiPo</v>
-      </c>
-      <c r="E15" s="21" t="str">
+        <v>Power Rail</v>
+      </c>
+      <c r="E16" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F15" s="16" t="str">
+      <c r="F16" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G15" s="16" t="str">
+      <c r="G16" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H15" s="17">
+      <c r="H16" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I16" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J16" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K15" s="18" t="str">
+      <c r="K16" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L16" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M15" s="18" t="str">
+      <c r="M16" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N15" s="23">
+      <c r="N16" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B17" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="14" t="str">
+      <c r="D17" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E16" s="21" t="str">
+      <c r="E17" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F16" s="16" t="str">
+      <c r="F17" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G16" s="16" t="str">
+      <c r="G17" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H17" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I17" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J16" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J17" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K16" s="18" t="str">
+      <c r="K17" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L16" s="18">
+      <c r="L17" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M16" s="18" t="str">
+      <c r="M17" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N16" s="23">
+      <c r="N17" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="14" t="str">
+      <c r="C18" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiPo</v>
-      </c>
-      <c r="E17" s="21" t="str">
+        <v>Power Rail</v>
+      </c>
+      <c r="E18" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F17" s="16" t="str">
+      <c r="F18" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G17" s="16" t="str">
+      <c r="G18" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H17" s="17">
+      <c r="H18" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I18" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J18" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K17" s="18" t="str">
+      <c r="K18" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L18" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M17" s="18" t="str">
+      <c r="M18" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N17" s="23">
+      <c r="N18" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="str">
+      <c r="D19" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E18" s="21" t="str">
+      <c r="E19" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F18" s="16" t="str">
+      <c r="F19" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G18" s="16" t="str">
+      <c r="G19" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H19" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I19" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J18" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J19" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K18" s="18" t="str">
+      <c r="K19" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L18" s="18">
+      <c r="L19" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M18" s="18" t="str">
+      <c r="M19" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N18" s="23">
+      <c r="N19" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B20" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="14" t="str">
+      <c r="C20" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiPo</v>
-      </c>
-      <c r="E19" s="21" t="str">
+        <v>Power Rail</v>
+      </c>
+      <c r="E20" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F19" s="16" t="str">
+      <c r="F20" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G19" s="16" t="str">
+      <c r="G20" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H19" s="17">
+      <c r="H20" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I20" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J20" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K19" s="18" t="str">
+      <c r="K20" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L20" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M19" s="18" t="str">
+      <c r="M20" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N19" s="23">
+      <c r="N20" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="14" t="str">
+      <c r="D21" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E20" s="21" t="str">
+      <c r="E21" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F20" s="16" t="str">
+      <c r="F21" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G20" s="16" t="str">
+      <c r="G21" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H21" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I21" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J20" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J21" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K20" s="18" t="str">
+      <c r="K21" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L20" s="18">
+      <c r="L21" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M20" s="18" t="str">
+      <c r="M21" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N20" s="23">
+      <c r="N21" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B22" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="14" t="str">
+      <c r="C22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>LiPo</v>
-      </c>
-      <c r="E21" s="21" t="str">
+        <v>Power Rail</v>
+      </c>
+      <c r="E22" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F21" s="16" t="str">
+      <c r="F22" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G21" s="16" t="str">
+      <c r="G22" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H21" s="17">
+      <c r="H22" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I22" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J22" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K21" s="18" t="str">
+      <c r="K22" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L22" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M21" s="18" t="str">
+      <c r="M22" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N21" s="23">
+      <c r="N22" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="14" t="str">
+      <c r="D23" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E22" s="21" t="str">
+      <c r="E23" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
-      <c r="F22" s="16" t="str">
+      <c r="F23" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>BaneBot</v>
       </c>
-      <c r="G22" s="16" t="str">
+      <c r="G23" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>http://robotshop.com/en/banebots-rs-550-motor-12v-19300rpm.html</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H23" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>7.25</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I23" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>1224</v>
-      </c>
-      <c r="J22" s="18">
+        <v>1332</v>
+      </c>
+      <c r="J23" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>100</v>
       </c>
-      <c r="K22" s="18" t="str">
+      <c r="K23" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L22" s="18">
+      <c r="L23" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M22" s="18" t="str">
+      <c r="M23" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N22" s="23">
+      <c r="N23" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B24" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="16" t="str">
+      <c r="D24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>20A 24V-&gt;12V Regulator</v>
       </c>
-      <c r="E23" s="21" t="str">
+      <c r="E24" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Talon SRX DC Motor  Driver</v>
       </c>
-      <c r="F23" s="16" t="str">
+      <c r="F24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G23" s="16" t="str">
+      <c r="G24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H23" s="17">
+      <c r="H24" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>90</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I24" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J24" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K23" s="18" t="str">
+      <c r="K24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>[INPUT]</v>
       </c>
-      <c r="L23" s="18">
+      <c r="L24" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M23" s="18" t="str">
+      <c r="M24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N23" s="23">
+      <c r="N24" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="14" t="str">
+      <c r="D25" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>28V VEX ESC</v>
       </c>
-      <c r="E24" s="21" t="str">
+      <c r="E25" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>12 RPM HD Premium Planetary Gear Motor w/Encoder</v>
       </c>
-      <c r="F24" s="16" t="str">
+      <c r="F25" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="G24" s="16" t="str">
+      <c r="G25" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>https://www.servocity.com/12-rpm-hd-premium-planetary-gear-motor-w-encoder</v>
-      </c>
-      <c r="H24" s="17">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
-      </c>
-      <c r="I24" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>240</v>
-      </c>
-      <c r="J24" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>180</v>
-      </c>
-      <c r="K24" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="L24" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="N24" s="23">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="16" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20A 24V-&gt;12V Regulator</v>
-      </c>
-      <c r="E25" s="21" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Victor SP DC Motor Driver</v>
-      </c>
-      <c r="F25" s="16" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Cross The Road Electronics</v>
-      </c>
-      <c r="G25" s="16" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.vexrobotics.com/217-9090.html</v>
       </c>
       <c r="H25" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3498,238 +3562,247 @@
       </c>
       <c r="I25" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="J25" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="18">
+        <v>180</v>
+      </c>
+      <c r="K25" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="L25" s="18">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="N25" s="23">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
+        <v>20A 24V-&gt;12V Regulator</v>
+      </c>
+      <c r="E26" s="21" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>Victor SP DC Motor Driver</v>
+      </c>
+      <c r="F26" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>Cross The Road Electronics</v>
+      </c>
+      <c r="G26" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>https://www.vexrobotics.com/217-9090.html</v>
+      </c>
+      <c r="H26" s="17">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>60</v>
+      </c>
+      <c r="I26" s="18">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="18">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>12</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L26" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M25" s="18" t="str">
+      <c r="M26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N25" s="23">
+      <c r="N26" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="14" t="str">
+      <c r="D27" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>12V VEX ESC</v>
       </c>
-      <c r="E26" s="21" t="str">
+      <c r="E27" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
       </c>
-      <c r="F26" s="16" t="str">
+      <c r="F27" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="G26" s="16" t="str">
+      <c r="G27" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>https://www.servocity.com/26-rpm-premium-planetary-gear-motor-w-encoder</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H27" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>50</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I27" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>18</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J27" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>12</v>
       </c>
-      <c r="K26" s="18" t="str">
+      <c r="K27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L26" s="18">
+      <c r="L27" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="M26" s="18" t="str">
+      <c r="M27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N26" s="23">
+      <c r="N27" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B28" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="16" t="str">
+      <c r="D28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>20A 24V-&gt;12V Regulator</v>
       </c>
-      <c r="E27" s="21" t="str">
+      <c r="E28" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Victor SP DC Motor Driver</v>
       </c>
-      <c r="F27" s="16" t="str">
+      <c r="F28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>Cross The Road Electronics</v>
       </c>
-      <c r="G27" s="16" t="str">
+      <c r="G28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>https://www.vexrobotics.com/217-9090.html</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H28" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I28" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J28" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K28" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>12</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L28" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>60</v>
       </c>
-      <c r="M27" s="18" t="str">
+      <c r="M28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N27" s="23">
+      <c r="N28" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="14" t="str">
+      <c r="D29" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v>12V VEX ESC</v>
       </c>
-      <c r="E28" s="21" t="str">
+      <c r="E29" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
       </c>
-      <c r="F28" s="16" t="str">
+      <c r="F29" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="G28" s="16" t="str">
+      <c r="G29" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>https://www.servocity.com/26-rpm-premium-planetary-gear-motor-w-encoder</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H29" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>50</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I29" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>18</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J29" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v>12</v>
       </c>
-      <c r="K28" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="L28" s="18">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="N28" s="23">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D29" s="14" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E29" s="21" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F29" s="16" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="G29" s="16" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H29" s="17" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I29" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="J29" s="18" t="str">
-        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
       <c r="K29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L29" s="18" t="str">
+      <c r="L29" s="18">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N29" s="23" t="str">
+      <c r="N29" s="23">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3967,7 +4040,7 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="E35" s="16" t="str">
+      <c r="E35" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
@@ -4008,9 +4081,55 @@
         <v/>
       </c>
     </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D36" s="14" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E36" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="F36" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="G36" s="16" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="H36" s="17" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="I36" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="J36" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="K36" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="L36" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="M36" s="18" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+      <c r="N36" s="23" t="str">
+        <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>ComponentIDs</formula1>
     </dataValidation>
   </dataValidations>
@@ -4179,7 +4298,7 @@
       </c>
       <c r="E3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>346.33108108108109</v>
+        <v>375.52027027027026</v>
       </c>
       <c r="F3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
@@ -4203,11 +4322,11 @@
       </c>
       <c r="K3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>7688.55</v>
+        <v>8336.5499999999993</v>
       </c>
       <c r="L3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>7688.55</v>
+        <v>8336.5499999999993</v>
       </c>
       <c r="M3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4659,7 +4778,7 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>FrontRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="B11" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
@@ -4675,19 +4794,19 @@
       </c>
       <c r="E11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>360</v>
       </c>
       <c r="F11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v>27.027027027027028</v>
       </c>
       <c r="G11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>360</v>
       </c>
       <c r="H11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v>27.027027027027028</v>
       </c>
       <c r="I11" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4699,11 +4818,11 @@
       </c>
       <c r="K11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>7992</v>
       </c>
       <c r="L11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>7992</v>
       </c>
       <c r="M11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4711,41 +4830,41 @@
       </c>
       <c r="N11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="O11" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>FrontRight Motor</v>
+        <v>FrontRight ESC</v>
       </c>
       <c r="B12" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>FrontRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C12" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D12" s="26" t="str">
+      <c r="D12" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E12" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F12" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4757,23 +4876,23 @@
       </c>
       <c r="J12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O12" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4783,31 +4902,31 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>MidRight ESC</v>
+        <v>FrontRight Motor</v>
       </c>
       <c r="B13" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Battery Pack</v>
+        <v>FrontRight ESC</v>
       </c>
       <c r="C13" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>22.2</v>
-      </c>
-      <c r="E13" s="29">
+        <v/>
+      </c>
+      <c r="E13" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="F13" s="29">
+        <v/>
+      </c>
+      <c r="F13" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v/>
       </c>
       <c r="G13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4819,23 +4938,23 @@
       </c>
       <c r="J13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="L13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O13" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4845,31 +4964,31 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>MidRight Motor</v>
+        <v>MidRight ESC</v>
       </c>
       <c r="B14" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>MidRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C14" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D14" s="26" t="str">
+      <c r="D14" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E14" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F14" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4881,23 +5000,23 @@
       </c>
       <c r="J14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O14" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4907,31 +5026,31 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>BackRight ESC</v>
+        <v>MidRight Motor</v>
       </c>
       <c r="B15" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Battery Pack</v>
+        <v>MidRight ESC</v>
       </c>
       <c r="C15" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>22.2</v>
-      </c>
-      <c r="E15" s="29">
+        <v/>
+      </c>
+      <c r="E15" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="F15" s="29">
+        <v/>
+      </c>
+      <c r="F15" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v/>
       </c>
       <c r="G15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4943,23 +5062,23 @@
       </c>
       <c r="J15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="L15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O15" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4969,31 +5088,31 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>BackRight Motor</v>
+        <v>BackRight ESC</v>
       </c>
       <c r="B16" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>BackRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C16" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D16" s="26" t="str">
+      <c r="D16" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E16" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F16" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5005,23 +5124,23 @@
       </c>
       <c r="J16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O16" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5031,31 +5150,31 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>FrontLeft ESC</v>
+        <v>BackRight Motor</v>
       </c>
       <c r="B17" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Battery Pack</v>
+        <v>BackRight ESC</v>
       </c>
       <c r="C17" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>22.2</v>
-      </c>
-      <c r="E17" s="29">
+        <v/>
+      </c>
+      <c r="E17" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="F17" s="29">
+        <v/>
+      </c>
+      <c r="F17" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v/>
       </c>
       <c r="G17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5067,23 +5186,23 @@
       </c>
       <c r="J17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="L17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O17" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5093,31 +5212,31 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>FrontLeft Motor</v>
+        <v>FrontLeft ESC</v>
       </c>
       <c r="B18" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>FrontLeft ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C18" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D18" s="26" t="str">
+      <c r="D18" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E18" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F18" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5129,23 +5248,23 @@
       </c>
       <c r="J18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5155,31 +5274,31 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>MidLeft ESC</v>
+        <v>FrontLeft Motor</v>
       </c>
       <c r="B19" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Battery Pack</v>
+        <v>FrontLeft ESC</v>
       </c>
       <c r="C19" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>22.2</v>
-      </c>
-      <c r="E19" s="29">
+        <v/>
+      </c>
+      <c r="E19" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="F19" s="29">
+        <v/>
+      </c>
+      <c r="F19" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v/>
       </c>
       <c r="G19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5191,23 +5310,23 @@
       </c>
       <c r="J19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="L19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O19" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5217,31 +5336,31 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>MidLeft Motor</v>
+        <v>MidLeft ESC</v>
       </c>
       <c r="B20" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>MidLeft ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C20" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D20" s="26" t="str">
+      <c r="D20" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E20" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F20" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5253,23 +5372,23 @@
       </c>
       <c r="J20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O20" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5279,31 +5398,31 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>BackLeft ESC</v>
+        <v>MidLeft Motor</v>
       </c>
       <c r="B21" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Battery Pack</v>
+        <v>MidLeft ESC</v>
       </c>
       <c r="C21" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>22.2</v>
-      </c>
-      <c r="E21" s="29">
+        <v/>
+      </c>
+      <c r="E21" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="F21" s="29">
+        <v/>
+      </c>
+      <c r="F21" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.5045045045045047</v>
+        <v/>
       </c>
       <c r="G21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5315,23 +5434,23 @@
       </c>
       <c r="J21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="L21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O21" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5341,31 +5460,31 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>BackLeft Motor</v>
+        <v>BackLeft ESC</v>
       </c>
       <c r="B22" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>BackLeft ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="C22" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>22.2</v>
       </c>
-      <c r="D22" s="26" t="str">
+      <c r="D22" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E22" s="29" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="E22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F22" s="29" t="str">
+        <v>60</v>
+      </c>
+      <c r="F22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>4.5045045045045047</v>
       </c>
       <c r="G22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>55.135135135135137</v>
+        <v>60</v>
       </c>
       <c r="H22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5377,23 +5496,23 @@
       </c>
       <c r="J22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="K22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="L22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>1224</v>
+        <v>1332</v>
       </c>
       <c r="M22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O22" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5403,35 +5522,35 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
+        <v>BackLeft Motor</v>
       </c>
       <c r="B23" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 1</v>
+        <v>BackLeft ESC</v>
       </c>
       <c r="C23" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
-      </c>
-      <c r="D23" s="26">
+        <v>22.2</v>
+      </c>
+      <c r="D23" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E23" s="29">
+        <v/>
+      </c>
+      <c r="E23" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>20</v>
-      </c>
-      <c r="F23" s="29">
+        <v/>
+      </c>
+      <c r="F23" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="G23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="H23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>15</v>
+        <v>4.5045045045045047</v>
       </c>
       <c r="I23" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5439,53 +5558,53 @@
       </c>
       <c r="J23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="K23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="L23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>240</v>
+        <v>1332</v>
       </c>
       <c r="M23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="O23" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>180</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
+        <v>Shoulder ESC</v>
       </c>
       <c r="B24" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Shoulder ESC</v>
+        <v>Dirty Power 1</v>
       </c>
       <c r="C24" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
-      <c r="D24" s="26" t="str">
+      <c r="D24" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E24" s="29" t="str">
+        <v>12</v>
+      </c>
+      <c r="E24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F24" s="29" t="str">
+        <v>20</v>
+      </c>
+      <c r="F24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="G24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5501,11 +5620,11 @@
       </c>
       <c r="J24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="K24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="L24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -5513,11 +5632,11 @@
       </c>
       <c r="M24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="N24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="O24" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5527,35 +5646,35 @@
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
+        <v>Shoulder Motor</v>
       </c>
       <c r="B25" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 2</v>
+        <v>Shoulder ESC</v>
       </c>
       <c r="C25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E25" s="29">
+        <v/>
+      </c>
+      <c r="E25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="F25" s="29">
+        <v/>
+      </c>
+      <c r="F25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="H25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I25" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -5563,53 +5682,53 @@
       </c>
       <c r="J25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="K25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
+        <v>240</v>
       </c>
       <c r="M25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="N25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
+        <v>Base ESC</v>
       </c>
       <c r="B26" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Base ESC</v>
+        <v>Dirty Power 2</v>
       </c>
       <c r="C26" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
-      <c r="D26" s="26" t="str">
+      <c r="D26" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E26" s="29" t="str">
+        <v>12</v>
+      </c>
+      <c r="E26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F26" s="29" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="F26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5625,11 +5744,11 @@
       </c>
       <c r="J26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -5637,11 +5756,11 @@
       </c>
       <c r="M26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O26" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5651,27 +5770,27 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
+        <v>Base Motor</v>
       </c>
       <c r="B27" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 2</v>
+        <v>Base ESC</v>
       </c>
       <c r="C27" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E27" s="29">
+        <v/>
+      </c>
+      <c r="E27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="F27" s="29">
+        <v/>
+      </c>
+      <c r="F27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5687,11 +5806,11 @@
       </c>
       <c r="J27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -5699,11 +5818,11 @@
       </c>
       <c r="M27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O27" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5713,27 +5832,27 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
+        <v>Elbow ESC</v>
       </c>
       <c r="B28" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Elbow ESC</v>
+        <v>Dirty Power 2</v>
       </c>
       <c r="C28" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
         <v>12</v>
       </c>
-      <c r="D28" s="26" t="str">
+      <c r="D28" s="26">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E28" s="29" t="str">
+        <v>12</v>
+      </c>
+      <c r="E28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
-      </c>
-      <c r="F28" s="29" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="F28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -5749,11 +5868,11 @@
       </c>
       <c r="J28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -5761,11 +5880,11 @@
       </c>
       <c r="M28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O28" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -5775,15 +5894,15 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v/>
+        <v>Elbow Motor</v>
       </c>
       <c r="B29" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="C29" s="28" t="str">
+        <v>Elbow ESC</v>
+      </c>
+      <c r="C29" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="D29" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
@@ -5797,41 +5916,41 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G29" s="29" t="str">
+      <c r="G29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
-      </c>
-      <c r="H29" s="29" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="H29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
-      </c>
-      <c r="I29" s="30" t="str">
+        <v>1</v>
+      </c>
+      <c r="I29" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J29" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="J29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="K29" s="29" t="str">
+        <v>18</v>
+      </c>
+      <c r="K29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="L29" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="L29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="M29" s="29" t="str">
+        <v>18</v>
+      </c>
+      <c r="M29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="N29" s="29" t="str">
+        <v>12</v>
+      </c>
+      <c r="N29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="O29" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="O29" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -5913,8 +6032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5931,7 +6050,7 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="2.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
@@ -6012,7 +6131,7 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="5">
@@ -6025,11 +6144,11 @@
       </c>
       <c r="P2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>346.33108108108109</v>
+        <v>375.52027027027026</v>
       </c>
       <c r="Q2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>7688.55</v>
+        <v>8336.5499999999993</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -6043,7 +6162,7 @@
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>346.33108108108109</v>
+        <v>375.52027027027026</v>
       </c>
       <c r="D3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6051,7 +6170,7 @@
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.96203078078078086</v>
+        <v>1.0431118618618618</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -6070,9 +6189,9 @@
       </c>
       <c r="K3" s="12" t="str">
         <f>IF(COUNTIF(Results[Constant % Capacity], "&gt;1")=0, IF(COUNTIF(Results[Peak % Capacity], "&gt;1")=0, "GO", "MAYBE"), "HOLD")</f>
-        <v>GO</v>
-      </c>
-      <c r="M3" t="s">
+        <v>MAYBE</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>111</v>
       </c>
       <c r="N3" s="5">
@@ -6132,7 +6251,7 @@
         <f>IF(MIN(Results[Battery Life (hrs)]) &lt; 1, CONCATENATE(TEXT(MIN(Results[Battery Life (hrs)])*60, "#.#"), " min"), CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00")))</f>
         <v>37.8 min</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="5">
@@ -6185,7 +6304,7 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="5" t="s">
         <v>97</v>
       </c>
       <c r="N5" s="5">
@@ -6238,7 +6357,7 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="5" t="s">
         <v>98</v>
       </c>
       <c r="N6" s="5">
@@ -6293,21 +6412,24 @@
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="N7" t="str">
+      <c r="M7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="O7" t="str">
+        <v>22.2</v>
+      </c>
+      <c r="O7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="P7" s="5" t="str">
+        <v>27.027027027027028</v>
+      </c>
+      <c r="P7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="4" t="str">
+        <v>360</v>
+      </c>
+      <c r="Q7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v/>
+        <v>7992</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6343,11 +6465,12 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-      <c r="N8" t="str">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="O8" t="str">
+      <c r="O8" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
@@ -6355,7 +6478,7 @@
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
         <v/>
       </c>
-      <c r="Q8" s="4" t="str">
+      <c r="Q8" s="5" t="str">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
         <v/>
       </c>
@@ -6431,27 +6554,27 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="B11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
+        <v>400</v>
       </c>
       <c r="C11" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
+        <v>360</v>
       </c>
       <c r="D11" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
+        <v>27.027027027027028</v>
       </c>
       <c r="E11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
+        <v>0.9</v>
       </c>
       <c r="F11" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v>6.7567567567567571E-2</v>
       </c>
       <c r="G11" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6465,27 +6588,27 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontRight Motor</v>
+        <v>FrontRight ESC</v>
       </c>
       <c r="B12">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C12" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D12" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D12" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E12" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E12" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F12" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G12" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6499,27 +6622,27 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidRight ESC</v>
+        <v>FrontRight Motor</v>
       </c>
       <c r="B13">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="D13" s="11">
+        <v/>
+      </c>
+      <c r="D13" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
-      </c>
-      <c r="E13" s="6">
+        <v/>
+      </c>
+      <c r="E13" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="F13" s="6">
+        <v/>
+      </c>
+      <c r="F13" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v/>
       </c>
       <c r="G13" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6533,27 +6656,27 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidRight Motor</v>
+        <v>MidRight ESC</v>
       </c>
       <c r="B14">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C14" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D14" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D14" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E14" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F14" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G14" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6567,27 +6690,27 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackRight ESC</v>
+        <v>MidRight Motor</v>
       </c>
       <c r="B15" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="D15" s="11">
+        <v/>
+      </c>
+      <c r="D15" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
-      </c>
-      <c r="E15" s="6">
+        <v/>
+      </c>
+      <c r="E15" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="F15" s="6">
+        <v/>
+      </c>
+      <c r="F15" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v/>
       </c>
       <c r="G15" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6601,27 +6724,27 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackRight Motor</v>
+        <v>BackRight ESC</v>
       </c>
       <c r="B16" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C16" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D16" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D16" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E16" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E16" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F16" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G16" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6635,27 +6758,27 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontLeft ESC</v>
+        <v>BackRight Motor</v>
       </c>
       <c r="B17" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="D17" s="11">
+        <v/>
+      </c>
+      <c r="D17" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
-      </c>
-      <c r="E17" s="6">
+        <v/>
+      </c>
+      <c r="E17" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="F17" s="6">
+        <v/>
+      </c>
+      <c r="F17" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v/>
       </c>
       <c r="G17" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6669,27 +6792,27 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontLeft Motor</v>
+        <v>FrontLeft ESC</v>
       </c>
       <c r="B18" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C18" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D18" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D18" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E18" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E18" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F18" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G18" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6703,27 +6826,27 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidLeft ESC</v>
+        <v>FrontLeft Motor</v>
       </c>
       <c r="B19" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="D19" s="11">
+        <v/>
+      </c>
+      <c r="D19" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
-      </c>
-      <c r="E19" s="6">
+        <v/>
+      </c>
+      <c r="E19" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="F19" s="6">
+        <v/>
+      </c>
+      <c r="F19" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v/>
       </c>
       <c r="G19" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6737,27 +6860,27 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidLeft Motor</v>
+        <v>MidLeft ESC</v>
       </c>
       <c r="B20" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C20" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D20" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D20" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E20" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E20" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F20" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G20" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6771,27 +6894,27 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackLeft ESC</v>
+        <v>MidLeft Motor</v>
       </c>
       <c r="B21" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>55.135135135135137</v>
-      </c>
-      <c r="D21" s="11">
+        <v/>
+      </c>
+      <c r="D21" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.5045045045045047</v>
-      </c>
-      <c r="E21" s="6">
+        <v/>
+      </c>
+      <c r="E21" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="F21" s="6">
+        <v/>
+      </c>
+      <c r="F21" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>7.5075075075075076E-2</v>
+        <v/>
       </c>
       <c r="G21" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6805,27 +6928,27 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackLeft Motor</v>
+        <v>BackLeft ESC</v>
       </c>
       <c r="B22" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C22" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D22" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="D22" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E22" s="6" t="str">
+        <v>4.5045045045045047</v>
+      </c>
+      <c r="E22" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F22" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>7.5075075075075076E-2</v>
       </c>
       <c r="G22" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6839,27 +6962,27 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
+        <v>BackLeft Motor</v>
       </c>
       <c r="B23" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>20</v>
-      </c>
-      <c r="D23" s="11">
+        <v/>
+      </c>
+      <c r="D23" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>15</v>
-      </c>
-      <c r="E23" s="6">
+        <v/>
+      </c>
+      <c r="E23" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F23" s="6">
+        <v/>
+      </c>
+      <c r="F23" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.25</v>
+        <v/>
       </c>
       <c r="G23" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6873,27 +6996,27 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
+        <v>Shoulder ESC</v>
       </c>
       <c r="B24" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C24" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D24" s="11" t="str">
+        <v>20</v>
+      </c>
+      <c r="D24" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E24" s="6" t="str">
+        <v>15</v>
+      </c>
+      <c r="E24" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F24" s="6" t="str">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F24" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="G24" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6907,27 +7030,27 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
+        <v>Shoulder Motor</v>
       </c>
       <c r="B25" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C25" s="11">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.5</v>
-      </c>
-      <c r="D25" s="11">
+        <v/>
+      </c>
+      <c r="D25" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="E25" s="6">
+        <v/>
+      </c>
+      <c r="E25" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F25" s="6">
+        <v/>
+      </c>
+      <c r="F25" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="G25" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6941,27 +7064,27 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
+        <v>Base ESC</v>
       </c>
       <c r="B26" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C26" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D26" s="11" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E26" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F26" s="6" t="str">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F26" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="G26" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6975,27 +7098,27 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
+        <v>Base Motor</v>
       </c>
       <c r="B27" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="11">
+        <v/>
+      </c>
+      <c r="D27" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="6">
+        <v/>
+      </c>
+      <c r="E27" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F27" s="6">
+        <v/>
+      </c>
+      <c r="F27" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="G27" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7009,27 +7132,27 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
+        <v>Elbow ESC</v>
       </c>
       <c r="B28" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="11" t="str">
+        <v>60</v>
+      </c>
+      <c r="C28" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="D28" s="11" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="D28" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E28" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
-      </c>
-      <c r="F28" s="6" t="str">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F28" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v/>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="G28" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7043,11 +7166,11 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v/>
-      </c>
-      <c r="B29" s="1" t="str">
+        <v>Elbow Motor</v>
+      </c>
+      <c r="B29" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C29" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7110,13 +7233,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7124,10 +7247,10 @@
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.95"/>
         <cfvo type="num" val="1"/>
+        <cfvo type="num" val="1.1000000000000001"/>
         <color rgb="FF00B050"/>
-        <color theme="9" tint="0.39997558519241921"/>
+        <color rgb="FFDCDE80"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
@@ -7396,15 +7519,15 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontRight ESC</v>
+        <v>Drivetrain Power</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Virtual Node for system isolation</v>
       </c>
       <c r="C11" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>85</v>
@@ -7419,15 +7542,15 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontRight Motor</v>
+        <v>FrontRight ESC</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C12" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>60</v>
@@ -7442,179 +7565,179 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidRight ESC</v>
+        <v>FrontRight Motor</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C13" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidRight Motor</v>
+        <v>MidRight ESC</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C14" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackRight ESC</v>
+        <v>MidRight Motor</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C15" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackRight Motor</v>
+        <v>BackRight ESC</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C16" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontLeft ESC</v>
+        <v>BackRight Motor</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C17" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>FrontLeft Motor</v>
+        <v>FrontLeft ESC</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C18" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidLeft ESC</v>
+        <v>FrontLeft Motor</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C19" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>MidLeft Motor</v>
+        <v>MidLeft ESC</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C20" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackLeft ESC</v>
+        <v>MidLeft Motor</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C21" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>BackLeft Motor</v>
+        <v>BackLeft ESC</v>
       </c>
       <c r="B22" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C22" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>7.25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
+        <v>BackLeft Motor</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v>Banebots RS-550 Motor 19300rpm 12V 70.55oz-in</v>
       </c>
       <c r="C23" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
+        <v>Shoulder ESC</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12 RPM HD Premium Planetary Gear Motor w/Encoder</v>
+        <v>Talon SRX DC Motor  Driver</v>
       </c>
       <c r="C24" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
+        <v>Shoulder Motor</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v>12 RPM HD Premium Planetary Gear Motor w/Encoder</v>
       </c>
       <c r="C25" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
@@ -7624,57 +7747,57 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
+        <v>Base ESC</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
+        <v>Victor SP DC Motor Driver</v>
       </c>
       <c r="C26" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
+        <v>Base Motor</v>
       </c>
       <c r="B27" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
       </c>
       <c r="C27" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
+        <v>Elbow ESC</v>
       </c>
       <c r="B28" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
+        <v>Victor SP DC Motor Driver</v>
       </c>
       <c r="C28" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v/>
+        <v>Elbow Motor</v>
       </c>
       <c r="B29" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="C29" s="3" t="str">
+        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
+      </c>
+      <c r="C29" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified the power budget.
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F9760-9407-4130-98EF-5D511958517D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010B741B-B0ED-4FD4-8196-4F960705E830}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21090" yWindow="0" windowWidth="18825" windowHeight="4845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="ComponentIDs">ComponentData[ID]</definedName>
     <definedName name="ItemIDs">Analysis[ItemID]</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -195,9 +195,6 @@
     <t>12 RPM HD Premium Planetary Gear Motor w/Encoder</t>
   </si>
   <si>
-    <t>Shoulder Motor</t>
-  </si>
-  <si>
     <t>12RPM Motor</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>26 RPM Premium Planetary Gear Motor w/Encoder</t>
   </si>
   <si>
-    <t>Base Motor</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>Nextrox DC/DC Converter Regulator 24V Step Down to 12V 20A 240W</t>
   </si>
   <si>
-    <t>Elbow Motor</t>
-  </si>
-  <si>
     <t>Dirty Power 1</t>
   </si>
   <si>
@@ -343,15 +334,6 @@
   </si>
   <si>
     <t>Cross The Road Electronics</t>
-  </si>
-  <si>
-    <t>Shoulder ESC</t>
-  </si>
-  <si>
-    <t>Base ESC</t>
-  </si>
-  <si>
-    <t>Elbow ESC</t>
   </si>
   <si>
     <t>Current (A)</t>
@@ -534,46 +516,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="66">
     <dxf>
       <fill>
         <patternFill>
@@ -606,6 +549,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -797,6 +758,980 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Power Consumption </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:ofPieChart>
+        <c:ofPieType val="pie"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-41D2-4A06-A110-88B00327187D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-41D2-4A06-A110-88B00327187D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$M$13:$M$17</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Drivetrain Power</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Network Power</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logic Supply</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dirty Power 1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dirty Power 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$N$13:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41D2-4A06-A110-88B00327187D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:splitType val="pos"/>
+        <c:splitPos val="4"/>
+        <c:secondPieSize val="104"/>
+        <c:serLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:serLines>
+      </c:ofPieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="333">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9B84DA-8EEC-42BE-AC81-C6361D5F3EF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,7 +2003,7 @@
     <dataField name="Total Cost" fld="3" baseField="1" baseItem="1" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="15">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1094,65 +2029,65 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N16" totalsRowShown="0">
   <autoFilter ref="A1:N16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="64" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Source" dataDxfId="62"/>
+    <tableColumn id="14" xr3:uid="{6A244259-BB2A-459C-B0E1-991C19EA0C8F}" name="Notes" dataDxfId="61" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Peak Consumption (W)" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Constant Consumption (W)" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Output (V)" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Output (A)" dataDxfId="56">
       <calculatedColumnFormula>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="58"/>
-    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{EAB38889-81D8-483D-81AD-0E87BE980AFE}" name="Output Current Limit (A)" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{7019C30C-0028-430A-9C9F-F1D685462011}" name="Discharge (for batteries)" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Battery (mAh)" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Thoughput Loss" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N36" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Items" displayName="Items" ref="A1:N36" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ItemID" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Component" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Supply Item" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Supply Component" dataDxfId="46">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Name" dataDxfId="45">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Manufacturer" dataDxfId="44">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Source" dataDxfId="43">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Price" dataDxfId="42">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Peak Consumption (W)" dataDxfId="41">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Constant Consumption (W)" dataDxfId="40">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Output (V)" dataDxfId="39">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="41">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Output (A)" dataDxfId="38">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="40">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Battery (mAh)" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="39">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Thoughput Loss" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1164,47 +2099,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Analysis" displayName="Analysis" ref="A1:O30" totalsRowShown="0">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ItemID" dataDxfId="35">
       <calculatedColumnFormula>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="36">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Supply Item" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Input (V)" dataDxfId="33">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Output (V)" dataDxfId="32">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Peak Output (A)" dataDxfId="31">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="33">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Constant Output (A)" dataDxfId="30">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="32">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Peak Input (A)" dataDxfId="29">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="31">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Constant Input (A)" dataDxfId="28">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="30">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Thoughput Loss" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="29">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Self Peak Consumption (W)" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="28">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Children Peak Consumption (W)" dataDxfId="25">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="27">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Total Peak Consumption (W)" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="26">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Self Constant Consumption (W)" dataDxfId="23">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="25">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Children Constant Consumption (W)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="24">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Total Constant Consumption (W)" dataDxfId="21">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1216,28 +2151,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H30" totalsRowShown="0">
   <autoFilter ref="A1:H30" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="20">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="19">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1246,20 +2181,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0" dataDxfId="12">
   <autoFilter ref="M1:Q8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="9">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1271,13 +2206,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C30">
   <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="5">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="4">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="count" dataDxfId="3">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1589,7 +2524,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,16 +2558,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
@@ -1641,21 +2576,21 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="L1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
         <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1691,13 +2626,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="3">
@@ -1729,16 +2664,16 @@
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="3">
@@ -1840,10 +2775,10 @@
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>37</v>
@@ -1875,13 +2810,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>7</v>
@@ -1914,13 +2849,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1934,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J9" s="11">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -1986,7 +2921,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>51</v>
@@ -2020,14 +2955,14 @@
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="3">
@@ -2055,16 +2990,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="3">
@@ -2094,17 +3029,17 @@
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
         <v>93</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F14" s="3">
         <v>16</v>
@@ -2133,7 +3068,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2163,7 +3098,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="7"/>
@@ -2178,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J16" s="11">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -2211,11 +3146,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,10 +3197,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>10</v>
@@ -2277,7 +3212,7 @@
         <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2384,7 +3319,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>12</v>
@@ -2490,10 +3425,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>12</v>
@@ -2546,10 +3481,10 @@
         <v>40</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2598,13 +3533,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D8" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2653,10 +3588,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>12</v>
@@ -2708,10 +3643,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>12</v>
@@ -2763,7 +3698,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>45</v>
@@ -2820,10 +3755,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D12" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2930,10 +3865,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D14" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3040,10 +3975,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D16" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3150,10 +4085,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D18" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3260,10 +4195,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D20" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3370,10 +4305,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D22" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3476,77 +4411,59 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>97</v>
-      </c>
       <c r="D24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20A 24V-&gt;12V Regulator</v>
+        <v/>
       </c>
       <c r="E24" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Talon SRX DC Motor  Driver</v>
+        <v/>
       </c>
       <c r="F24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Cross The Road Electronics</v>
+        <v/>
       </c>
       <c r="G24" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>90</v>
-      </c>
-      <c r="I24" s="18">
+        <v/>
+      </c>
+      <c r="I24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
+        <v/>
+      </c>
+      <c r="J24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="K24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>[INPUT]</v>
-      </c>
-      <c r="L24" s="18">
+        <v/>
+      </c>
+      <c r="L24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
+        <v/>
       </c>
       <c r="M24" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>102</v>
-      </c>
       <c r="D25" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>28V VEX ESC</v>
+        <v/>
       </c>
       <c r="E25" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12 RPM HD Premium Planetary Gear Motor w/Encoder</v>
+        <v/>
       </c>
       <c r="F25" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3554,109 +4471,91 @@
       </c>
       <c r="G25" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.servocity.com/12-rpm-hd-premium-planetary-gear-motor-w-encoder</v>
-      </c>
-      <c r="H25" s="17">
+        <v/>
+      </c>
+      <c r="H25" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
-      </c>
-      <c r="I25" s="18">
+        <v/>
+      </c>
+      <c r="I25" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>240</v>
-      </c>
-      <c r="J25" s="18">
+        <v/>
+      </c>
+      <c r="J25" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>180</v>
+        <v/>
       </c>
       <c r="K25" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="M25" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N25" s="23">
+      <c r="N25" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="D26" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20A 24V-&gt;12V Regulator</v>
+        <v/>
       </c>
       <c r="E26" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v/>
       </c>
       <c r="F26" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Cross The Road Electronics</v>
+        <v/>
       </c>
       <c r="G26" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.vexrobotics.com/217-9090.html</v>
-      </c>
-      <c r="H26" s="17">
+        <v/>
+      </c>
+      <c r="H26" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
-      </c>
-      <c r="I26" s="18">
+        <v/>
+      </c>
+      <c r="I26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
+        <v/>
+      </c>
+      <c r="J26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="18">
+        <v/>
+      </c>
+      <c r="K26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="L26" s="18">
+        <v/>
+      </c>
+      <c r="L26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
+        <v/>
       </c>
       <c r="M26" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N26" s="23">
+      <c r="N26" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>103</v>
-      </c>
       <c r="D27" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12V VEX ESC</v>
+        <v/>
       </c>
       <c r="E27" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
+        <v/>
       </c>
       <c r="F27" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3664,109 +4563,91 @@
       </c>
       <c r="G27" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.servocity.com/26-rpm-premium-planetary-gear-motor-w-encoder</v>
-      </c>
-      <c r="H27" s="17">
+        <v/>
+      </c>
+      <c r="H27" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>50</v>
-      </c>
-      <c r="I27" s="18">
+        <v/>
+      </c>
+      <c r="I27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>18</v>
-      </c>
-      <c r="J27" s="18">
+        <v/>
+      </c>
+      <c r="J27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="K27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="M27" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N27" s="23">
+      <c r="N27" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="D28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>20A 24V-&gt;12V Regulator</v>
+        <v/>
       </c>
       <c r="E28" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Victor SP DC Motor Driver</v>
+        <v/>
       </c>
       <c r="F28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Cross The Road Electronics</v>
+        <v/>
       </c>
       <c r="G28" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.vexrobotics.com/217-9090.html</v>
-      </c>
-      <c r="H28" s="17">
+        <v/>
+      </c>
+      <c r="H28" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
-      </c>
-      <c r="I28" s="18">
+        <v/>
+      </c>
+      <c r="I28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="18">
+        <v/>
+      </c>
+      <c r="J28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
+        <v/>
+      </c>
+      <c r="K28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="L28" s="18">
+        <v/>
+      </c>
+      <c r="L28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>60</v>
+        <v/>
       </c>
       <c r="M28" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>104</v>
-      </c>
       <c r="D29" s="14" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12V VEX ESC</v>
+        <v/>
       </c>
       <c r="E29" s="21" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
+        <v/>
       </c>
       <c r="F29" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3774,35 +4655,35 @@
       </c>
       <c r="G29" s="16" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>https://www.servocity.com/26-rpm-premium-planetary-gear-motor-w-encoder</v>
-      </c>
-      <c r="H29" s="17">
+        <v/>
+      </c>
+      <c r="H29" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>50</v>
-      </c>
-      <c r="I29" s="18">
+        <v/>
+      </c>
+      <c r="I29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>18</v>
-      </c>
-      <c r="J29" s="18">
+        <v/>
+      </c>
+      <c r="J29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="K29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (V)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="L29" s="18">
+      <c r="L29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="M29" s="18" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="23" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -4181,43 +5062,43 @@
         <v>35</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>74</v>
-      </c>
       <c r="G1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>73</v>
-      </c>
       <c r="I1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>68</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4298,11 +5179,11 @@
       </c>
       <c r="E3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>375.52027027027026</v>
+        <v>361.84459459459458</v>
       </c>
       <c r="F3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>38.128378378378379</v>
+        <v>28.02027027027027</v>
       </c>
       <c r="G3" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4322,11 +5203,11 @@
       </c>
       <c r="K3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>8336.5499999999993</v>
+        <v>8032.95</v>
       </c>
       <c r="L3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>8336.5499999999993</v>
+        <v>8032.95</v>
       </c>
       <c r="M3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4334,11 +5215,11 @@
       </c>
       <c r="N3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>846.45</v>
+        <v>622.04999999999995</v>
       </c>
       <c r="O3" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>846.45</v>
+        <v>622.04999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4670,19 +5551,19 @@
       </c>
       <c r="E9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>11.891891891891893</v>
+        <v>0</v>
       </c>
       <c r="H9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>8.9189189189189193</v>
+        <v>0</v>
       </c>
       <c r="I9" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4690,27 +5571,27 @@
       </c>
       <c r="J9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="L9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="M9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="O9" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4732,19 +5613,19 @@
       </c>
       <c r="E10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.783783783783784</v>
+        <v>0</v>
       </c>
       <c r="H10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.1891891891891893</v>
+        <v>0</v>
       </c>
       <c r="I10" s="30">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4752,27 +5633,27 @@
       </c>
       <c r="J10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="K10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="L10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>39.6</v>
+        <v>0</v>
       </c>
       <c r="M10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>2.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="N10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="O10" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>26.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -5584,77 +6465,77 @@
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
+        <v/>
       </c>
       <c r="B24" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 1</v>
-      </c>
-      <c r="C24" s="28">
+        <v/>
+      </c>
+      <c r="C24" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
-      </c>
-      <c r="D24" s="26">
+        <v/>
+      </c>
+      <c r="D24" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E24" s="29">
+        <v/>
+      </c>
+      <c r="E24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>20</v>
-      </c>
-      <c r="F24" s="29">
+        <v/>
+      </c>
+      <c r="F24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>15</v>
-      </c>
-      <c r="G24" s="29">
+        <v/>
+      </c>
+      <c r="G24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>20</v>
-      </c>
-      <c r="H24" s="29">
+        <v/>
+      </c>
+      <c r="H24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>15</v>
-      </c>
-      <c r="I24" s="30">
+        <v/>
+      </c>
+      <c r="I24" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="29">
+        <v/>
+      </c>
+      <c r="J24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="29">
+        <v/>
+      </c>
+      <c r="K24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>240</v>
-      </c>
-      <c r="L24" s="29">
+        <v/>
+      </c>
+      <c r="L24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>240</v>
-      </c>
-      <c r="M24" s="29">
+        <v/>
+      </c>
+      <c r="M24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="29">
+        <v/>
+      </c>
+      <c r="N24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>180</v>
-      </c>
-      <c r="O24" s="29">
+        <v/>
+      </c>
+      <c r="O24" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>180</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
+        <v/>
       </c>
       <c r="B25" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Shoulder ESC</v>
-      </c>
-      <c r="C25" s="28">
+        <v/>
+      </c>
+      <c r="C25" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="D25" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
@@ -5668,117 +6549,117 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>20</v>
-      </c>
-      <c r="H25" s="29">
+        <v/>
+      </c>
+      <c r="H25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>15</v>
-      </c>
-      <c r="I25" s="30">
+        <v/>
+      </c>
+      <c r="I25" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="29">
+        <v/>
+      </c>
+      <c r="J25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>240</v>
-      </c>
-      <c r="K25" s="29">
+        <v/>
+      </c>
+      <c r="K25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="29">
+        <v/>
+      </c>
+      <c r="L25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>240</v>
-      </c>
-      <c r="M25" s="29">
+        <v/>
+      </c>
+      <c r="M25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>180</v>
-      </c>
-      <c r="N25" s="29">
+        <v/>
+      </c>
+      <c r="N25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="29">
+        <v/>
+      </c>
+      <c r="O25" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>180</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
+        <v/>
       </c>
       <c r="B26" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 2</v>
-      </c>
-      <c r="C26" s="28">
+        <v/>
+      </c>
+      <c r="C26" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
-      </c>
-      <c r="D26" s="26">
+        <v/>
+      </c>
+      <c r="D26" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E26" s="29">
+        <v/>
+      </c>
+      <c r="E26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="F26" s="29">
+        <v/>
+      </c>
+      <c r="F26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="29">
+        <v/>
+      </c>
+      <c r="G26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="H26" s="29">
+        <v/>
+      </c>
+      <c r="H26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="I26" s="30">
+        <v/>
+      </c>
+      <c r="I26" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="29">
+        <v/>
+      </c>
+      <c r="J26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="29">
+        <v/>
+      </c>
+      <c r="K26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>18</v>
-      </c>
-      <c r="L26" s="29">
+        <v/>
+      </c>
+      <c r="L26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="M26" s="29">
+        <v/>
+      </c>
+      <c r="M26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="29">
+        <v/>
+      </c>
+      <c r="N26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>12</v>
-      </c>
-      <c r="O26" s="29">
+        <v/>
+      </c>
+      <c r="O26" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
+        <v/>
       </c>
       <c r="B27" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Base ESC</v>
-      </c>
-      <c r="C27" s="28">
+        <v/>
+      </c>
+      <c r="C27" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="D27" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
@@ -5792,117 +6673,117 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="H27" s="29">
+        <v/>
+      </c>
+      <c r="H27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="30">
+        <v/>
+      </c>
+      <c r="I27" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="29">
+        <v/>
+      </c>
+      <c r="J27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="K27" s="29">
+        <v/>
+      </c>
+      <c r="K27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="29">
+        <v/>
+      </c>
+      <c r="L27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="M27" s="29">
+        <v/>
+      </c>
+      <c r="M27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
-      </c>
-      <c r="N27" s="29">
+        <v/>
+      </c>
+      <c r="N27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="29">
+        <v/>
+      </c>
+      <c r="O27" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
+        <v/>
       </c>
       <c r="B28" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Dirty Power 2</v>
-      </c>
-      <c r="C28" s="28">
+        <v/>
+      </c>
+      <c r="C28" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
-      </c>
-      <c r="D28" s="26">
+        <v/>
+      </c>
+      <c r="D28" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
-        <v>12</v>
-      </c>
-      <c r="E28" s="29">
+        <v/>
+      </c>
+      <c r="E28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="F28" s="29">
+        <v/>
+      </c>
+      <c r="F28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="G28" s="29">
+        <v/>
+      </c>
+      <c r="G28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="H28" s="29">
+        <v/>
+      </c>
+      <c r="H28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="I28" s="30">
+        <v/>
+      </c>
+      <c r="I28" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="29">
+        <v/>
+      </c>
+      <c r="J28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="29">
+        <v/>
+      </c>
+      <c r="K28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>18</v>
-      </c>
-      <c r="L28" s="29">
+        <v/>
+      </c>
+      <c r="L28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="M28" s="29">
+        <v/>
+      </c>
+      <c r="M28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="29">
+        <v/>
+      </c>
+      <c r="N28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>12</v>
-      </c>
-      <c r="O28" s="29">
+        <v/>
+      </c>
+      <c r="O28" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
+        <v/>
       </c>
       <c r="B29" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Elbow ESC</v>
-      </c>
-      <c r="C29" s="28">
+        <v/>
+      </c>
+      <c r="C29" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v>12</v>
+        <v/>
       </c>
       <c r="D29" s="26" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", IF(INDEX(Items[], ROW()-1, COLUMN(Items[Output (V)]))="[INPUT]", Analysis[[#This Row],[Input (V)]], VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE)))</f>
@@ -5916,41 +6797,41 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1.5</v>
-      </c>
-      <c r="H29" s="29">
+        <v/>
+      </c>
+      <c r="H29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>1</v>
-      </c>
-      <c r="I29" s="30">
+        <v/>
+      </c>
+      <c r="I29" s="30" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="29">
+        <v/>
+      </c>
+      <c r="J29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="K29" s="29">
+        <v/>
+      </c>
+      <c r="K29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="29">
+        <v/>
+      </c>
+      <c r="L29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>18</v>
-      </c>
-      <c r="M29" s="29">
+        <v/>
+      </c>
+      <c r="M29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
-      </c>
-      <c r="N29" s="29">
+        <v/>
+      </c>
+      <c r="N29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="29">
+        <v/>
+      </c>
+      <c r="O29" s="29" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -6032,8 +6913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6062,19 +6943,19 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
         <v>34</v>
@@ -6089,10 +6970,10 @@
         <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="Q1" t="s">
         <v>47</v>
@@ -6140,15 +7021,15 @@
       </c>
       <c r="O2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>38.128378378378379</v>
+        <v>28.02027027027027</v>
       </c>
       <c r="P2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>375.52027027027026</v>
+        <v>361.84459459459458</v>
       </c>
       <c r="Q2" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>8336.5499999999993</v>
+        <v>8032.95</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -6162,19 +7043,19 @@
       </c>
       <c r="C3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>375.52027027027026</v>
+        <v>361.84459459459458</v>
       </c>
       <c r="D3" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>38.128378378378379</v>
+        <v>28.02027027027027</v>
       </c>
       <c r="E3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.0431118618618618</v>
+        <v>1.0051238738738739</v>
       </c>
       <c r="F3" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.10591216216216216</v>
+        <v>7.7834084084084085E-2</v>
       </c>
       <c r="G3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6182,7 +7063,7 @@
       </c>
       <c r="H3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>0.62945241892610315</v>
+        <v>0.85652278755727029</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
@@ -6192,23 +7073,23 @@
         <v>MAYBE</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="N3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>12</v>
+        <v>22.2</v>
       </c>
       <c r="O3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.1666666666666667</v>
+        <v>27.027027027027028</v>
       </c>
       <c r="P3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2.6666666666666665</v>
+        <v>360</v>
       </c>
       <c r="Q3" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>32</v>
+        <v>7992</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6245,30 +7126,30 @@
         <v/>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K4" s="13" t="str">
         <f>IF(MIN(Results[Battery Life (hrs)]) &lt; 1, CONCATENATE(TEXT(MIN(Results[Battery Life (hrs)])*60, "#.#"), " min"), CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00")))</f>
-        <v>37.8 min</v>
+        <v>51.4 min</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="N4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.4</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="P4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.4</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="Q4" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6305,23 +7186,23 @@
         <v/>
       </c>
       <c r="M5" s="5" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="N5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>15</v>
+        <v>1.4</v>
       </c>
       <c r="P5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>20</v>
+        <v>1.4</v>
       </c>
       <c r="Q5" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>240</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6358,7 +7239,7 @@
         <v/>
       </c>
       <c r="M6" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -6366,15 +7247,15 @@
       </c>
       <c r="O6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6413,23 +7294,23 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="M7" s="5" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="N7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>22.2</v>
+        <v>12</v>
       </c>
       <c r="O7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>27.027027027027028</v>
+        <v>0</v>
       </c>
       <c r="P7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="5">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>7992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6494,19 +7375,19 @@
       </c>
       <c r="C9" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D9" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.95238095238095233</v>
+        <v>0</v>
       </c>
       <c r="F9" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.7142857142857143</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6528,19 +7409,19 @@
       </c>
       <c r="C10" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="11">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.14285714285714285</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>9.5238095238095233E-2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6652,6 +7533,14 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="M13" s="5" t="str">
+        <f>M3</f>
+        <v>Drivetrain Power</v>
+      </c>
+      <c r="N13" s="5">
+        <f>Q3</f>
+        <v>7992</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
@@ -6686,6 +7575,14 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="M14" s="5" t="str">
+        <f t="shared" ref="M14:M17" si="0">M4</f>
+        <v>Network Power</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" ref="N14:N17" si="1">Q4</f>
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
@@ -6720,6 +7617,14 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
+      <c r="M15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Logic Supply</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
@@ -6754,8 +7659,16 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Dirty Power 1</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackRight Motor</v>
@@ -6788,8 +7701,16 @@
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Dirty Power 2</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft ESC</v>
@@ -6823,7 +7744,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>FrontLeft Motor</v>
@@ -6857,7 +7778,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft ESC</v>
@@ -6891,7 +7812,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>MidLeft Motor</v>
@@ -6925,7 +7846,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft ESC</v>
@@ -6959,7 +7880,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v>BackLeft Motor</v>
@@ -6993,30 +7914,30 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
-      </c>
-      <c r="B24" s="1">
+        <v/>
+      </c>
+      <c r="B24" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C24" s="11">
+        <v/>
+      </c>
+      <c r="C24" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>20</v>
-      </c>
-      <c r="D24" s="11">
+        <v/>
+      </c>
+      <c r="D24" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>15</v>
-      </c>
-      <c r="E24" s="6">
+        <v/>
+      </c>
+      <c r="E24" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F24" s="6">
+        <v/>
+      </c>
+      <c r="F24" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.25</v>
+        <v/>
       </c>
       <c r="G24" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7027,14 +7948,14 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
-      </c>
-      <c r="B25" s="1">
+        <v/>
+      </c>
+      <c r="B25" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="C25" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7061,30 +7982,30 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
-      </c>
-      <c r="B26" s="1">
+        <v/>
+      </c>
+      <c r="B26" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C26" s="11">
+        <v/>
+      </c>
+      <c r="C26" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.5</v>
-      </c>
-      <c r="D26" s="11">
+        <v/>
+      </c>
+      <c r="D26" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="E26" s="6">
+        <v/>
+      </c>
+      <c r="E26" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F26" s="6">
+        <v/>
+      </c>
+      <c r="F26" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="G26" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7095,14 +8016,14 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
-      </c>
-      <c r="B27" s="1">
+        <v/>
+      </c>
+      <c r="B27" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="C27" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7129,30 +8050,30 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
-      </c>
-      <c r="B28" s="1">
+        <v/>
+      </c>
+      <c r="B28" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>60</v>
-      </c>
-      <c r="C28" s="11">
+        <v/>
+      </c>
+      <c r="C28" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1.5</v>
-      </c>
-      <c r="D28" s="11">
+        <v/>
+      </c>
+      <c r="D28" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="E28" s="6">
+        <v/>
+      </c>
+      <c r="E28" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F28" s="6">
+        <v/>
+      </c>
+      <c r="F28" s="6" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>1.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="G28" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7163,14 +8084,14 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
-      </c>
-      <c r="B29" s="1">
+        <v/>
+      </c>
+      <c r="B29" s="1" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="C29" s="11" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7197,7 +8118,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
         <v/>
@@ -7233,13 +8154,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7256,16 +8177,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 M2:M8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30 M2:M7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>ItemIDs</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7291,22 +8213,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -7346,7 +8268,7 @@
         <v>254</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -7507,7 +8429,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -7530,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -7553,7 +8475,7 @@
         <v>90</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1">
         <v>22</v>
@@ -7719,85 +8641,85 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder ESC</v>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Talon SRX DC Motor  Driver</v>
-      </c>
-      <c r="C24" s="3">
+        <v/>
+      </c>
+      <c r="C24" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Shoulder Motor</v>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>12 RPM HD Premium Planetary Gear Motor w/Encoder</v>
-      </c>
-      <c r="C25" s="3">
+        <v/>
+      </c>
+      <c r="C25" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base ESC</v>
+        <v/>
       </c>
       <c r="B26" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Victor SP DC Motor Driver</v>
-      </c>
-      <c r="C26" s="3">
+        <v/>
+      </c>
+      <c r="C26" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Base Motor</v>
+        <v/>
       </c>
       <c r="B27" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
-      </c>
-      <c r="C27" s="3">
+        <v/>
+      </c>
+      <c r="C27" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow ESC</v>
+        <v/>
       </c>
       <c r="B28" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>Victor SP DC Motor Driver</v>
-      </c>
-      <c r="C28" s="3">
+        <v/>
+      </c>
+      <c r="C28" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>60</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
-        <v>Elbow Motor</v>
+        <v/>
       </c>
       <c r="B29" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v>26 RPM Premium Planetary Gear Motor w/Encoder</v>
-      </c>
-      <c r="C29" s="3">
+        <v/>
+      </c>
+      <c r="C29" s="3" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to power budget
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6109C993-61ED-4203-ABE0-768E250005FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5622F5-A205-4509-90B1-E00BA550CC3A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="ComponentIDs">ComponentData[ID]</definedName>
     <definedName name="ItemIDs">Analysis[ItemID]</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -1570,11 +1570,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,7 +2118,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,10 +4536,10 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4552,7 +4552,7 @@
     <col min="6" max="6" width="21.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.7109375" style="25" bestFit="1" customWidth="1"/>
@@ -4750,11 +4750,11 @@
       </c>
       <c r="E4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>4.9054054054054061</v>
+        <v>6.6891891891891895</v>
       </c>
       <c r="F4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>2.4031531531531529</v>
+        <v>3.3396396396396391</v>
       </c>
       <c r="G4" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4774,7 +4774,7 @@
       </c>
       <c r="K4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>108.9</v>
+        <v>148.5</v>
       </c>
       <c r="L4" s="28" t="e">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="N4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>53.349999999999994</v>
+        <v>74.139999999999986</v>
       </c>
       <c r="O4" s="28" t="e">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4936,19 +4936,19 @@
       </c>
       <c r="E7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>7.666666666666667</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="F7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.7916666666666665</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="G7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>4.5585585585585591</v>
+        <v>6.3423423423423433</v>
       </c>
       <c r="H7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>2.2545045045045042</v>
+        <v>3.1909909909909908</v>
       </c>
       <c r="I7" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4956,27 +4956,27 @@
       </c>
       <c r="J7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>9.2000000000000011</v>
+        <v>12.8</v>
       </c>
       <c r="K7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="L7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>101.2</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="M7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>4.55</v>
+        <v>6.4399999999999995</v>
       </c>
       <c r="N7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>45.5</v>
+        <v>64.399999999999991</v>
       </c>
       <c r="O7" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>50.05</v>
+        <v>70.839999999999989</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6052,19 +6052,19 @@
       </c>
       <c r="E25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Peak Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>2.625</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="G25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>2.625</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="I25" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -6076,11 +6076,11 @@
       </c>
       <c r="K25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="L25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="M25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -6088,11 +6088,11 @@
       </c>
       <c r="N25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>31.5</v>
+        <v>50.399999999999991</v>
       </c>
       <c r="O25" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>31.5</v>
+        <v>50.399999999999991</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -6410,10 +6410,13 @@
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
         <v>Colling Fan 6</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27" t="str">
+      <c r="B31" s="26" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
+        <v>Cooling Fans Power</v>
+      </c>
+      <c r="C31" s="27">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="D31" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6427,13 +6430,13 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G31" s="28" t="str">
+      <c r="G31" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
-      </c>
-      <c r="H31" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="H31" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
+        <v>0.52500000000000002</v>
       </c>
       <c r="I31" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -6469,10 +6472,13 @@
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
         <v>Colling Fan 7</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27" t="str">
+      <c r="B32" s="26" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
+        <v>Cooling Fans Power</v>
+      </c>
+      <c r="C32" s="27">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="D32" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6486,13 +6492,13 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G32" s="28" t="str">
+      <c r="G32" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
-      </c>
-      <c r="H32" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="H32" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
+        <v>0.52500000000000002</v>
       </c>
       <c r="I32" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -6528,10 +6534,13 @@
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
         <v>Colling Fan 8</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27" t="str">
+      <c r="B33" s="26" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Supply Item])-COLUMN(Items[])+1, FALSE))</f>
+        <v>Cooling Fans Power</v>
+      </c>
+      <c r="C33" s="27">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]=""), "", VLOOKUP(Analysis[[#This Row],[Supply Item]], Analysis[], COLUMN(Analysis[Output (V)]), FALSE))</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="D33" s="27" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (V)])-COLUMN(Items[])+1, FALSE))</f>
@@ -6545,13 +6554,13 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
         <v/>
       </c>
-      <c r="G33" s="28" t="str">
+      <c r="G33" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
-      </c>
-      <c r="H33" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="H33" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v/>
+        <v>0.52500000000000002</v>
       </c>
       <c r="I33" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -7131,7 +7140,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7298,15 +7307,15 @@
       </c>
       <c r="O3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2.4031531531531529</v>
+        <v>3.3396396396396391</v>
       </c>
       <c r="P3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.9054054054054061</v>
+        <v>6.6891891891891895</v>
       </c>
       <c r="Q3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</f>
-        <v>108.90000000000002</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -7320,19 +7329,19 @@
       </c>
       <c r="C4" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>4.9054054054054061</v>
+        <v>6.6891891891891895</v>
       </c>
       <c r="D4" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2.4031531531531529</v>
+        <v>3.3396396396396391</v>
       </c>
       <c r="E4" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.12577962577962579</v>
+        <v>0.17151767151767153</v>
       </c>
       <c r="F4" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>6.1619311619311612E-2</v>
+        <v>8.5631785631785612E-2</v>
       </c>
       <c r="G4" s="9">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7340,7 +7349,7 @@
       </c>
       <c r="H4" s="4">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>3.2457357075913777</v>
+        <v>2.335581332613974</v>
       </c>
       <c r="J4" t="s">
         <v>62</v>
@@ -7444,19 +7453,19 @@
       </c>
       <c r="C7" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>7.666666666666667</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="D7" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.7916666666666665</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="E7" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.63888888888888895</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F7" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.31597222222222221</v>
+        <v>0.44722222222222219</v>
       </c>
       <c r="G7" s="9" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -8068,11 +8077,11 @@
       </c>
       <c r="C25" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D25" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>2.625</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="E25" s="5" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -8542,8 +8551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor changes to power budget document
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5622F5-A205-4509-90B1-E00BA550CC3A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AFFB53-526A-4627-8D9F-7F2FFD941D28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="12210" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,6 @@
     <t>https://www.aliexpress.com/item/DC-Adjustable-Voltage-Regulator-Module-DC-4-5-30V-to-0-8-30V-12A-Buck-Converters/1724570414.html</t>
   </si>
   <si>
-    <t>Aihsd</t>
-  </si>
-  <si>
     <t>Thoughput Loss</t>
   </si>
   <si>
@@ -391,6 +388,9 @@
   </si>
   <si>
     <t>Colling Fan 8</t>
+  </si>
+  <si>
+    <t>Aihasd</t>
   </si>
 </sst>
 </file>
@@ -1570,11 +1570,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>4</v>
@@ -1626,21 +1626,21 @@
         <v>11</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>33</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1676,13 +1676,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="3">
@@ -1714,15 +1714,15 @@
     </row>
     <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="21"/>
       <c r="E4" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>71</v>
@@ -1801,7 +1801,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6" s="10">
         <v>3.3</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>36</v>
@@ -1856,13 +1856,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
@@ -1895,13 +1895,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J9" s="10">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -1967,17 +1967,17 @@
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="3">
         <v>16</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2036,7 +2036,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
@@ -2051,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="10">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -2066,15 +2066,15 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="10">
@@ -2180,7 +2180,7 @@
         <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2378,7 +2378,7 @@
         <v>67</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="F5" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Aihsd</v>
+        <v>Aihasd</v>
       </c>
       <c r="G5" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="J6" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" s="17">
         <f>IF(
@@ -2493,13 +2493,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="F7" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>Aihsd</v>
+        <v>Aihasd</v>
       </c>
       <c r="G7" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2549,10 +2549,10 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2747,13 +2747,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2814,13 +2814,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2883,10 +2883,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3017,10 +3017,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3151,10 +3151,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3285,10 +3285,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3419,10 +3419,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3553,10 +3553,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3684,13 +3684,13 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3818,13 +3818,13 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D27" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3885,13 +3885,13 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D28" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3952,13 +3952,13 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4019,13 +4019,13 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D30" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4086,13 +4086,13 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D31" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4153,13 +4153,13 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4220,13 +4220,13 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4589,7 +4589,7 @@
         <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J1" s="25" t="s">
         <v>50</v>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="F4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>3.3396396396396391</v>
+        <v>3.3891891891891892</v>
       </c>
       <c r="G4" s="28" t="str">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="N4" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>74.139999999999986</v>
+        <v>75.239999999999995</v>
       </c>
       <c r="O4" s="28" t="e">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="F5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Output (V)]]), ISTEXT(Analysis[[#This Row],[Output (V)]]), Analysis[[#This Row],[Output (V)]]&lt;=0), "", Analysis[[#This Row],[Children Constant Consumption (W)]]/Analysis[[#This Row],[Output (V)]])</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Peak Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
@@ -4824,7 +4824,7 @@
       </c>
       <c r="H5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.14864864864864866</v>
+        <v>0.19819819819819823</v>
       </c>
       <c r="I5" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4844,15 +4844,15 @@
       </c>
       <c r="M5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="N5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O5" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>3.3</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -4886,7 +4886,7 @@
       </c>
       <c r="H6" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I6" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="M6" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="O6" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -7196,10 +7196,10 @@
         <v>40</v>
       </c>
       <c r="O1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q1" t="s">
         <v>41</v>
@@ -7239,7 +7239,7 @@
         <v/>
       </c>
       <c r="M2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7299,7 +7299,7 @@
         <v>GO</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="O3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.3396396396396391</v>
+        <v>3.3891891891891892</v>
       </c>
       <c r="P3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="D4" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>3.3396396396396391</v>
+        <v>3.3891891891891892</v>
       </c>
       <c r="E4" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="F4" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>8.5631785631785612E-2</v>
+        <v>8.6902286902286907E-2</v>
       </c>
       <c r="G4" s="9">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -7349,7 +7349,7 @@
       </c>
       <c r="H4" s="4">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>2.335581332613974</v>
+        <v>2.3014354066985647</v>
       </c>
       <c r="J4" t="s">
         <v>62</v>
@@ -7379,7 +7379,7 @@
       </c>
       <c r="D5" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E5" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="F5" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>4.9999999999999996E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G5" s="9" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
@@ -8551,7 +8551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13:E29"/>
     </sheetView>
   </sheetViews>
@@ -8692,7 +8692,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -8715,7 +8715,7 @@
         <v>8.48</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -8738,7 +8738,7 @@
         <v>180</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -8761,7 +8761,7 @@
         <v/>
       </c>
       <c r="E9" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1">
         <v>6</v>
@@ -9075,7 +9075,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31">
         <f>SUBTOTAL(9,Costs[Cost])</f>

</xml_diff>

<commit_message>
Minor changes to the power budget
</commit_message>
<xml_diff>
--- a/Electrical/PowerBudget.xlsx
+++ b/Electrical/PowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AFFB53-526A-4627-8D9F-7F2FFD941D28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170E836-E6BB-4C49-8894-ED5C2E649F2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="18" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>24 V Lithuim Ion Battery back</t>
-  </si>
-  <si>
     <t>Adjustable Linear Voltage Regulator</t>
   </si>
   <si>
@@ -391,6 +388,27 @@
   </si>
   <si>
     <t>Aihasd</t>
+  </si>
+  <si>
+    <t>IP Camera</t>
+  </si>
+  <si>
+    <t>ELP 1280720p 1MP Camera</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/ELP-1280720p-Megapixel-Camera-Network/dp/B00KA4M4WS</t>
+  </si>
+  <si>
+    <t>Hazard Camera 1</t>
+  </si>
+  <si>
+    <t>Hazard Camera 2</t>
+  </si>
+  <si>
+    <t>Hazard Camera 3</t>
+  </si>
+  <si>
+    <t>16-Port network switch</t>
   </si>
 </sst>
 </file>
@@ -524,6 +542,30 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
@@ -531,9 +573,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -576,27 +615,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -770,7 +788,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="James Talbert" refreshedDate="43192.567844097219" createdVersion="5" refreshedVersion="6" minRefreshableVersion="3" recordCount="29" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="James Talbert" refreshedDate="43319.654593981482" createdVersion="5" refreshedVersion="6" minRefreshableVersion="3" recordCount="40" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Costs"/>
   </cacheSource>
@@ -779,20 +797,25 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Component Name" numFmtId="0">
-      <sharedItems count="17">
+      <sharedItems count="22">
         <s v=""/>
-        <s v="24 V Lithuim Ion Battery back"/>
+        <s v="22.2 V Lithuim Polymer Battery back"/>
+        <s v="22.2V Lithium Ion Battery Pack"/>
         <s v="Adjustable Linear Voltage Regulator"/>
         <s v="Raspberry Pi 3 Rev 1.2"/>
         <s v="Ubiquity Rocket M5"/>
+        <s v="16-Port network switch"/>
         <s v="Nextrox DC/DC Converter Regulator 24V Step Down to 12V 20A 240W"/>
         <s v="Virtual Node for system isolation"/>
         <s v="Talon SRX DC Motor  Driver"/>
         <s v="Banebots RS-550 Motor 19300rpm 12V 70.55oz-in"/>
+        <s v="???"/>
+        <s v="ELP 1280720p 1MP Camera"/>
         <s v="26 RPM Premium Planetary Gear Motor w/Encoder" u="1"/>
         <s v="Ubiquity Rocket M3" u="1"/>
         <s v="Homemade POE injection" u="1"/>
         <s v="12 RPM HD Premium Planetary Gear Motor w/Encoder" u="1"/>
+        <s v="24 V Lithuim Ion Battery back" u="1"/>
         <s v="Victor SP DC Motor Driver" u="1"/>
         <s v="Linear Voltage Regulator" u="1"/>
         <s v="Linear Regulator" u="1"/>
@@ -813,126 +836,181 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
   <r>
     <s v=""/>
     <x v="0"/>
     <s v=""/>
   </r>
   <r>
-    <s v="Battery Pack"/>
+    <s v="Primary Battery Pack"/>
     <x v="1"/>
     <n v="254"/>
   </r>
   <r>
+    <s v="E-Box Battery"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
     <s v="Logic Supply"/>
-    <x v="2"/>
+    <x v="3"/>
     <n v="8.48"/>
   </r>
   <r>
     <s v="Master Control"/>
-    <x v="3"/>
+    <x v="4"/>
     <n v="30"/>
   </r>
   <r>
     <s v="Network Power"/>
-    <x v="2"/>
+    <x v="3"/>
     <n v="8.48"/>
   </r>
   <r>
     <s v="Transceiver"/>
-    <x v="4"/>
+    <x v="5"/>
     <n v="180"/>
   </r>
   <r>
     <s v="Network Switch"/>
-    <x v="0"/>
-    <s v=""/>
+    <x v="6"/>
+    <n v="60"/>
   </r>
   <r>
     <s v="Dirty Power 1"/>
-    <x v="5"/>
+    <x v="7"/>
     <n v="16"/>
   </r>
   <r>
     <s v="Dirty Power 2"/>
-    <x v="5"/>
+    <x v="7"/>
     <n v="16"/>
   </r>
   <r>
     <s v="Drivetrain Power"/>
-    <x v="6"/>
+    <x v="8"/>
     <n v="0"/>
   </r>
   <r>
     <s v="FrontRight ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="FrontRight Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
     <s v="MidRight ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="MidRight Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
     <s v="BackRight ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="BackRight Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
     <s v="FrontLeft ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="FrontLeft Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
     <s v="MidLeft ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="MidLeft Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
     <s v="BackLeft ESC"/>
-    <x v="7"/>
+    <x v="9"/>
     <n v="90"/>
   </r>
   <r>
     <s v="BackLeft Motor"/>
-    <x v="8"/>
+    <x v="10"/>
     <n v="7.25"/>
   </r>
   <r>
-    <s v=""/>
-    <x v="0"/>
-    <s v=""/>
+    <s v="Cooling Fans Power"/>
+    <x v="8"/>
+    <n v="0"/>
   </r>
   <r>
-    <s v=""/>
-    <x v="0"/>
-    <s v=""/>
+    <s v="Colling Fan 1"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 2"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 3"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 4"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 5"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 6"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 7"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Colling Fan 8"/>
+    <x v="11"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="Hazard Camera 1"/>
+    <x v="12"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <s v="Hazard Camera 2"/>
+    <x v="12"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <s v="Hazard Camera 3"/>
+    <x v="12"/>
+    <n v="20"/>
   </r>
   <r>
     <s v=""/>
@@ -963,29 +1041,34 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="Costs By Component" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
-  <location ref="E1:G10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="Costs By Component" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+  <location ref="E1:G14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
-      <items count="18">
+      <items count="23">
         <item h="1" x="0"/>
-        <item m="1" x="12"/>
-        <item m="1" x="9"/>
         <item m="1" x="16"/>
+        <item m="1" x="13"/>
+        <item m="1" x="21"/>
+        <item x="10"/>
+        <item m="1" x="15"/>
+        <item m="1" x="20"/>
+        <item x="4"/>
+        <item m="1" x="14"/>
+        <item m="1" x="18"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="7"/>
         <item x="8"/>
-        <item m="1" x="11"/>
-        <item m="1" x="15"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item m="1" x="13"/>
+        <item x="9"/>
         <item x="1"/>
-        <item m="1" x="14"/>
         <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
+        <item x="11"/>
+        <item x="12"/>
         <item x="6"/>
-        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -995,15 +1078,12 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="13">
     <i>
       <x v="4"/>
     </i>
     <i>
       <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
     </i>
     <i>
       <x v="12"/>
@@ -1019,6 +1099,21 @@
     </i>
     <i>
       <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
     </i>
     <i t="grand">
       <x/>
@@ -1063,8 +1158,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N14" totalsRowShown="0" headerRowDxfId="66">
-  <autoFilter ref="A1:N14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ComponentData" displayName="ComponentData" ref="A1:N15" totalsRowShown="0" headerRowDxfId="66">
+  <autoFilter ref="A1:N15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="65"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name" dataDxfId="64"/>
@@ -1200,28 +1295,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Results" displayName="Results" ref="A1:H37" totalsRowShown="0">
   <autoFilter ref="A1:H37" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ItemID" dataDxfId="20">
       <calculatedColumnFormula>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="16">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Current Capacity" dataDxfId="19">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Peak Current Used" dataDxfId="18">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="14">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Constant Current Used" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Peak % Capacity" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Constant % Capacity" dataDxfId="15">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Battery (mAh)" dataDxfId="14">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Battery Life (hrs)" dataDxfId="13">
       <calculatedColumnFormula>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1230,20 +1325,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="RailSummary" displayName="RailSummary" ref="M1:Q8" totalsRowShown="0" dataDxfId="12">
   <autoFilter ref="M1:Q8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Power Rail" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Voltage (V)" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{5734B35D-169B-4597-A9BA-F7DB77804437}" name="Current (A)" dataDxfId="9">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Constant Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Peak Current (A)" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Power (W)" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", RailSummary[[#This Row],[Voltage (V)]]*RailSummary[[#This Row],[Peak Current (A)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1252,16 +1347,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C31" totalsRowCount="1">
-  <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Costs" displayName="Costs" ref="A1:C42" totalsRowCount="1">
+  <autoFilter ref="A1:C41" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="6">
       <calculatedColumnFormula>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Component Name" dataDxfId="5">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="custom" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Cost" totalsRowFunction="custom" dataDxfId="4">
       <calculatedColumnFormula>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</calculatedColumnFormula>
       <totalsRowFormula>SUBTOTAL(9,Costs[Cost])</totalsRowFormula>
     </tableColumn>
@@ -1568,13 +1663,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>4</v>
@@ -1626,21 +1721,21 @@
         <v>11</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>33</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1676,13 +1771,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>87</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="3">
@@ -1699,14 +1794,14 @@
       </c>
       <c r="J3" s="10">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="30">
         <v>15</v>
       </c>
       <c r="M3" s="10">
-        <v>24000</v>
+        <v>12000</v>
       </c>
       <c r="N3" s="5">
         <v>0</v>
@@ -1714,15 +1809,15 @@
     </row>
     <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="21"/>
       <c r="E4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -1752,13 +1847,13 @@
         <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>71</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="3">
@@ -1821,10 +1916,10 @@
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>36</v>
@@ -1856,13 +1951,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
@@ -1895,13 +1990,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1915,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="10">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -1967,17 +2062,17 @@
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="3">
         <v>16</v>
@@ -2006,13 +2101,17 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>60</v>
+      </c>
       <c r="G12" s="10">
         <v>24</v>
       </c>
@@ -2036,7 +2135,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
@@ -2051,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="10">
         <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
@@ -2066,17 +2165,19 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="F14" s="3">
+        <v>18</v>
+      </c>
       <c r="G14" s="10">
         <v>12</v>
       </c>
@@ -2092,6 +2193,39 @@
       <c r="L14" s="30"/>
       <c r="M14" s="10"/>
       <c r="N14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="3">
+        <v>20</v>
+      </c>
+      <c r="G15" s="10">
+        <v>24</v>
+      </c>
+      <c r="H15" s="10">
+        <v>6</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10">
+        <f>MAX(ComponentData[[#This Row],[Output Current Limit (A)]], ComponentData[[#This Row],[Discharge (for batteries)]]*ComponentData[[#This Row],[Battery (mAh)]]/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2101,11 +2235,12 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{86EF303B-6B5E-4E0B-8983-28A252B0769B}"/>
     <hyperlink ref="D11" r:id="rId3" xr:uid="{7D768727-DEDA-40C8-9759-80357E423FFD}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{3AFCC2EA-FA64-44BD-8ABF-E11110400232}"/>
+    <hyperlink ref="D15" r:id="rId5" xr:uid="{5BC0D8B4-1FD4-485B-B6D9-C32E008C0EE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2115,10 +2250,10 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2315,7 @@
         <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2244,7 +2379,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
@@ -2295,11 +2430,11 @@
       </c>
       <c r="L3" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="M3" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v>24000</v>
+        <v>12000</v>
       </c>
       <c r="N3" s="31">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2308,10 +2443,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2378,7 +2513,7 @@
         <v>67</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2493,13 +2628,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2549,10 +2684,10 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2613,13 +2748,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2627,7 +2762,7 @@
       </c>
       <c r="E9" s="20" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>16-Port network switch</v>
       </c>
       <c r="F9" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2637,9 +2772,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H9" s="16" t="str">
+      <c r="H9" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>60</v>
       </c>
       <c r="I9" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -2680,13 +2815,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2747,13 +2882,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2814,13 +2949,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -2883,10 +3018,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3017,10 +3152,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3151,10 +3286,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3285,10 +3420,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3419,10 +3554,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3553,10 +3688,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D23" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3684,13 +3819,13 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3751,13 +3886,13 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3775,9 +3910,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H26" s="16" t="str">
+      <c r="H26" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I26" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3818,13 +3953,13 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3842,9 +3977,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H27" s="16" t="str">
+      <c r="H27" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I27" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3885,13 +4020,13 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D28" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3909,9 +4044,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H28" s="16" t="str">
+      <c r="H28" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I28" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -3952,13 +4087,13 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D29" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -3976,9 +4111,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H29" s="16" t="str">
+      <c r="H29" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I29" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4019,13 +4154,13 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4043,9 +4178,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H30" s="16" t="str">
+      <c r="H30" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I30" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4086,13 +4221,13 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4110,9 +4245,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H31" s="16" t="str">
+      <c r="H31" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I31" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4153,13 +4288,13 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4177,9 +4312,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H32" s="16" t="str">
+      <c r="H32" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I32" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4220,13 +4355,13 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
@@ -4244,9 +4379,9 @@
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="H33" s="16" t="str">
+      <c r="H33" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I33" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4286,13 +4421,22 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="D34" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>Regulator</v>
       </c>
       <c r="E34" s="20" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>ELP 1280720p 1MP Camera</v>
       </c>
       <c r="F34" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4300,19 +4444,19 @@
       </c>
       <c r="G34" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H34" s="16" t="str">
+        <v>https://www.amazon.com/ELP-1280720p-Megapixel-Camera-Network/dp/B00KA4M4WS</v>
+      </c>
+      <c r="H34" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I34" s="17" t="str">
+        <v>20</v>
+      </c>
+      <c r="I34" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="J34" s="17" t="str">
+        <v>24</v>
+      </c>
+      <c r="J34" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="K34" s="17" t="str">
         <f>IF(
@@ -4330,27 +4474,36 @@
    )</f>
         <v/>
       </c>
-      <c r="L34" s="17" t="str">
+      <c r="L34" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M34" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N34" s="22" t="str">
+      <c r="N34" s="22">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="D35" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>Regulator</v>
       </c>
       <c r="E35" s="20" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>ELP 1280720p 1MP Camera</v>
       </c>
       <c r="F35" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4358,19 +4511,19 @@
       </c>
       <c r="G35" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H35" s="16" t="str">
+        <v>https://www.amazon.com/ELP-1280720p-Megapixel-Camera-Network/dp/B00KA4M4WS</v>
+      </c>
+      <c r="H35" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I35" s="17" t="str">
+        <v>20</v>
+      </c>
+      <c r="I35" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="J35" s="17" t="str">
+        <v>24</v>
+      </c>
+      <c r="J35" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="K35" s="17" t="str">
         <f>IF(
@@ -4388,27 +4541,36 @@
    )</f>
         <v/>
       </c>
-      <c r="L35" s="17" t="str">
+      <c r="L35" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M35" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N35" s="22" t="str">
+      <c r="N35" s="22">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="D36" s="13" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Supply Item]]), Items[[#This Row],[Supply Item]]="", Items[[#This Row],[Supply Item]]=0), "", VLOOKUP(Items[[#This Row],[Supply Item]], Items[], COLUMN(Items[Component])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>Regulator</v>
       </c>
       <c r="E36" s="20" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Name])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>ELP 1280720p 1MP Camera</v>
       </c>
       <c r="F36" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Manufacturer])-COLUMN(ComponentData[])+1, FALSE)))</f>
@@ -4416,19 +4578,19 @@
       </c>
       <c r="G36" s="15" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Source])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H36" s="16" t="str">
+        <v>https://www.amazon.com/ELP-1280720p-Megapixel-Camera-Network/dp/B00KA4M4WS</v>
+      </c>
+      <c r="H36" s="16">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Price])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I36" s="17" t="str">
+        <v>20</v>
+      </c>
+      <c r="I36" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Peak Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
-      </c>
-      <c r="J36" s="17" t="str">
+        <v>24</v>
+      </c>
+      <c r="J36" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Constant Consumption (W)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="K36" s="17" t="str">
         <f>IF(
@@ -4446,17 +4608,17 @@
    )</f>
         <v/>
       </c>
-      <c r="L36" s="17" t="str">
+      <c r="L36" s="17">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Output (A)])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M36" s="17" t="str">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Battery (mAh)])-COLUMN(ComponentData[])+1, FALSE)))</f>
         <v/>
       </c>
-      <c r="N36" s="22" t="str">
+      <c r="N36" s="22">
         <f>IF(OR(ISBLANK(Items[[#This Row],[Component]]), Items[[#This Row],[Component]]="", Items[[#This Row],[Component]]=0), "", IF(ISBLANK(VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)), "", VLOOKUP(Items[[#This Row],[Component]], ComponentData[], COLUMN(ComponentData[Thoughput Loss])-COLUMN(ComponentData[])+1, FALSE)))</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4589,7 +4751,7 @@
         <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J1" s="25" t="s">
         <v>50</v>
@@ -6594,7 +6756,7 @@
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v/>
+        <v>Hazard Camera 1</v>
       </c>
       <c r="B34" s="27"/>
       <c r="C34" s="27" t="str">
@@ -6621,39 +6783,39 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
         <v/>
       </c>
-      <c r="I34" s="29" t="str">
+      <c r="I34" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J34" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="J34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="K34" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="K34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="L34" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="L34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="M34" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="M34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="N34" s="28" t="str">
+        <v>6</v>
+      </c>
+      <c r="N34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="O34" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="O34" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v/>
+        <v>Hazard Camera 2</v>
       </c>
       <c r="B35" s="27"/>
       <c r="C35" s="27" t="str">
@@ -6680,39 +6842,39 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
         <v/>
       </c>
-      <c r="I35" s="29" t="str">
+      <c r="I35" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J35" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="J35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="K35" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="K35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="L35" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="L35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="M35" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="M35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="N35" s="28" t="str">
+        <v>6</v>
+      </c>
+      <c r="N35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="O35" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="O35" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="str">
         <f>IF(IFERROR(Items[[#This Row],[ItemID]], 0)=0, "", Items[[#This Row],[ItemID]])</f>
-        <v/>
+        <v>Hazard Camera 3</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="27" t="str">
@@ -6739,33 +6901,33 @@
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", ISBLANK(Analysis[[#This Row],[Supply Item]]), Analysis[[#This Row],[Supply Item]]="", Analysis[[#This Row],[Input (V)]]&lt;=0), "", Analysis[[#This Row],[Total Constant Consumption (W)]]/Analysis[[#This Row],[Input (V)]])</f>
         <v/>
       </c>
-      <c r="I36" s="29" t="str">
+      <c r="I36" s="29">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Thoughput Loss])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="J36" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="J36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Peak Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="K36" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="K36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Peak Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="L36" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="L36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Peak Consumption (W)]]+Analysis[[#This Row],[Children Peak Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="M36" s="28" t="str">
+        <v>24</v>
+      </c>
+      <c r="M36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", VLOOKUP(Analysis[[#This Row],[ItemID]], Items[], COLUMN(Items[Constant Consumption (W)])-COLUMN(Items[])+1, FALSE)+(Analysis[[#This Row],[Thoughput Loss]])*Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
-      </c>
-      <c r="N36" s="28" t="str">
+        <v>6</v>
+      </c>
+      <c r="N36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", SUMIFS(Analysis[Total Constant Consumption (W)], Analysis[Supply Item], Analysis[[#This Row],[ItemID]]))</f>
-        <v/>
-      </c>
-      <c r="O36" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="O36" s="28">
         <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]=""), "", Analysis[[#This Row],[Self Constant Consumption (W)]]+Analysis[[#This Row],[Children Constant Consumption (W)]])</f>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -7196,10 +7358,10 @@
         <v>40</v>
       </c>
       <c r="O1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q1" t="s">
         <v>41</v>
@@ -7239,7 +7401,7 @@
         <v/>
       </c>
       <c r="M2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N2" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7265,7 +7427,7 @@
       </c>
       <c r="B3">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="C3" s="10">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7277,19 +7439,19 @@
       </c>
       <c r="E3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Peak Current Used]]=""), "", Results[[#This Row],[Peak Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>0.18333333333333332</v>
+        <v>0.36666666666666664</v>
       </c>
       <c r="F3" s="5">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Current Capacity]]=0, Results[[#This Row],[Current Capacity]]="", Results[[#This Row],[Constant Current Used]]=""), "", Results[[#This Row],[Constant Current Used]]/Results[[#This Row],[Current Capacity]])</f>
-        <v>3.0555555555555555E-2</v>
+        <v>6.1111111111111109E-2</v>
       </c>
       <c r="G3" s="9">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]="", IFERROR(ISBLANK(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE)), TRUE), IFERROR(VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE), TRUE)=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Battery (mAh)])-COLUMN(Items[])+1, FALSE))</f>
-        <v>24000</v>
+        <v>12000</v>
       </c>
       <c r="H3" s="4">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[Constant Current Used]]="", Results[[#This Row],[Battery (mAh)]]=""), "", (Results[[#This Row],[Battery (mAh)]]/1000)/Results[[#This Row],[Constant Current Used]])</f>
-        <v>2.1818181818181817</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="J3" t="s">
         <v>35</v>
@@ -7299,7 +7461,7 @@
         <v>GO</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N3" s="4">
         <f>IF(ISBLANK(RailSummary[[#This Row],[Power Rail]]), "", VLOOKUP(RailSummary[[#This Row],[Power Rail]], Analysis[], COLUMN(Analysis[Output (V)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -7356,7 +7518,7 @@
       </c>
       <c r="K4" s="12" t="str">
         <f>IF(MIN(Results[Battery Life (hrs)]) &lt; 1, CONCATENATE(TEXT(MIN(Results[Battery Life (hrs)])*60, "#.#"), " min"), CONCATENATE(TEXT(INT(MIN(Results[Battery Life (hrs)])), "0#"),":",TEXT(MOD(MIN(Results[Battery Life (hrs)]), 1)*60, "00")))</f>
-        <v>02:11</v>
+        <v>01:05</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -8375,11 +8537,11 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v/>
-      </c>
-      <c r="B34" s="1" t="str">
+        <v>Hazard Camera 1</v>
+      </c>
+      <c r="B34" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C34" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -8409,11 +8571,11 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v/>
-      </c>
-      <c r="B35" s="1" t="str">
+        <v>Hazard Camera 2</v>
+      </c>
+      <c r="B35" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C35" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -8443,11 +8605,11 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF(IFERROR(Analysis[[#This Row],[ItemID]], 0)=0, "", Analysis[[#This Row],[ItemID]])</f>
-        <v/>
-      </c>
-      <c r="B36" s="1" t="str">
+        <v>Hazard Camera 3</v>
+      </c>
+      <c r="B36" s="1">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Items[], COLUMN(Items[Output (A)])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C36" s="10" t="str">
         <f>IF(OR(ISBLANK(Results[[#This Row],[ItemID]]), Results[[#This Row],[ItemID]]=0, Results[[#This Row],[ItemID]]=""), "", VLOOKUP(Results[[#This Row],[ItemID]], Analysis[], COLUMN(Analysis[Peak Output (A)])-COLUMN(Analysis[])+1, FALSE))</f>
@@ -8510,13 +8672,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="HOLD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="MAYBE"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>INDIRECT(ADDRESS(ROW(), COLUMN()))="GO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8549,10 +8711,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E29"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8649,10 +8811,10 @@
         <v>69</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>254</v>
+        <v>16.96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8669,13 +8831,13 @@
         <v>8.48</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
-        <v>16.96</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8692,13 +8854,13 @@
         <v>30</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>180</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8715,13 +8877,13 @@
         <v>8.48</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -8738,13 +8900,13 @@
         <v>180</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -8754,20 +8916,20 @@
       </c>
       <c r="B9" s="1" t="str">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="C9" s="3" t="str">
+        <v>16-Port network switch</v>
+      </c>
+      <c r="C9" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>60</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="F9" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>540</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -8784,13 +8946,13 @@
         <v>16</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="F10" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>1096.46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -8806,6 +8968,15 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
         <v>16</v>
       </c>
+      <c r="E11" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="1">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
@@ -8820,6 +8991,15 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
         <v>0</v>
       </c>
+      <c r="E12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
@@ -8834,6 +9014,15 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
         <v>90</v>
       </c>
+      <c r="E13" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
@@ -8848,6 +9037,15 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
         <v>7.25</v>
       </c>
+      <c r="E14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1">
+        <v>34</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1360.46</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
@@ -9012,9 +9210,9 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>???</v>
       </c>
-      <c r="C26" s="3" t="str">
+      <c r="C26" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -9026,9 +9224,9 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>???</v>
       </c>
-      <c r="C27" s="3" t="str">
+      <c r="C27" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9040,9 +9238,9 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>???</v>
       </c>
-      <c r="C28" s="3" t="str">
+      <c r="C28" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9054,9 +9252,9 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>???</v>
       </c>
-      <c r="C29" s="3" t="str">
+      <c r="C29" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9068,18 +9266,172 @@
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
         <v>???</v>
       </c>
-      <c r="C30" s="3" t="str">
+      <c r="C30" s="3">
         <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
-        <v/>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31">
+      <c r="A31" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Colling Fan 6</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>???</v>
+      </c>
+      <c r="C31" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Colling Fan 7</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>???</v>
+      </c>
+      <c r="C32" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Colling Fan 8</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>???</v>
+      </c>
+      <c r="C33" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Hazard Camera 1</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>ELP 1280720p 1MP Camera</v>
+      </c>
+      <c r="C34" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Hazard Camera 2</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>ELP 1280720p 1MP Camera</v>
+      </c>
+      <c r="C35" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v>Hazard Camera 3</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v>ELP 1280720p 1MP Camera</v>
+      </c>
+      <c r="C36" s="3">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v/>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="C37" s="3" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v/>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="C38" s="3" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v/>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="C39" s="3" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v/>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="C40" s="3" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f>IF(OR(ISBLANK(Analysis[[#This Row],[ItemID]]), Analysis[[#This Row],[ItemID]]="", Analysis[[#This Row],[ItemID]]=0), "", Analysis[[#This Row],[ItemID]])</f>
+        <v/>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Name])-COLUMN(Items[])+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="C41" s="3" t="str">
+        <f>IF(OR(ISBLANK(Costs[[#This Row],[Item]]), Costs[[#This Row],[Item]]="", Costs[[#This Row],[Item]]=0), "", IF(ISNUMBER(VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE)), VLOOKUP(Costs[[#This Row],[Item]], Items[], COLUMN(Items[Price])-COLUMN(Items[])+1, FALSE), ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42">
         <f>SUBTOTAL(9,Costs[Cost])</f>
-        <v>1096.46</v>
+        <v>1360.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>